<commit_message>
changes to extraction process, need further improvement
</commit_message>
<xml_diff>
--- a/QALD9-Plus-testing/CoT-entity-aligned/CoT-wikidata-dbpedia/comparison_results_llama_CoT_wikidata_dbpedia.xlsx
+++ b/QALD9-Plus-testing/CoT-entity-aligned/CoT-wikidata-dbpedia/comparison_results_llama_CoT_wikidata_dbpedia.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,17 +458,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Who is the founder of Penguin Books?</t>
+          <t>Which films did Stanley Kubrick direct?</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Allen_Lane']</t>
+          <t>['http://dbpedia.org/resource/2001:_A_Space_Odyssey_(film)', 'http://dbpedia.org/resource/A_Clockwork_Orange_(film)', 'http://dbpedia.org/resource/Barry_Lyndon', 'http://dbpedia.org/resource/Day_of_the_Fight', 'http://dbpedia.org/resource/Dr._Strangelove', 'http://dbpedia.org/resource/Eyes_Wide_Shut', 'http://dbpedia.org/resource/Fear_and_Desire', 'http://dbpedia.org/resource/Flying_Padre', 'http://dbpedia.org/resource/Full_Metal_Jacket', "http://dbpedia.org/resource/Killer's_Kiss", 'http://dbpedia.org/resource/Lolita_(1962_film)', 'http://dbpedia.org/resource/Paths_of_Glory', 'http://dbpedia.org/resource/Spartacus_(film)', 'http://dbpedia.org/resource/The_Killing_(film)__The_Killing__1', 'http://dbpedia.org/resource/The_Seafarers__The_Seafarers__1', 'http://dbpedia.org/resource/The_Shining_(film)']</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Allen_Lane']</t>
+          <t>['http://dbpedia.org/resource/2001:_A_Space_Odyssey_(film)', 'http://dbpedia.org/resource/A_Clockwork_Orange_(film)', 'http://dbpedia.org/resource/Barry_Lyndon', 'http://dbpedia.org/resource/Day_of_the_Fight', 'http://dbpedia.org/resource/Dr._Strangelove', 'http://dbpedia.org/resource/Eyes_Wide_Shut', 'http://dbpedia.org/resource/Fear_and_Desire', 'http://dbpedia.org/resource/Flying_Padre', 'http://dbpedia.org/resource/Full_Metal_Jacket', "http://dbpedia.org/resource/Killer's_Kiss", 'http://dbpedia.org/resource/Lolita_(1962_film)', 'http://dbpedia.org/resource/Paths_of_Glory', 'http://dbpedia.org/resource/Spartacus_(film)', 'http://dbpedia.org/resource/The_Killing_(film)__The_Killing__1', 'http://dbpedia.org/resource/The_Seafarers__The_Seafarers__1', 'http://dbpedia.org/resource/The_Shining_(film)']</t>
         </is>
       </c>
       <c r="D2" t="b">
@@ -478,17 +478,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Give me all actors starring in movies directed by William Shatner.</t>
+          <t>Who developed Skype?</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/DeForest_Kelley', 'http://dbpedia.org/resource/George_Takei', 'http://dbpedia.org/resource/James_Doohan', 'http://dbpedia.org/resource/Leonard_Nimoy', 'http://dbpedia.org/resource/Nichelle_Nichols', 'http://dbpedia.org/resource/Walter_Koenig', 'http://dbpedia.org/resource/William_Shatner']</t>
+          <t>['http://dbpedia.org/resource/Skype_Technologies']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/DeForest_Kelley', 'http://dbpedia.org/resource/George_Takei', 'http://dbpedia.org/resource/James_Doohan', 'http://dbpedia.org/resource/Leonard_Nimoy', 'http://dbpedia.org/resource/Nichelle_Nichols', 'http://dbpedia.org/resource/Walter_Koenig', 'http://dbpedia.org/resource/William_Shatner']</t>
+          <t>['http://dbpedia.org/resource/Skype_Technologies']</t>
         </is>
       </c>
       <c r="D3" t="b">
@@ -558,37 +558,37 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>What is the most frequent cause of death?</t>
+          <t>In which year was Rachel Stevens born?</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Assassination_of_Wissam_al-Hassan']</t>
+          <t>['1978']</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Execution_by_hanging']</t>
+          <t>['1978']</t>
         </is>
       </c>
       <c r="D7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Who was the doctoral supervisor of Albert Einstein?</t>
+          <t>How high is the Yokohama Marine Tower?</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Alfred_Kleiner']</t>
+          <t>['106.07']</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Alfred_Kleiner']</t>
+          <t>['106.07']</t>
         </is>
       </c>
       <c r="D8" t="b">
@@ -598,17 +598,17 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>When was John Adams born?</t>
+          <t>What is Donald Trump's main business?</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>['1735-10-30']</t>
+          <t>['http://dbpedia.org/resource/GoTrump.com', 'http://dbpedia.org/resource/The_Trump_Organization', 'http://dbpedia.org/resource/Trump_Model_Management']</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>['1735-10-30']</t>
+          <t>['http://dbpedia.org/resource/GoTrump.com', 'http://dbpedia.org/resource/The_Trump_Organization', 'http://dbpedia.org/resource/Trump_Model_Management']</t>
         </is>
       </c>
       <c r="D9" t="b">
@@ -618,21 +618,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>how much is the total population of european union?</t>
+          <t>How many people live in Eurasia?</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>['446828803']</t>
+          <t>['5360351985']</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['446828803']</t>
+          <t>['3']</t>
         </is>
       </c>
       <c r="D10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -678,17 +678,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Who developed the video game World of Warcraft?</t>
+          <t>Which university did Angela Merkel attend?</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Blizzard_Entertainment']</t>
+          <t>['http://dbpedia.org/resource/German_Academy_of_Sciences_at_Berlin', 'http://dbpedia.org/resource/Leipzig_University']</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['http://adj.nimh.nih.gov/sscc/', 'http://archone.sourceforge.net', 'http://artica.es/', 'http://asprise.com/ocr-document-scanning-java.net/library-api-about.html%7CAsprise', 'http://avtechscientific.com/', 'http://bairanalytics.com/', 'http://bazaar.launchpad.net/~kirkland/byobu/trunk/view/head:/AUTHORS', 'http://bioinformatics.org/ghemical/ghemical/authors.html', 'http://biostat.mc.vanderbilt.edu/wiki/Main/WilliamDupont', 'http://birdinskygames.com', 'http://blumentals.net', 'http://brenwill.com', 'http://bytonic.de/index.html', 'http://cakefoundation.org/', 'http://calf-studio-gear.org/', 'http://chromium.org', 'http://colloquy.info/project/wiki/Timothy%20Hatcher', 'http://compoundthinking.com/', 'http://cooffice.ntu.edu.sg', 'http://d3web.sourceforge.net', 'http://dbpedia.org/resource/.Gears', 'http://dbpedia.org/resource/.NET_Foundation', 'http://dbpedia.org/resource/.theprodukkt', 'http://dbpedia.org/resource/01_Communique', 'http://dbpedia.org/resource/07th_Expansion', 'http://dbpedia.org/resource/0verflow', 'http://dbpedia.org/resource/1-Up_Studio', 'http://dbpedia.org/resource/10tacle_Mobile_GMBH', 'http://dbpedia.org/resource/10tacle_Studios', 'http://dbpedia.org/resource/10tons_Entertainment', 'http://dbpedia.org/resource/11_bit_studios', 'http://dbpedia.org/resource/1337_Game_Design', 'http://dbpedia.org/resource/13AM_Games', 'http://dbpedia.org/resource/14_Degrees_East', 'http://dbpedia.org/resource/17-Bit', 'http://dbpedia.org/resource/19_Entertainment', 'http://dbpedia.org/resource/1C_Company', 'http://dbpedia.org/resource/1C_Entertainment', 'http://dbpedia.org/resource/1C:Ino-Co', 'http://dbpedia.org/resource/1C:Maddox_Games', 'http://dbpedia.org/resource/1st_Playable_Productions', 'http://dbpedia.org/resource/1STEIN', 'http://dbpedia.org/resource/2015,_Inc.', 'http://dbpedia.org/resource/20th_Century_Fox_Home_Entertainment', 'http://dbpedia.org/resource/20th_Century_Fox_Television', 'http://dbpedia.org/resource/20th_Century_Fox', 'http://dbpedia.org/resource/21-6_Productions', 'http://dbpedia.org/resource/22cans', 'http://dbpedia.org/resource/23_YYZee', 'http://dbpedia.org/resource/258_Productions_AB', 'http://dbpedia.org/resource/2K_Australia', 'http://dbpedia.org/resource/2K_Boston', 'http://dbpedia.org/resource/2K_China', 'http://dbpedia.org/resource/2K_Czech', 'http://dbpedia.org/resource/2K_Los_Angeles', 'http://dbpedia.org/resource/2K_Marin', 'http://dbpedia.org/resource/2waytraffic', 'http://dbpedia.org/resource/2XL_Games', 'http://dbpedia.org/resource/3000AD', 'http://dbpedia.org/resource/321_Studios', 'http://dbpedia.org/resource/32X', 'http://dbpedia.org/resource/343_Industries', 'http://dbpedia.org/resource/38_Studios', 'http://dbpedia.org/resource/3A_Games', 'http://dbpedia.org/resource/3Com', 'http://dbpedia.org/resource/3CX_Phone_System', 'http://dbpedia.org/resource/3CX', 'http://dbpedia.org/resource/3D_Realms', 'http://dbpedia.org/resource/3d6_Games', 'http://dbpedia.org/resource/3DFLOW', 'http://dbpedia.org/resource/3dfx_Interactive', 'http://dbpedia.org/resource/3DO_Interactive_Multiplayer', 'http://dbpedia.org/resource/3L_Alliance', 'http://dbpedia.org/resource/3P_Learning', 'http://dbpedia.org/resource/3QD_Developments', 'http://dbpedia.org/resource/3T_Productions', 'http://dbpedia.org/resource/42_Entertainment', 'http://dbpedia.org/resource/44_Blue_Productions', 'http://dbpedia.org/resource/454_Life_Sciences', 'http://dbpedia.org/resource/49_Games', 'http://dbpedia.org/resource/49Games', 'http://dbpedia.org/resource/4A_Games', 'http://dbpedia.org/resource/4chan', 'http://dbpedia.org/resource/4D_Rulers', 'http://dbpedia.org/resource/4D_SAS', 'http://dbpedia.org/resource/4J_Studios', 'http://dbpedia.org/resource/4Kids_Entertainment', 'http://dbpedia.org/resource/4M_Software', 'http://dbpedia.org/resource/4mm_Games', 'http://dbpedia.org/resource/4X_Studio', 'http://dbpedia.org/resource/4x_Technologies', 'http://dbpedia.org/resource/5000ft', 'http://dbpedia.org/resource/505_Games', 'http://dbpedia.org/resource/5pb.', 'http://dbpedia.org/resource/5th_Cell', 'http://dbpedia.org/resource/64WD_Creation', 'http://dbpedia.org/resource/7_Studios', 'http://dbpedia.org/resource/704Games', 'http://dbpedia.org/resource/7FX', 'http://dbpedia.org/resource/7th_Chord', 'http://dbpedia.org/resource/7th_Level', 'http://dbpedia.org/resource/7th_Sky_Entertainment', 'http://dbpedia.org/resource/8ing/Raizing', 'http://dbpedia.org/resource/8ing', 'http://dbpedia.org/resource/8TV_(Malaysia)', 'http://dbpedia.org/resource/8x8', 'http://dbpedia.org/resource/989_Sports', 'http://dbpedia.org/resource/989_Studios', 'http://dbpedia.org/resource/A-1_Pictures', 'http://dbpedia.org/resource/A-Max', 'http://dbpedia.org/resource/A._D._Miles', 'http://dbpedia.org/resource/A._K._Dewdney', 'http://dbpedia.org/resource/A.I_(company)', 'http://dbpedia.org/resource/A.i._solutions,_Inc.', 'http://dbpedia.org/resource/A&amp;E_Networks', 'http://dbpedia.org/resource/A2_Multimedia', 'http://dbpedia.org/resource/A2A_Simulations', 'http://dbpedia.org/resource/Aalborg_University', 'http://dbpedia.org/resource/Aardman_Animations', 'http://dbpedia.org/resource/Aardvark_Software', 'http://dbpedia.org/resource/Aarhus_University', 'http://dbpedia.org/resource/Aaron_and_Todd_Helbing', 'http://dbpedia.org/resource/Aaron_Giles', 'http://dbpedia.org/resource/Aaron_Horvath', 'http://dbpedia.org/resource/Aaron_J._Seigo', 'http://dbpedia.org/resource/Aaron_McElligott', 'http://dbpedia.org/resource/Aaron_Rahsaan_Thomas', 'http://dbpedia.org/resource/Aaron_Saidman', 'http://dbpedia.org/resource/Aaron_Simpson_(producer)', 'http://dbpedia.org/resource/Aaron_Yonda', 'http://dbpedia.org/resource/Aaron_Zelman', 'http://dbpedia.org/resource/ABB_Group', 'http://dbpedia.org/resource/ABC_Development_Corporation', 'http://dbpedia.org/resource/Abdullah_Al-Salloum', 'http://dbpedia.org/resource/Abdullah_Kadwani', 'http://dbpedia.org/resource/Abe_Ruef', 'http://dbpedia.org/resource/Abersoft', 'http://dbpedia.org/resource/Abhimanyu_Singh_(producer)', 'http://dbpedia.org/resource/Ableton', 'http://dbpedia.org/resource/ABN_AMRO', 'http://dbpedia.org/resource/About_Fun', 'http://dbpedia.org/resource/Abraham_Hirschfeld', 'http://dbpedia.org/resource/ABS-CBN_Corporation', 'http://dbpedia.org/resource/ABS-CBN_Entertainment', 'http://dbpedia.org/resource/ABS-CBN_Lingkod_Kapamilya_Foundation', 'http://dbpedia.org/resource/ABS-CBN_News_&amp;_Current_Affairs', 'http://dbpedia.org/resource/ABS-CBN_News_and_Current_Affairs', 'http://dbpedia.org/resource/ABS-CBN_News', 'http://dbpedia.org/resource/ABS-CBN_Regional_Network_Group', 'http://dbpedia.org/resource/ABS-CBN_Sports', 'http://dbpedia.org/resource/ABS-CBN', 'http://dbpedia.org/resource/AbsInt', 'http://dbpedia.org/resource/Absolute_Entertainment', 'http://dbpedia.org/resource/Absolutist_(video_game_developer)', 'http://dbpedia.org/resource/Abstraction_Games', 'http://dbpedia.org/resource/Abzu_(company)', 'http://dbpedia.org/resource/Academy_Software_Foundation', 'http://dbpedia.org/resource/Accelrys', 'http://dbpedia.org/resource/Accenture', 'http://dbpedia.org/resource/Accentus_Music', 'http://dbpedia.org/resource/Access_(company)', 'http://dbpedia.org/resource/Access_Co.', 'http://dbpedia.org/resource/Access_Games', 'http://dbpedia.org/resource/Access_Software', 'http://dbpedia.org/resource/Acclaim_Cheltenham', 'http://dbpedia.org/resource/Acclaim_Entertainment', 'http://dbpedia.org/resource/Acclaim_Studios_Austin', 'http://dbpedia.org/resource/Acclaim_Studios_Cheltenham', 'http://dbpedia.org/resource/Acclaim_Studios_London', 'http://dbpedia.org/resource/Acclaim_Studios_Manchester', 'http://dbpedia.org/resource/Acclaim_Studios_Salt_Lake_City', 'http://dbpedia.org/resource/Acclaim_Studios_Teesside', 'http://dbpedia.org/resource/Accolade_(company)', 'http://dbpedia.org/resource/Accomplice_Television', 'http://dbpedia.org/resource/Accursed_Toys', 'http://dbpedia.org/resource/ACD_Systems', 'http://dbpedia.org/resource/ACE_Team', 'http://dbpedia.org/resource/Aces_Game_Studio', 'http://dbpedia.org/resource/Acid_Nerve', 'http://dbpedia.org/resource/Acid_Software', 'http://dbpedia.org/resource/ACME_Interactive', 'http://dbpedia.org/resource/Acon_Digital', 'http://dbpedia.org/resource/ACONY_(company)', 'http://dbpedia.org/resource/Acorn_Computers', 'http://dbpedia.org/resource/Acornsoft', 'http://dbpedia.org/resource/ACOT', 'http://dbpedia.org/resource/Acquire_(company)', 'http://dbpedia.org/resource/Acquire_(game_developer)', 'http://dbpedia.org/resource/Acronis', 'http://dbpedia.org/resource/Acropoliis_Entertainment', 'http://dbpedia.org/resource/Across_Systems', 'http://dbpedia.org/resource/Act_Japan', 'http://dbpedia.org/resource/Actian_Corporation', 'http://dbpedia.org/resource/Actian', 'http://dbpedia.org/resource/Action_Button_Entertainment', 'http://dbpedia.org/resource/Action_Forms', 'http://dbpedia.org/resource/Activant', 'http://dbpedia.org/resource/ActiveState', 'http://dbpedia.org/resource/Activision', 'http://dbpedia.org/resource/Actoz_Soft', 'http://dbpedia.org/resource/ActozSoft', 'http://dbpedia.org/resource/Actual_Entertainment', 'http://dbpedia.org/resource/AdaCore', 'http://dbpedia.org/resource/Adam_Beechen', 'http://dbpedia.org/resource/Adam_Cadre', 'http://dbpedia.org/resource/Adam_Dunkels', 'http://dbpedia.org/resource/Adam_F._Goldberg', 'http://dbpedia.org/resource/Adam_Horowitz_(screenwriter)', 'http://dbpedia.org/resource/Adam_Kennedy_(programmer)', 'http://dbpedia.org/resource/Adam_Megacz', 'http://dbpedia.org/resource/Adam_Muto', 'http://dbpedia.org/resource/Adam_Peltzman', 'http://dbpedia.org/resource/Adam_Retter', "http://dbpedia.org/resource/Adam's_Mark", 'http://dbpedia.org/resource/Addeen_Multimedia_Sdn._Bhd.', 'http://dbpedia.org/resource/Addictive_Games', 'http://dbpedia.org/resource/Addison_Mizner', 'http://dbpedia.org/resource/ADDPCS_(company)', 'http://dbpedia.org/resource/Addstor,_Inc.', 'http://dbpedia.org/resource/Addy_Osmani', 'http://dbpedia.org/resource/Adele_Goldberg_(computer_scientist)', 'http://dbpedia.org/resource/Adeline_Software_International', 'http://dbpedia.org/resource/AdHoc_Studio', 'http://dbpedia.org/resource/Adi_Hasak', 'http://dbpedia.org/resource/Adil_Ray', 'http://dbpedia.org/resource/Aditya_Mahajan', 'http://dbpedia.org/resource/ADK_(company)', 'http://dbpedia.org/resource/Admiral_Jota', 'http://dbpedia.org/resource/Adness_Entertainment', 'http://dbpedia.org/resource/Adobe_Inc.', 'http://dbpedia.org/resource/Adobe_Systems', 'http://dbpedia.org/resource/Adrenalin_Entertainment', 'http://dbpedia.org/resource/Adrenium_Games', 'http://dbpedia.org/resource/Adri_van_Os', 'http://dbpedia.org/resource/Adrian_Millett', 'http://dbpedia.org/resource/Adrian_Zecha', 'http://dbpedia.org/resource/Adriana_Barraza', 'http://dbpedia.org/resource/Adult_Swim_Games', 'http://dbpedia.org/resource/Adult_Swim', 'http://dbpedia.org/resource/Advance_Communication_Company', 'http://dbpedia.org/resource/Advance_Communication', 'http://dbpedia.org/resource/Advance_Reality_Interactive', 'http://dbpedia.org/resource/Advanced_Chemistry_Development', 'http://dbpedia.org/resource/Advanced_Micro_Devices', 'http://dbpedia.org/resource/Advanced_Productions', 'http://dbpedia.org/resource/Advanced_Systems_Concepts,_Inc.', 'http://dbpedia.org/resource/Adventure_International', 'http://dbpedia.org/resource/Adventure_Soft', 'http://dbpedia.org/resource/Aerospike_(company)', 'http://dbpedia.org/resource/Affect_(company)', 'http://dbpedia.org/resource/Africa-Israel', 'http://dbpedia.org/resource/Aga_Khan_Development_Network', 'http://dbpedia.org/resource/Agat_Films_&amp;_Cie_–_Ex_Nihilo', 'http://dbpedia.org/resource/Agatsuma_Entertainment', 'http://dbpedia.org/resource/AGD_Interactive', 'http://dbpedia.org/resource/Ageia', "http://dbpedia.org/resource/Agence_nationale_de_la_sécurité_des_systèmes_d'information", 'http://dbpedia.org/resource/Agencia_Atlas', 'http://dbpedia.org/resource/Agenda_(software_developer)', 'http://dbpedia.org/resource/AGEOD', 'http://dbpedia.org/resource/AgeofRappelz', 'http://dbpedia.org/resource/Agetec', 'http://dbpedia.org/resource/AGFA', 'http://dbpedia.org/resource/Agisoft_LLC', 'http://dbpedia.org/resource/Agmondisham_Vesey_(died_1785)', 'http://dbpedia.org/resource/Agora_SA', 'http://dbpedia.org/resource/Agung_Podomoro_Land', 'http://dbpedia.org/resource/AH-Software', 'http://dbpedia.org/resource/Aicom', 'http://dbpedia.org/resource/Aidy_Bryant', 'http://dbpedia.org/resource/AIG_Global_Real_Estate', 'http://dbpedia.org/resource/AIG/Lincoln', 'http://dbpedia.org/resource/AIGRIND_LLC', 'http://dbpedia.org/resource/AiLive', 'http://dbpedia.org/resource/Aimsun', 'http://dbpedia.org/resource/Air_Force_Research_Laboratory', 'http://dbpedia.org/resource/Airship_Syndicate', 'http://dbpedia.org/resource/Airtight_Games', 'http://dbpedia.org/resource/Aisha_Enterprises,_Inc', 'http://dbpedia.org/resource/Aisystem_Tokyo', 'http://dbpedia.org/resource/Ajax.org', 'http://dbpedia.org/resource/Ajinomoto', 'http://dbpedia.org/resource/Akabeisoft2', 'http://dbpedia.org/resource/Akaoni_Studio', 'http://dbpedia.org/resource/Akella', 'http://dbpedia.org/resource/Aki_Corporation', 'http://dbpedia.org/resource/Akira_Ueda', 'http://dbpedia.org/resource/Akiva_Goldsman', 'http://dbpedia.org/resource/Aksjeselskap', 'http://dbpedia.org/resource/Aksys_Games', 'http://dbpedia.org/resource/Aktiebolag', 'http://dbpedia.org/resource/Al_Attar_Properties', 'http://dbpedia.org/resource/Al_Mahad_Group_of_Companies', 'http://dbpedia.org/resource/Al_Nekhreh_Contracting_Co._LLC', 'http://dbpedia.org/resource/Al_Sayyah_&amp;_Sons_Investment_Co._LLC', 'http://dbpedia.org/resource/Al_Shafar_General_Contracting_Co_(L.L.C.)', 'http://dbpedia.org/resource/Al_Smith', 'http://dbpedia.org/resource/Aladdin_Systems', 'http://dbpedia.org/resource/Alan_B._McElroy', 'http://dbpedia.org/resource/Alan_Bond', 'http://dbpedia.org/resource/Alan_Burnett', 'http://dbpedia.org/resource/Alan_Cox_(computer_programmer)', 'http://dbpedia.org/resource/Alan_Jardine_(programmer)', 'http://dbpedia.org/resource/Alan_Kay', 'http://dbpedia.org/resource/Alan_Kitching', 'http://dbpedia.org/resource/Alan_Plater', 'http://dbpedia.org/resource/Alan_Shalleck', 'http://dbpedia.org/resource/Alan_Turing', 'http://dbpedia.org/resource/Alan_Zaslove', 'http://dbpedia.org/resource/Alasdair_Beckett-King', 'http://dbpedia.org/resource/Albany_Crown', 'http://dbpedia.org/resource/Albert_E._Carlton', 'http://dbpedia.org/resource/Albert,_Prince_Consort', 'http://dbpedia.org/resource/Alberto_Gómez_(writer)', 'http://dbpedia.org/resource/Alberto_Santini_Lara', 'http://dbpedia.org/resource/Alcachofa_Soft', 'http://dbpedia.org/resource/Alcan', 'http://dbpedia.org/resource/Alchemist_(company)', 'http://dbpedia.org/resource/Alchemy_Software_Development_Limited', 'http://dbpedia.org/resource/Alcoa', 'http://dbpedia.org/resource/Alcon_Entertainment', 'http://dbpedia.org/resource/ALcot_Honey_Comb', 'http://dbpedia.org/resource/ALcot', 'http://dbpedia.org/resource/Aldar_Properties', 'http://dbpedia.org/resource/Aldebaran_Robotics', 'http://dbpedia.org/resource/Aldo_Vitagliano', 'http://dbpedia.org/resource/Aldus_Corporation', 'http://dbpedia.org/resource/Alec_Muffett', 'http://dbpedia.org/resource/Alejandro_Bustillo', 'http://dbpedia.org/resource/Aleks_Essex', 'http://dbpedia.org/resource/Aleksandr_Boyarsky', 'http://dbpedia.org/resource/Aleksandr_Smirnov_(producer)', 'http://dbpedia.org/resource/Alessandro_Migliaccio', 'http://dbpedia.org/resource/Alessandro_Tasora', 'http://dbpedia.org/resource/Alessandro_Vespignani', 'http://dbpedia.org/resource/Alex_Gansa', 'http://dbpedia.org/resource/Alex_Hirsch', 'http://dbpedia.org/resource/Alex_Kurtzman', 'http://dbpedia.org/resource/Alex_Madonna', 'http://dbpedia.org/resource/Alex_McLean', 'http://dbpedia.org/resource/Alex_Tew', 'http://dbpedia.org/resource/Alex_Timbers', 'http://dbpedia.org/resource/Alex_Zamm', 'http://dbpedia.org/resource/Alexander_Aiken', 'http://dbpedia.org/resource/Alexander_Brevig', 'http://dbpedia.org/resource/Alexander_Cary,_Master_of_Falkland', 'http://dbpedia.org/resource/Alexander_Duff,_1st_Duke_of_Fife', 'http://dbpedia.org/resource/Alexander_Muse', 'http://dbpedia.org/resource/Alexander_Salkind', 'http://dbpedia.org/resource/Alexandra_Cunningham', 'http://dbpedia.org/resource/Alfa_System', 'http://dbpedia.org/resource/Alfred_Akirov', 'http://dbpedia.org/resource/Alfred_Gough', 'http://dbpedia.org/resource/Alfred_Gwynne_Vanderbilt', 'http://dbpedia.org/resource/Alfred_Shaughnessy', 'http://dbpedia.org/resource/Alfred_Wegener_Institute_for_Polar_and_Marine_Research', 'http://dbpedia.org/resource/Alfredo_Flores', 'http://dbpedia.org/resource/Alfresco_(software)', 'http://dbpedia.org/resource/Algoryx_Simulation_AB', 'http://dbpedia.org/resource/Ali_Adler', 'http://dbpedia.org/resource/Ali_LeRoi', 'http://dbpedia.org/resource/Alias_Systems_Corporation', 'http://dbpedia.org/resource/Aliasworlds_Entertainment', 'http://dbpedia.org/resource/Alibaba_Cloud', 'http://dbpedia.org/resource/Alibaba_Group', 'http://dbpedia.org/resource/Alibre,_LLC', 'http://dbpedia.org/resource/AliceSoft', 'http://dbpedia.org/resource/Alicia_Luna', 'http://dbpedia.org/resource/Alientrap', 'http://dbpedia.org/resource/Alison_Snowden', 'http://dbpedia.org/resource/Alkacon_Software', 'http://dbpedia.org/resource/Alko', 'http://dbpedia.org/resource/Allaire_Corporation', 'http://dbpedia.org/resource/Allan_Heinberg', 'http://dbpedia.org/resource/Allan_Neuwirth', 'http://dbpedia.org/resource/Allen_Funt', 'http://dbpedia.org/resource/Allen_Newell', 'http://dbpedia.org/resource/Allen_Rucker', 'http://dbpedia.org/resource/Allen_Spraggett', 'http://dbpedia.org/resource/Alliance_for_Open_Media', 'http://dbpedia.org/resource/Allied_Kingdoms', 'http://dbpedia.org/resource/Allied_London', 'http://dbpedia.org/resource/Allied_Telesis', 'http://dbpedia.org/resource/Alligata', 'http://dbpedia.org/resource/Allison_Grodner', 'http://dbpedia.org/resource/Allods_Team', 'http://dbpedia.org/resource/Allu_Aravind', 'http://dbpedia.org/resource/Allumer', 'http://dbpedia.org/resource/Aloy_Adlawan', 'http://dbpedia.org/resource/Alpha_Denshi', 'http://dbpedia.org/resource/Alpha_Microsystems', 'http://dbpedia.org/resource/Alpha_Software', 'http://dbpedia.org/resource/Alpha_Unit', 'http://dbpedia.org/resource/AlphaDream_Corporation', 'http://dbpedia.org/resource/AlphaDream', 'http://dbpedia.org/resource/Alt_Media', 'http://dbpedia.org/resource/Alt1', 'http://dbpedia.org/resource/Altair_Engineering', 'http://dbpedia.org/resource/ALTAP', 'http://dbpedia.org/resource/Altar_Interactive', 'http://dbpedia.org/resource/ALTAR_Interactive', 'http://dbpedia.org/resource/AlternativaPlatform', 'http://dbpedia.org/resource/Alternative_Reality_Technologies', 'http://dbpedia.org/resource/Alternative_Software', 'http://dbpedia.org/resource/Altinex_Inc.', 'http://dbpedia.org/resource/Altium', 'http://dbpedia.org/resource/Altor_Systems', 'http://dbpedia.org/resource/Altova', 'http://dbpedia.org/resource/Altran', 'http://dbpedia.org/resource/Altsys', 'http://dbpedia.org/resource/Alvin_Yapan', 'http://dbpedia.org/resource/Alvion', 'http://dbpedia.org/resource/AMA_Studios', 'http://dbpedia.org/resource/Amabilis_Software', 'http://dbpedia.org/resource/Amanita_Design', 'http://dbpedia.org/resource/Amaze_Entertainment', 'http://dbpedia.org/resource/Amazon_(company)', 'http://dbpedia.org/resource/Amazon_Game_Studios', 'http://dbpedia.org/resource/Amazon_Games_Orange_County', 'http://dbpedia.org/resource/Amazon_Studios', 'http://dbpedia.org/resource/Amazon_Web_Services', 'http://dbpedia.org/resource/Amazon.com,_Inc.', 'http://dbpedia.org/resource/Amazon.com', 'http://dbpedia.org/resource/Ambiera', 'http://dbpedia.org/resource/Ambrella_(Marigul)', 'http://dbpedia.org/resource/Ambrella', 'http://dbpedia.org/resource/Ambrosia_Software', 'http://dbpedia.org/resource/AMD', 'http://dbpedia.org/resource/Amdahl_Corporation', 'http://dbpedia.org/resource/America_Online', 'http://dbpedia.org/resource/América_Televisión', 'http://dbpedia.org/resource/American_Action_(company)', 'http://dbpedia.org/resource/American_Astronomical_Society', 'http://dbpedia.org/resource/American_Broadcasting_Company', 'http://dbpedia.org/resource/American_Game_Cartridges', 'http://dbpedia.org/resource/American_International_Group', 'http://dbpedia.org/resource/American_Laser_Games', 'http://dbpedia.org/resource/American_Mathematical_Society', 'http://dbpedia.org/resource/American_McGee', 'http://dbpedia.org/resource/American_Museum_of_Natural_History', 'http://dbpedia.org/resource/American_National_Standards_Institute', 'http://dbpedia.org/resource/American_Society_of_Civil_Engineers', 'http://dbpedia.org/resource/American_Telephone_&amp;_Telegraph', 'http://dbpedia.org/resource/American_Tract_Society', 'http://dbpedia.org/resource/Ameriprise_Financial', 'http://dbpedia.org/resource/Ames_Laboratory', 'http://dbpedia.org/resource/Ames_Research_Center', 'http://dbpedia.org/resource/Amherst,_Ohio', 'http://dbpedia.org/resource/Amiga_Corporation', 'http://dbpedia.org/resource/Amiga', 'http://dbpedia.org/resource/Amirali_Rajan', 'http://dbpedia.org/resource/Amit_Cohen', 'http://dbpedia.org/resource/AMLI_Residential', 'http://dbpedia.org/resource/Amos_Eno', 'http://dbpedia.org/resource/AMP_Capital_Investors', 'http://dbpedia.org/resource/AMP_Capital', 'http://dbpedia.org/resource/AMP_Limited', 'http://dbpedia.org/resource/Amplitude_Studios', 'http://dbpedia.org/resource/Amstrad_CPC', 'http://dbpedia.org/resource/Amstrad', 'http://dbpedia.org/resource/Amusement_Vision', 'http://dbpedia.org/resource/Amuze', 'http://dbpedia.org/resource/Amy_and_Wendy_Engelberg', 'http://dbpedia.org/resource/Amy_B._Harris', 'http://dbpedia.org/resource/ANALOG_Computing', 'http://dbpedia.org/resource/Analog_Devices', 'http://dbpedia.org/resource/Analyse-it_Software,_Ltd.', 'http://dbpedia.org/resource/Analytical_Graphics,_Inc.', 'http://dbpedia.org/resource/Anarchy_Enterprises', 'http://dbpedia.org/resource/Anark_Game_Studios', 'http://dbpedia.org/resource/Anchor_Inc.', 'http://dbpedia.org/resource/AnchorFree', 'http://dbpedia.org/resource/Ancient_(company)', 'http://dbpedia.org/resource/Anco_Software', 'http://dbpedia.org/resource/Andamiro', 'http://dbpedia.org/resource/Anders_Jahre', 'http://dbpedia.org/resource/Andhra_Pradesh_Industrial_Infrastructure_Corporation', 'http://dbpedia.org/resource/André_Balazs', 'http://dbpedia.org/resource/André_Bormanis', 'http://dbpedia.org/resource/André_Nemec', 'http://dbpedia.org/resource/André_Wüthrich', 'http://dbpedia.org/resource/Andrea_Greppi', 'http://dbpedia.org/resource/Andrea_Loredan', 'http://dbpedia.org/resource/Andrea_Lucchetta', 'http://dbpedia.org/resource/Andreas_Dilger', 'http://dbpedia.org/resource/Andreas_Illiger', 'http://dbpedia.org/resource/Andreas_Morfonios', 'http://dbpedia.org/resource/Andreas_Raab', 'http://dbpedia.org/resource/Andrei_Voronkov', 'http://dbpedia.org/resource/Andrés_Indriðason', 'http://dbpedia.org/resource/Andrew_Aksyonoff', 'http://dbpedia.org/resource/Andrew_Alexander_(producer)', 'http://dbpedia.org/resource/Andrew_Bradfield', 'http://dbpedia.org/resource/Andrew_Braybrook', 'http://dbpedia.org/resource/Andrew_Dabb', 'http://dbpedia.org/resource/Andrew_Davenport', 'http://dbpedia.org/resource/Andrew_Davies_(writer)', 'http://dbpedia.org/resource/Andrew_Glaister', 'http://dbpedia.org/resource/Andrew_Glassman', 'http://dbpedia.org/resource/Andrew_Howard_(robotics)', 'http://dbpedia.org/resource/Andrew_J._Fenady', 'http://dbpedia.org/resource/Andrew_Kreisberg', 'http://dbpedia.org/resource/Andrew_Leker', 'http://dbpedia.org/resource/Andrew_McCallum', 'http://dbpedia.org/resource/Andrew_Miller_(actor)', 'http://dbpedia.org/resource/Andrew_Nicholls_and_Darrell_Vickers', 'http://dbpedia.org/resource/Andrew_Nicholls', 'http://dbpedia.org/resource/Andrew_Plotkin', 'http://dbpedia.org/resource/Andrew_S._Tanenbaum', 'http://dbpedia.org/resource/Andrew_Sabiston', 'http://dbpedia.org/resource/Andrew_Sasson', 'http://dbpedia.org/resource/Andrew_Severn', 'http://dbpedia.org/resource/Andrew_Tanenbaum', 'http://dbpedia.org/resource/Andrew_W._Marlowe', 'http://dbpedia.org/resource/Andrew_W._Mellon', 'http://dbpedia.org/resource/Andrey_Pominov', 'http://dbpedia.org/resource/Android_(operating_system)', 'http://dbpedia.org/resource/Androsoft', 'http://dbpedia.org/resource/Andy_Daly', 'http://dbpedia.org/resource/Andy_Heyward', 'http://dbpedia.org/resource/Andy_Jervis', 'http://dbpedia.org/resource/Andy_Knight', 'http://dbpedia.org/resource/Andy_Lassner', 'http://dbpedia.org/resource/Andy_Sipes', 'http://dbpedia.org/resource/Andy_Wray', 'http://dbpedia.org/resource/Angela_Santomero', 'http://dbpedia.org/resource/Angels_Landing_Partners_LLC', 'http://dbpedia.org/resource/AngelSmile', 'http://dbpedia.org/resource/Anglia_Multimedia', 'http://dbpedia.org/resource/Anglia_Television', 'http://dbpedia.org/resource/Anglo_American_plc', 'http://dbpedia.org/resource/Anil_Gupta_(writer)', 'http://dbpedia.org/resource/Anil_V._Rao', 'http://dbpedia.org/resource/Anim-X', 'http://dbpedia.org/resource/Anima_ppd-interactive', 'http://dbpedia.org/resource/Animasia_Studio', 'http://dbpedia.org/resource/AnimaTek', 'http://dbpedia.org/resource/Animation_F/X', 'http://dbpedia.org/resource/Animation_Magic', 'http://dbpedia.org/resource/Anime_International_Company', 'http://dbpedia.org/resource/Animoca_Brands', 'http://dbpedia.org/resource/Animoca', 'http://dbpedia.org/resource/Animonsta_Studios', 'http://dbpedia.org/resource/Anino_Games', 'http://dbpedia.org/resource/Anirog_Software', 'http://dbpedia.org/resource/Ankama_Games', 'http://dbpedia.org/resource/Ankama', 'http://dbpedia.org/resource/Ankit_Fadia', 'http://dbpedia.org/resource/Ann_Arbor_Softworks', 'http://dbpedia.org/resource/Anna_Anthropy', 'http://dbpedia.org/resource/Anna_Fricke', 'http://dbpedia.org/resource/Anna_Hatzisofia', 'http://dbpedia.org/resource/Anna_Muylaert', 'http://dbpedia.org/resource/Anna_Wallner', 'http://dbpedia.org/resource/Anne_E._Carpenter', 'http://dbpedia.org/resource/Anne_Wood', 'http://dbpedia.org/resource/Annette_Tison', 'http://dbpedia.org/resource/ANSES', 'http://dbpedia.org/resource/ANSI_C', 'http://dbpedia.org/resource/ANSTO', 'http://dbpedia.org/resource/Ansys', 'http://dbpedia.org/resource/ANT_Software_Limited', 'http://dbpedia.org/resource/Anthony_Campagna', 'http://dbpedia.org/resource/Anthony_Cipriano', 'http://dbpedia.org/resource/Anthony_D._Giarratana', 'http://dbpedia.org/resource/Anthony_Minghella', 'http://dbpedia.org/resource/Antic_Software', 'http://dbpedia.org/resource/Antics_Technologies', 'http://dbpedia.org/resource/Antilogic_Software', 'http://dbpedia.org/resource/Antimatter_Games', 'http://dbpedia.org/resource/Antix_Productions', 'http://dbpedia.org/resource/Antonio_Da_Cruz', 'http://dbpedia.org/resource/Antony_Crowther', 'http://dbpedia.org/resource/Antradar', 'http://dbpedia.org/resource/Antulio_Jimenez_Pons', 'http://dbpedia.org/resource/Antv', 'http://dbpedia.org/resource/Anuman_Interactive', 'http://dbpedia.org/resource/AOL', 'http://dbpedia.org/resource/Apache_Software_Foundation', 'http://dbpedia.org/resource/Apache_Software', 'http://dbpedia.org/resource/APD_Inc.', 'http://dbpedia.org/resource/Apex_Computer_Productions', 'http://dbpedia.org/resource/APh_Technological_Consulting', 'http://dbpedia.org/resource/Apocalypse_Studios', 'http://dbpedia.org/resource/Apogee_Software', 'http://dbpedia.org/resource/Apollo_Computer', 'http://dbpedia.org/resource/Apollosoft', 'http://dbpedia.org/resource/Apothecary_Studios', 'http://dbpedia.org/resource/Appaloosa_Interactive', 'http://dbpedia.org/resource/AppAssure_Software', 'http://dbpedia.org/resource/Appcelerator', 'http://dbpedia.org/resource/Apple_Computer', 'http://dbpedia.org/resource/Apple_Inc.', 'http://dbpedia.org/resource/Apple_Inc', 'http://dbpedia.org/resource/Applied_Engineering', 'http://dbpedia.org/resource/Applied_Maths', 'http://dbpedia.org/resource/Applied_Science_International', 'http://dbpedia.org/resource/Approximatrix,_LLC', 'http://dbpedia.org/resource/AppTapp_Team', 'http://dbpedia.org/resource/Appxplore_(company)', 'http://dbpedia.org/resource/Aprinet', 'http://dbpedia.org/resource/APT_Entertainment', 'http://dbpedia.org/resource/Aptana', 'http://dbpedia.org/resource/Aptech_Systems', 'http://dbpedia.org/resource/Apus_Software', 'http://dbpedia.org/resource/AQ_Interactive', 'http://dbpedia.org/resource/Aqua_Pacific', 'http://dbpedia.org/resource/Aquaplus', 'http://dbpedia.org/resource/Aquaveo', 'http://dbpedia.org/resource/Aquria', 'http://dbpedia.org/resource/Araneta_Group', 'http://dbpedia.org/resource/Arberth_Studios', 'http://dbpedia.org/resource/Arc_Developments', 'http://dbpedia.org/resource/Arc_System_Works', 'http://dbpedia.org/resource/Arcade_Moon', 'http://dbpedia.org/resource/Arcadia_Systems', 'http://dbpedia.org/resource/Arcane_Kids', 'http://dbpedia.org/resource/Arcanium_Productions', 'http://dbpedia.org/resource/Arcelor_Mittal', 'http://dbpedia.org/resource/Arcen_Games', 'http://dbpedia.org/resource/Archer_Maclean', 'http://dbpedia.org/resource/Archetype_Studios', 'http://dbpedia.org/resource/Architectural_Services_Department', 'http://dbpedia.org/resource/Archive_Entertainment', 'http://dbpedia.org/resource/ArcSoft', 'http://dbpedia.org/resource/Ardour_(software)', 'http://dbpedia.org/resource/AREA_Property_Partners', 'http://dbpedia.org/resource/ArenaNet', 'http://dbpedia.org/resource/Argo_Games', 'http://dbpedia.org/resource/Argonaut_Games', 'http://dbpedia.org/resource/Argonaut_Sheffield', 'http://dbpedia.org/resource/Argonaut_Software', 'http://dbpedia.org/resource/Argonne_National_Laboratory', 'http://dbpedia.org/resource/Argos_Comunicación', 'http://dbpedia.org/resource/Argos_Television', 'http://dbpedia.org/resource/Argus_Press_Software', 'http://dbpedia.org/resource/Arief_Suditomo', 'http://dbpedia.org/resource/Ariel_Schulman', 'http://dbpedia.org/resource/Arika', 'http://dbpedia.org/resource/Ariolasoft', 'http://dbpedia.org/resource/Aristotle_University_of_Thessaloniki', 'http://dbpedia.org/resource/Ariya_Hidayat', 'http://dbpedia.org/resource/Arjan_Dikhoff', 'http://dbpedia.org/resource/Arkadium', 'http://dbpedia.org/resource/Arkane_Studios', 'http://dbpedia.org/resource/Arkedo_Studio', 'http://dbpedia.org/resource/Arlen_Realty_and_Development_Corporation', 'http://dbpedia.org/resource/Arlene_Klasky', 'http://dbpedia.org/resource/Arlington_C._Hall', 'http://dbpedia.org/resource/Arm_Holdings', 'http://dbpedia.org/resource/Armada_Hoffler', 'http://dbpedia.org/resource/Armature_Studio', 'http://dbpedia.org/resource/Armen_Petrosyan_(Mench)', 'http://dbpedia.org/resource/Armin_Rigo', 'http://dbpedia.org/resource/Armin_Ronacher', 'http://dbpedia.org/resource/Armor_Games', 'http://dbpedia.org/resource/Army_Research_Laboratory', 'http://dbpedia.org/resource/Arne_Sultan', 'http://dbpedia.org/resource/Arnowitz_Studios', 'http://dbpedia.org/resource/Aron_Eli_Coleite', 'http://dbpedia.org/resource/Arris_Group', 'http://dbpedia.org/resource/Arrowhead_Game_Studios', 'http://dbpedia.org/resource/Arsys_Software', 'http://dbpedia.org/resource/Art_And_Animation_studio', 'http://dbpedia.org/resource/Art_Co.,_Ltd', 'http://dbpedia.org/resource/Art_Data_Interactive', 'http://dbpedia.org/resource/Art_Wallace', 'http://dbpedia.org/resource/Artdink', 'http://dbpedia.org/resource/Artech_Digital_Entertainment', 'http://dbpedia.org/resource/Artech_Studios', 'http://dbpedia.org/resource/Artefacts_Studio', 'http://dbpedia.org/resource/Artematica', 'http://dbpedia.org/resource/ArtePiazza', 'http://dbpedia.org/resource/Arthur_(TV_presenter)', 'http://dbpedia.org/resource/Arthur_Brisbane', 'http://dbpedia.org/resource/Arthur_Davis_(animator)', 'http://dbpedia.org/resource/Arthur_Silver', 'http://dbpedia.org/resource/Artic_Computing', 'http://dbpedia.org/resource/Artifice_Studio', 'http://dbpedia.org/resource/Artificial_Life,_Inc.', 'http://dbpedia.org/resource/Artificial_Mind_&amp;_Movement', 'http://dbpedia.org/resource/Artificial_Mind_and_Movement', 'http://dbpedia.org/resource/Artificial_Solutions', 'http://dbpedia.org/resource/Artificial_Studios', 'http://dbpedia.org/resource/ARTIS_Software', 'http://dbpedia.org/resource/Artix_Entertainment', 'http://dbpedia.org/resource/Artman21', 'http://dbpedia.org/resource/Artoon', 'http://dbpedia.org/resource/Arturo_Castro_(Computer_Programmer)', 'http://dbpedia.org/resource/Artworx', 'http://dbpedia.org/resource/Arunabh_Kumar', 'http://dbpedia.org/resource/ARUSH_Entertainment', 'http://dbpedia.org/resource/Arxel_Tribe', 'http://dbpedia.org/resource/Arzest', 'http://dbpedia.org/resource/Asaph_Fipke', 'http://dbpedia.org/resource/Ascaron_Entertainment', 'http://dbpedia.org/resource/Ascaron', 'http://dbpedia.org/resource/ASCII_(com</t>
+          <t>['http://dbpedia.org/resource/Leipzig_University']</t>
         </is>
       </c>
       <c r="D13" t="b">
@@ -698,17 +698,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Where was JFK assassinated?</t>
+          <t>Give me all movies with Tom Cruise.</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Dallas']</t>
+          <t>['http://dbpedia.org/resource/A_Few_Good_Men', 'http://dbpedia.org/resource/All_the_Right_Moves_(film)', 'http://dbpedia.org/resource/American_Made_(film)', 'http://dbpedia.org/resource/Born_on_the_Fourth_of_July_(film)', 'http://dbpedia.org/resource/Cocktail_(1988_film)', 'http://dbpedia.org/resource/Collateral_(film)', 'http://dbpedia.org/resource/Days_of_Thunder', 'http://dbpedia.org/resource/Edge_of_Tomorrow', 'http://dbpedia.org/resource/Eyes_Wide_Shut', 'http://dbpedia.org/resource/Far_and_Away__Far_and_Away__1', 'http://dbpedia.org/resource/Interview_with_the_Vampire_(film)', 'http://dbpedia.org/resource/Jack_Reacher_(film)', 'http://dbpedia.org/resource/Jack_Reacher:_Never_Go_Back', 'http://dbpedia.org/resource/Jerry_Maguire__Jerry_Maguire__1', 'http://dbpedia.org/resource/Knight_and_Day__Knight_and_Day__1', 'http://dbpedia.org/resource/Legend_(1985_film)', 'http://dbpedia.org/resource/Lions_for_Lambs', "http://dbpedia.org/resource/Losin'_It", 'http://dbpedia.org/resource/Magnolia_(film)__Magnolia__1', 'http://dbpedia.org/resource/Minority_Report_(film)', 'http://dbpedia.org/resource/Mission:_Impossible_–_Dead_Reckoning_Part_One', 'http://dbpedia.org/resource/Mission:_Impossible_–_Dead_Reckoning_Part_Two', 'http://dbpedia.org/resource/Mission:_Impossible_–_Fallout', 'http://dbpedia.org/resource/Mission:_Impossible_–_Ghost_Protocol', 'http://dbpedia.org/resource/Mission:_Impossible_–_Rogue_Nation', 'http://dbpedia.org/resource/Mission:_Impossible_(film)', 'http://dbpedia.org/resource/Mission:_Impossible_2', 'http://dbpedia.org/resource/Mission:_Impossible_III', 'http://dbpedia.org/resource/Oblivion_(2013_film)', 'http://dbpedia.org/resource/Rain_Man', 'http://dbpedia.org/resource/Risky_Business', 'http://dbpedia.org/resource/Rock_of_Ages_(2012_film)', 'http://dbpedia.org/resource/Taps_(film)', 'http://dbpedia.org/resource/The_Color_of_Money', 'http://dbpedia.org/resource/The_Firm_(1993_film)', 'http://dbpedia.org/resource/The_Last_Samurai', 'http://dbpedia.org/resource/The_Mummy_(2017_film)', 'http://dbpedia.org/resource/The_Outsiders_(film)', 'http://dbpedia.org/resource/Top_Gun:_Maverick', 'http://dbpedia.org/resource/Top_Gun', 'http://dbpedia.org/resource/Valkyrie_(film)', 'http://dbpedia.org/resource/Vanilla_Sky', 'http://dbpedia.org/resource/War_of_the_Worlds_(2005_film)']</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Dallas']</t>
+          <t>['http://dbpedia.org/resource/A_Few_Good_Men', 'http://dbpedia.org/resource/All_the_Right_Moves_(film)', 'http://dbpedia.org/resource/American_Made_(film)', 'http://dbpedia.org/resource/Born_on_the_Fourth_of_July_(film)', 'http://dbpedia.org/resource/Cocktail_(1988_film)', 'http://dbpedia.org/resource/Collateral_(film)', 'http://dbpedia.org/resource/Days_of_Thunder', 'http://dbpedia.org/resource/Edge_of_Tomorrow', 'http://dbpedia.org/resource/Eyes_Wide_Shut', 'http://dbpedia.org/resource/Far_and_Away__Far_and_Away__1', 'http://dbpedia.org/resource/Interview_with_the_Vampire_(film)', 'http://dbpedia.org/resource/Jack_Reacher_(film)', 'http://dbpedia.org/resource/Jack_Reacher:_Never_Go_Back', 'http://dbpedia.org/resource/Jerry_Maguire__Jerry_Maguire__1', 'http://dbpedia.org/resource/Knight_and_Day__Knight_and_Day__1', 'http://dbpedia.org/resource/Legend_(1985_film)', 'http://dbpedia.org/resource/Lions_for_Lambs', "http://dbpedia.org/resource/Losin'_It", 'http://dbpedia.org/resource/Magnolia_(film)__Magnolia__1', 'http://dbpedia.org/resource/Minority_Report_(film)', 'http://dbpedia.org/resource/Mission:_Impossible_–_Dead_Reckoning_Part_One', 'http://dbpedia.org/resource/Mission:_Impossible_–_Dead_Reckoning_Part_Two', 'http://dbpedia.org/resource/Mission:_Impossible_–_Fallout', 'http://dbpedia.org/resource/Mission:_Impossible_–_Ghost_Protocol', 'http://dbpedia.org/resource/Mission:_Impossible_–_Rogue_Nation', 'http://dbpedia.org/resource/Mission:_Impossible_(film)', 'http://dbpedia.org/resource/Mission:_Impossible_2', 'http://dbpedia.org/resource/Mission:_Impossible_III', 'http://dbpedia.org/resource/Oblivion_(2013_film)', 'http://dbpedia.org/resource/Rain_Man', 'http://dbpedia.org/resource/Risky_Business', 'http://dbpedia.org/resource/Rock_of_Ages_(2012_film)', 'http://dbpedia.org/resource/Taps_(film)', 'http://dbpedia.org/resource/The_Color_of_Money', 'http://dbpedia.org/resource/The_Firm_(1993_film)', 'http://dbpedia.org/resource/The_Last_Samurai', 'http://dbpedia.org/resource/The_Mummy_(2017_film)', 'http://dbpedia.org/resource/The_Outsiders_(film)', 'http://dbpedia.org/resource/Top_Gun:_Maverick', 'http://dbpedia.org/resource/Top_Gun', 'http://dbpedia.org/resource/Valkyrie_(film)', 'http://dbpedia.org/resource/Vanilla_Sky', 'http://dbpedia.org/resource/War_of_the_Worlds_(2005_film)']</t>
         </is>
       </c>
       <c r="D14" t="b">
@@ -718,17 +718,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Which river does the Brooklyn Bridge cross?</t>
+          <t>Where was JFK assassinated?</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/East_River']</t>
+          <t>['http://dbpedia.org/resource/Dallas']</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/East_River']</t>
+          <t>['http://dbpedia.org/resource/Dallas']</t>
         </is>
       </c>
       <c r="D15" t="b">
@@ -738,17 +738,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>What was the last movie with Alec Guinness?</t>
+          <t>Which river does the Brooklyn Bridge cross?</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Star_Wars_original_trilogy']</t>
+          <t>['http://dbpedia.org/resource/East_River']</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Star_Wars_original_trilogy']</t>
+          <t>['http://dbpedia.org/resource/East_River']</t>
         </is>
       </c>
       <c r="D16" t="b">
@@ -758,17 +758,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>What is the population of Cairo?</t>
+          <t>What was the last movie with Alec Guinness?</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>['10100166']</t>
+          <t>['http://dbpedia.org/resource/Star_Wars_original_trilogy']</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['10100166']</t>
+          <t>['http://dbpedia.org/resource/Star_Wars_original_trilogy']</t>
         </is>
       </c>
       <c r="D17" t="b">
@@ -798,17 +798,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>In which country is Mecca located?</t>
+          <t>What kind of music did Lou Reed play?</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Saudi_Arabia']</t>
+          <t>['http://dbpedia.org/resource/Art_rock', 'http://dbpedia.org/resource/Experimental_music', 'http://dbpedia.org/resource/Glam_rock', 'http://dbpedia.org/resource/Noise_rock', 'http://dbpedia.org/resource/Proto-punk', 'http://dbpedia.org/resource/Rock_music']</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Saudi_Arabia']</t>
+          <t>['http://dbpedia.org/resource/Art_rock', 'http://dbpedia.org/resource/Experimental_music', 'http://dbpedia.org/resource/Glam_rock', 'http://dbpedia.org/resource/Noise_rock', 'http://dbpedia.org/resource/Proto-punk', 'http://dbpedia.org/resource/Rock_music']</t>
         </is>
       </c>
       <c r="D19" t="b">
@@ -818,17 +818,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Which holidays are celebrated around the world?</t>
+          <t>Where did Abraham Lincoln die?</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/140th_Anniversary_Celebration_of_the_Emancipation_Proclamation', 'http://dbpedia.org/resource/19_Kislev', "http://dbpedia.org/resource/21_July_Martyr's_Day_Rally", 'http://dbpedia.org/resource/3_May_Constitution_Day', 'http://dbpedia.org/resource/420_(cannabis_culture)', 'http://dbpedia.org/resource/75th_Anniversary_of_Indian_Independence', 'http://dbpedia.org/resource/Aadi_Perukku', 'http://dbpedia.org/resource/Abaca_Festival', 'http://dbpedia.org/resource/Aberri_Eguna', 'http://dbpedia.org/resource/Absentee_funeral_prayer_(Islam)', 'http://dbpedia.org/resource/Accession_Day_(Jammu_and_Kashmir)', 'http://dbpedia.org/resource/Adae_Festival', 'http://dbpedia.org/resource/Advent_Sunday', 'http://dbpedia.org/resource/Advent', 'http://dbpedia.org/resource/Adwa_Victory_Day', 'http://dbpedia.org/resource/Afghan_Independence_Day', 'http://dbpedia.org/resource/Africa_Day', 'http://dbpedia.org/resource/Afro-Colombian_Day', 'http://dbpedia.org/resource/Agawan_Festival', 'http://dbpedia.org/resource/Agonalia', 'http://dbpedia.org/resource/Agrasen_Jayanti', 'http://dbpedia.org/resource/Ahoi_Ashtami', 'http://dbpedia.org/resource/Air_Force_Day_(Pakistan)', 'http://dbpedia.org/resource/Airborne_March', 'http://dbpedia.org/resource/Akita_Kantō', 'http://dbpedia.org/resource/Akitu', 'http://dbpedia.org/resource/Akshaya_Tritiya', 'http://dbpedia.org/resource/Akwasidae_Festival', 'http://dbpedia.org/resource/Alabama_Day', "http://dbpedia.org/resource/Åland's_Autonomy_Day", 'http://dbpedia.org/resource/Alaska_Day', 'http://dbpedia.org/resource/Aldersgate_Day', 'http://dbpedia.org/resource/Alexandra_Rose_Day', "http://dbpedia.org/resource/All_Saints'_Day", "http://dbpedia.org/resource/All_Souls'_Day", 'http://dbpedia.org/resource/Allantide', 'http://dbpedia.org/resource/Allhallowtide', 'http://dbpedia.org/resource/Amalaka_Ekadashi', 'http://dbpedia.org/resource/Ambedkar_Jayanti', 'http://dbpedia.org/resource/Ambubachi_Mela', 'http://dbpedia.org/resource/Amburbium', 'http://dbpedia.org/resource/America_Recycles_Day', "http://dbpedia.org/resource/American_Business_Women's_Day", 'http://dbpedia.org/resource/American_Family_Day', 'http://dbpedia.org/resource/American_Heart_Month', 'http://dbpedia.org/resource/An_Act_for_the_Admission_of_the_State_of_California', 'http://dbpedia.org/resource/Anant_Chaturdashi', 'http://dbpedia.org/resource/Angam_Day', 'http://dbpedia.org/resource/Angarki_Sankashti_Chaturthi', 'http://dbpedia.org/resource/Anishinaabe_Giizhigad', 'http://dbpedia.org/resource/Anniversary_of_the_Unification_of_Italy', 'http://dbpedia.org/resource/Antarctica_Day', 'http://dbpedia.org/resource/Anti-Bullying_Day', 'http://dbpedia.org/resource/Anti-Fascist_Struggle_Day', 'http://dbpedia.org/resource/Anzac_Day', 'http://dbpedia.org/resource/Apple_Feast_of_the_Saviour', "http://dbpedia.org/resource/April_Fools'_Day", 'http://dbpedia.org/resource/Arattupuzha_Pooram', 'http://dbpedia.org/resource/Aravan_Festival_in_Coimbatore', "http://dbpedia.org/resource/Arba'een", 'http://dbpedia.org/resource/Arbor_Day', 'http://dbpedia.org/resource/Armed_Forces_Day_(Bangladesh)', 'http://dbpedia.org/resource/Armed_Forces_Day_(Poland)', 'http://dbpedia.org/resource/Armed_Forces_Day_(South_Korea)', 'http://dbpedia.org/resource/Armed_Forces_Day_(Tajikistan)', 'http://dbpedia.org/resource/Armed_Forces_Day_(United_Kingdom)', 'http://dbpedia.org/resource/Armenian_Genocide_Remembrance_Day', 'http://dbpedia.org/resource/Armilustrium', 'http://dbpedia.org/resource/Armistice_Day', 'http://dbpedia.org/resource/Army_Day_(Armenia)', 'http://dbpedia.org/resource/Aromanian_National_Day', 'http://dbpedia.org/resource/Artsakh_Revival_Day', 'http://dbpedia.org/resource/Asalha_Puja', 'http://dbpedia.org/resource/Ash_Wednesday', 'http://dbpedia.org/resource/Ashadhi_Puja', 'http://dbpedia.org/resource/Ashanti_Yam_Festival', 'http://dbpedia.org/resource/Ashenda', 'http://dbpedia.org/resource/Ashtimki', 'http://dbpedia.org/resource/Ashura', 'http://dbpedia.org/resource/Asian_American_and_Pacific_Islander_Heritage_Month', 'http://dbpedia.org/resource/Ask_a_Stupid_Question_Day', 'http://dbpedia.org/resource/Asr_prayer', 'http://dbpedia.org/resource/Assumption_of_Mary', 'http://dbpedia.org/resource/Astan_Bandar', 'http://dbpedia.org/resource/Asteroid_Day', 'http://dbpedia.org/resource/Astronauts_Day', 'http://dbpedia.org/resource/Ati-Atihan_festival', 'http://dbpedia.org/resource/Atla_Tadde', 'http://dbpedia.org/resource/Attukal_Pongala', 'http://dbpedia.org/resource/Auckland_Anniversary_Day', 'http://dbpedia.org/resource/August_Holiday', 'http://dbpedia.org/resource/Australia_Day', 'http://dbpedia.org/resource/Australian_Citizenship_Day', 'http://dbpedia.org/resource/Autism_Sunday', 'http://dbpedia.org/resource/Autumnal_Equinox_Day', 'http://dbpedia.org/resource/Awukudae_Festival', 'http://dbpedia.org/resource/Ayudha_Puja', 'http://dbpedia.org/resource/Ayurveda_Day', 'http://dbpedia.org/resource/Azad_Kashmir_Day', 'http://dbpedia.org/resource/Azores_Day', 'http://dbpedia.org/resource/Baba_Marta_Day', 'http://dbpedia.org/resource/Babinden', 'http://dbpedia.org/resource/Baci', 'http://dbpedia.org/resource/Bali_Jatra', 'http://dbpedia.org/resource/Balipratipada', 'http://dbpedia.org/resource/Ballarat_Show', 'http://dbpedia.org/resource/Baltic_Freedom_Day', 'http://dbpedia.org/resource/Baltic_Unity_Day', 'http://dbpedia.org/resource/Bandi_Chhor_Divas', 'http://dbpedia.org/resource/Bandna', 'http://dbpedia.org/resource/Banned_Books_Week', 'http://dbpedia.org/resource/Barack_Obama_Day', 'http://dbpedia.org/resource/Basant_(festival)', 'http://dbpedia.org/resource/Bastille_Day_military_parade', 'http://dbpedia.org/resource/Bastille_Day', 'http://dbpedia.org/resource/Batakari_Day', 'http://dbpedia.org/resource/Bathukamma', 'http://dbpedia.org/resource/Batik_Day', 'http://dbpedia.org/resource/Battle_of_Saragarhi__Day__1', 'http://dbpedia.org/resource/Bauernfest', 'http://dbpedia.org/resource/Belgian_National_Day', 'http://dbpedia.org/resource/Beltane', 'http://dbpedia.org/resource/Ben-Gurion_Day', 'http://dbpedia.org/resource/Beñesmen', 'http://dbpedia.org/resource/Bengali_Genocide_Remembrance_Day', 'http://dbpedia.org/resource/Bennington_Battle_Day', 'http://dbpedia.org/resource/Berchtoldstag', 'http://dbpedia.org/resource/Bhai_Dooj', 'http://dbpedia.org/resource/Bhairava_Ashtami', 'http://dbpedia.org/resource/Bhimana_Amavasya', 'http://dbpedia.org/resource/Bhogi', 'http://dbpedia.org/resource/Bhumchu', 'http://dbpedia.org/resource/Bhume_Naach', 'http://dbpedia.org/resource/Bibi-Ka-Alam', 'http://dbpedia.org/resource/Bihar_Day', 'http://dbpedia.org/resource/Bihu', 'http://dbpedia.org/resource/Binirayan_festival', 'http://dbpedia.org/resource/Birkat_Hachama', "http://dbpedia.org/resource/Birth_of_Baháʼu'lláh", 'http://dbpedia.org/resource/Bisexual_Awareness_Week', 'http://dbpedia.org/resource/Bisu_Parba', 'http://dbpedia.org/resource/Bizhu', 'http://dbpedia.org/resource/Black_Day_(South_Korea)', 'http://dbpedia.org/resource/Black_Friday_(partying)', 'http://dbpedia.org/resource/Black_Friday_(shopping)', 'http://dbpedia.org/resource/Black_History_Month', 'http://dbpedia.org/resource/Black_Ribbon_Day', 'http://dbpedia.org/resource/Blackout_Wednesday', "http://dbpedia.org/resource/Blacks_and_Whites'_Carnival", 'http://dbpedia.org/resource/Blasphemy_Day', 'http://dbpedia.org/resource/Blessed_Rainy_Day', 'http://dbpedia.org/resource/Blue_Beanie_Day', 'http://dbpedia.org/resource/Blue_Christmas_(holiday)', 'http://dbpedia.org/resource/Blue_Mass', 'http://dbpedia.org/resource/Bodhi_Day', 'http://dbpedia.org/resource/Bohag_Bihu', 'http://dbpedia.org/resource/Boishakhi_Mela', 'http://dbpedia.org/resource/Boita_Bandana', 'http://dbpedia.org/resource/Bon_(festival)', 'http://dbpedia.org/resource/Bon_Festival', 'http://dbpedia.org/resource/Bon_Om_Touk', 'http://dbpedia.org/resource/Bonalu', 'http://dbpedia.org/resource/Bonifacio_Day', 'http://dbpedia.org/resource/Book_Lovers_Day', 'http://dbpedia.org/resource/Border_Guards_Day', "http://dbpedia.org/resource/Boss's_Day", 'http://dbpedia.org/resource/Boun_Suang_Huea', 'http://dbpedia.org/resource/Boxing_Day', 'http://dbpedia.org/resource/Boxing_Week', 'http://dbpedia.org/resource/Brain_Tumor_Awareness_Month', "http://dbpedia.org/resource/Buddha's_Birthday", 'http://dbpedia.org/resource/Buhe', 'http://dbpedia.org/resource/Buisu', 'http://dbpedia.org/resource/Bukovina_Day', 'http://dbpedia.org/resource/Bulgarian_Armed_Forces_Day', "http://dbpedia.org/resource/Burmese_Martyrs'_Day", 'http://dbpedia.org/resource/Burns_supper', 'http://dbpedia.org/resource/Buß-_und_Bettag', 'http://dbpedia.org/resource/Busu_Dima', 'http://dbpedia.org/resource/Buwan_ng_Wika', 'http://dbpedia.org/resource/Buy_Nothing_Day', 'http://dbpedia.org/resource/Bwisagu', 'http://dbpedia.org/resource/Cake_and_Cunnilingus_Day', 'http://dbpedia.org/resource/Calan_Gaeaf', 'http://dbpedia.org/resource/Cambodian_New_Year', 'http://dbpedia.org/resource/Canada_Day', 'http://dbpedia.org/resource/Canberra_Day', 'http://dbpedia.org/resource/Cancer_Control_Month', 'http://dbpedia.org/resource/Candlemas', 'http://dbpedia.org/resource/Caribbean-American_Heritage_Month', 'http://dbpedia.org/resource/Caristia', 'http://dbpedia.org/resource/Carl_Garner_Federal_Lands_Cleanup_Day', 'http://dbpedia.org/resource/Carmentalia', 'http://dbpedia.org/resource/Carnaval_de_Ponce', 'http://dbpedia.org/resource/Carnaval_de_Vejigantes', 'http://dbpedia.org/resource/Carnival_in_Belize', 'http://dbpedia.org/resource/Carnival_of_Madeira', 'http://dbpedia.org/resource/Carnival_of_Ovar', 'http://dbpedia.org/resource/Carnival_of_Santa_Cruz_de_Tenerife', 'http://dbpedia.org/resource/Casimir_Pulaski_Day', 'http://dbpedia.org/resource/Cassette_Store_Day', 'http://dbpedia.org/resource/Cassinga_Day', 'http://dbpedia.org/resource/Castile_and_León_Day', 'http://dbpedia.org/resource/Castleton_Garland_Day', 'http://dbpedia.org/resource/Catandungan_Festival', 'http://dbpedia.org/resource/Celebrate_Bisexuality_Day', 'http://dbpedia.org/resource/Ceremony_of_the_Keys_(London)', 'http://dbpedia.org/resource/Cesar_Chavez_Day', 'http://dbpedia.org/resource/Ceuta_Day', 'http://dbpedia.org/resource/Chaand_Raat', "http://dbpedia.org/resource/Chafa'a", 'http://dbpedia.org/resource/Chaharshanbe_Suri', 'http://dbpedia.org/resource/Chaiti_Festival,_Rayagada', 'http://dbpedia.org/resource/Chak_Phra', 'http://dbpedia.org/resource/Chandeshwori_Jatra', 'http://dbpedia.org/resource/Chapchar_Kut', 'http://dbpedia.org/resource/Charak_Puja', 'http://dbpedia.org/resource/Charro_Days', 'http://dbpedia.org/resource/Chasok_Tangnam', 'http://dbpedia.org/resource/Chatar_jatra', 'http://dbpedia.org/resource/Chaturmasya', 'http://dbpedia.org/resource/Cheti_Chand', 'http://dbpedia.org/resource/Chhadakhai', 'http://dbpedia.org/resource/Chhath', 'http://dbpedia.org/resource/Child_Health_Day', 'http://dbpedia.org/resource/Childbirth_Masses', "http://dbpedia.org/resource/Children's_Day_(India)", "http://dbpedia.org/resource/Children's_Day_(Japan)", "http://dbpedia.org/resource/Children's_Day", 'http://dbpedia.org/resource/Chilseok', "http://dbpedia.org/resource/Chinese_New_Year's_Eve", 'http://dbpedia.org/resource/Chinese_New_Year', 'http://dbpedia.org/resource/Chitra_Pournami_(festival)', 'http://dbpedia.org/resource/Chocolate_Day_(Ghana)', 'http://dbpedia.org/resource/Christmas_and_holiday_season', 'http://dbpedia.org/resource/Christmas_Eve', 'http://dbpedia.org/resource/Christmas_in_Ireland', 'http://dbpedia.org/resource/Christmas_in_Romania', 'http://dbpedia.org/resource/Christmas_in_Russia', 'http://dbpedia.org/resource/Christmas_in_Sweden', 'http://dbpedia.org/resource/Christmas_in_Ukraine', 'http://dbpedia.org/resource/Christmas_lights_in_Medellín', 'http://dbpedia.org/resource/Christmas_pageant', 'http://dbpedia.org/resource/Christmas_Sunday', 'http://dbpedia.org/resource/Christmas_traditions', 'http://dbpedia.org/resource/Christmas', 'http://dbpedia.org/resource/Christmastide', 'http://dbpedia.org/resource/Cimarrones_Festival', 'http://dbpedia.org/resource/Cinco_de_Mayo', 'http://dbpedia.org/resource/Cinnamon_Roll_Day', 'http://dbpedia.org/resource/Civic_Holiday', 'http://dbpedia.org/resource/Classics_Day', 'http://dbpedia.org/resource/Coast_Guard_Day', 'http://dbpedia.org/resource/Cold_Food_Festival', 'http://dbpedia.org/resource/Coming_of_Age_Day', 'http://dbpedia.org/resource/Commemoration_Day_of_Fallen_Soldiers', 'http://dbpedia.org/resource/Commemoration_Day', 'http://dbpedia.org/resource/Commemoration_of_Atatürk,_Youth_and_Sports_Day', 'http://dbpedia.org/resource/Commonwealth_Day', 'http://dbpedia.org/resource/Concord_Day', 'http://dbpedia.org/resource/Confederate_Memorial_Day', 'http://dbpedia.org/resource/Constitution_Day_(Denmark)', 'http://dbpedia.org/resource/Constitution_Day_(Ghana)', 'http://dbpedia.org/resource/Constitution_Day_(India)', 'http://dbpedia.org/resource/Constitution_Day_(Kazakhstan)', 'http://dbpedia.org/resource/Constitution_Day_(Norway)', 'http://dbpedia.org/resource/Constitution_Day_(Russia)', 'http://dbpedia.org/resource/Constitution_Day_(South_Korea)', 'http://dbpedia.org/resource/Constitution_Day_(Ukraine)', 'http://dbpedia.org/resource/Constitution_Day_(United_States)', 'http://dbpedia.org/resource/Constitution_Memorial_Day', 'http://dbpedia.org/resource/Constitution_Week', 'http://dbpedia.org/resource/Consualia', 'http://dbpedia.org/resource/Contraband_Days', 'http://dbpedia.org/resource/COPD_Awareness_Month', 'http://dbpedia.org/resource/Coral_Triangle_Day', 'http://dbpedia.org/resource/Cosmonautics_Day', 'http://dbpedia.org/resource/Côte-Rôtie', 'http://dbpedia.org/resource/Courir_de_Mardi_Gras', 'http://dbpedia.org/resource/Cow_Harbor_Day', 'http://dbpedia.org/resource/Crop_Over', "http://dbpedia.org/resource/Cruisin'_Downriver", 'http://dbpedia.org/resource/Cry_of_Dolores', 'http://dbpedia.org/resource/Culture_Day', 'http://dbpedia.org/resource/Čuvari_Hristovog_groba', 'http://dbpedia.org/resource/Cyber_Monday', 'http://dbpedia.org/resource/Daeboreum', 'http://dbpedia.org/resource/Dahi_Handi', 'http://dbpedia.org/resource/Dahi_Jatra', 'http://dbpedia.org/resource/Dalit_History_Month', 'http://dbpedia.org/resource/Dano_(festival)', 'http://dbpedia.org/resource/Dano_(Korean_festival)', 'http://dbpedia.org/resource/Darwin_Day', 'http://dbpedia.org/resource/Dashain', 'http://dbpedia.org/resource/Data_Privacy_Day', 'http://dbpedia.org/resource/Datta_Jayanti', 'http://dbpedia.org/resource/Davao_City_Torotot_Festival', 'http://dbpedia.org/resource/Day_of_Arafah', 'http://dbpedia.org/resource/Day_of_Conception', 'http://dbpedia.org/resource/Day_of_Missile_Forces_and_Artillery', 'http://dbpedia.org/resource/Day_of_National_Dignity', 'http://dbpedia.org/resource/Day_of_Neutrality', 'http://dbpedia.org/resource/Day_of_Prayer', 'http://dbpedia.org/resource/Day_of_Reconciliation', 'http://dbpedia.org/resource/Day_of_Remembrance_for_All_Victims_of_Chemical_Warfare', 'http://dbpedia.org/resource/Day_of_Remembrance_for_Truth_and_Justice', 'http://dbpedia.org/resource/Day_of_Remembrance_of_the_Victims_of_Political_Repressions', 'http://dbpedia.org/resource/Day_of_Republika_Srpska', 'http://dbpedia.org/resource/Day_of_Restoration_of_Independence_(Azerbaijan)', 'http://dbpedia.org/resource/Day_of_Silence', 'http://dbpedia.org/resource/Day_of_Songun', 'http://dbpedia.org/resource/Day_of_the_Armed_Forces_(Kyrgyzstan)', 'http://dbpedia.org/resource/Day_of_the_Armed_Forces_of_Azerbaijan', 'http://dbpedia.org/resource/Day_of_the_Canary_Islands', 'http://dbpedia.org/resource/Day_of_the_Cuban_Armed_Forces', 'http://dbpedia.org/resource/Day_of_the_Dead', 'http://dbpedia.org/resource/Day_of_the_Flemish_Community', 'http://dbpedia.org/resource/Day_of_the_Foundation_of_the_Republic', 'http://dbpedia.org/resource/Day_of_the_founding_of_the_German_Empire', 'http://dbpedia.org/resource/Day_of_the_German-speaking_Community_of_Belgium', 'http://dbpedia.org/resource/Day_of_the_German-speaking_Community', 'http://dbpedia.org/resource/Day_of_the_Little_Candles', 'http://dbpedia.org/resource/Day_of_the_National_Flag_(Ukraine)', 'http://dbpedia.org/resource/Day_of_the_Shining_Star', 'http://dbpedia.org/resource/Day_of_the_Sun', 'http://dbpedia.org/resource/Day_of_the_Unification_of_the_Romanian_Principalities', 'http://dbpedia.org/resource/Day_of_the_Union_of_Bessarabia_with_Romania', 'http://dbpedia.org/resource/Day_of_the_Walloon_Region', 'http://dbpedia.org/resource/Day_of_the_Young_Combatant', 'http://dbpedia.org/resource/Day_of_Ukrainian_Literature_and_Language', 'http://dbpedia.org/resource/Day_of_Valor', 'http://dbpedia.org/resource/Day_of_Victory_in_the_Great_Fatherland_Liberation_War', 'http://dbpedia.org/resource/Daylight_saving_time_in_Canada', 'http://dbpedia.org/resource/Deepothsavam', 'http://dbpedia.org/resource/Defence_Day', 'http://dbpedia.org/resource/Defender_of_the_Fatherland_Day_(Kazakhstan)', 'http://dbpedia.org/resource/Defender_of_the_Fatherland_Day', 'http://dbpedia.org/resource/Defender_of_the_Motherland_Day', 'http://dbpedia.org/resource/Defenders_Day_(Maryland)', 'http://dbpedia.org/resource/Defenders_Day_(Ukraine)', 'http://dbpedia.org/resource/Dehwa_Daimana', 'http://dbpedia.org/resource/Dehwa_Hanina', 'http://dbpedia.org/resource/Dehwa_Rabba', 'http://dbpedia.org/resource/Democracy_and_National_Unity_Day', 'http://dbpedia.org/resource/Dev_Deepawali_(Varanasi)', 'http://dbpedia.org/resource/Dhammachakra_Pravartan_Din', 'http://dbpedia.org/resource/Dhanteras', 'http://dbpedia.org/resource/Dhanu_jatra', 'http://dbpedia.org/resource/Dhodha', 'http://dbpedia.org/resource/Día_de_la_Altagracia', 'http://dbpedia.org/resource/Día_Mundial_de_Ponce', 'http://dbpedia.org/resource/Día_Nacional_de_Galicia', 'http://dbpedia.org/resource/Días_Patrios_(Guatemala)', 'http://dbpedia.org/resource/Dinagyang', 'http://dbpedia.org/resource/Dinamulag_Festival', 'http://dbpedia.org/resource/Disabled_Access_Day', 'http://dbpedia.org/resource/Distaff_Day', 'http://dbpedia.org/resource/Dita_e_Verës', 'http://dbpedia.org/resource/Diwali_(Jainism)', 'http://dbpedia.org/resource/Diwali', 'http://dbpedia.org/resource/DNA_Day', 'http://dbpedia.org/resource/Dobruja_Day', 'http://dbpedia.org/resource/Dongzhi_Festival', 'http://dbpedia.org/resource/Dormition_of_the_Mother_of_God', 'http://dbpedia.org/resource/Dosmoche', 'http://dbpedia.org/resource/Double_Sixth_Festival', 'http://dbpedia.org/resource/Double_Third_Festival', 'http://dbpedia.org/resource/Downfall_of_the_Derg_(holiday)', 'http://dbpedia.org/resource/Dożynki', 'http://dbpedia.org/resource/Dragon_Boat_Festival', 'http://dbpedia.org/resource/Drupka_Teshi', 'http://dbpedia.org/resource/Duanwu_Festival', 'http://dbpedia.org/resource/Duha', 'http://dbpedia.org/resource/Dundee_Fortnight', 'http://dbpedia.org/resource/Durga_Puja', 'http://dbpedia.org/resource/Durgapur_Free_Day', 'http://dbpedia.org/resource/Dziady', 'http://dbpedia.org/resource/Earth_Day', 'http://dbpedia.org/resource/Earth_Hour', 'http://dbpedia.org/resource/Easter', 'http://dbpedia.org/resource/Economics_of_Christmas', 'http://dbpedia.org/resource/Eid_al-Adha', 'http://dbpedia.org/resource/Eid_al-Fitr', 'http://dbpedia.org/resource/Eid_al-Ghadir', 'http://dbpedia.org/resource/Eid_il-Burbara', 'http://dbpedia.org/resource/Eid_prayers', 'http://dbpedia.org/resource/El_Buen_Fin', 'http://dbpedia.org/resource/Ely_Eel_Day', 'http://dbpedia.org/resource/Emergency_Services_Day_(United_Kingdom)', 'http://dbpedia.org/resource/Employee_Appreciation_Day', 'http://dbpedia.org/resource/Enkutatash', 'http://dbpedia.org/resource/Epiphany_(Christian)', 'http://dbpedia.org/resource/Epiphany_(holiday)', 'http://dbpedia.org/resource/Epiphanytide', 'http://dbpedia.org/resource/Errol_Barrow_Day', 'http://dbpedia.org/resource/Erzya_Language_Day', 'http://dbpedia.org/resource/Ethiopian_Christmas', "http://dbpedia.org/resource/Ethiopian_Patriots'_Victory_Day", 'http://dbpedia.org/resource/Ettu_Nombu', 'http://dbpedia.org/resource/Europe_Day', 'http://dbpedia.org/resource/European_Day_of_the_Righteous', 'http://dbpedia.org/resource/Evacuation_Day_(Massachusetts)', 'http://dbpedia.org/resource/Evacuation_Day_(New_York)', 'http://dbpedia.org/resource/Evacuation_Day_(Syria)', 'http://dbpedia.org/resource/Evelio_Javier_Day', 'http://dbpedia.org/resource/Evolution_Day', 'http://dbpedia.org/resource/Execution_of_the_Báb', 'http://dbpedia.org/resource/Fajr_nafl_prayer', 'http://dbpedia.org/resource/Fajr_prayer', 'http://dbpedia.org/resource/Falklands_Day', 'http://dbpedia.org/resource/Family_Day_(Canada)', "http://dbpedia.org/resource/Farmers'_Day", 'http://dbpedia.org/resource/Fast_of_Esther', 'http://dbpedia.org/resource/Fast_of_Gedalia', 'http://dbpedia.org/resource/Fast_of_Nineveh', 'http://dbpedia.org/resource/Fast_of_the_Firstborn', 'http://dbpedia.org/resource/Father–Daughter_Day', "http://dbpedia.org/resource/Father's_Day_(United_States)", "http://dbpedia.org/resource/Father's_Day", 'http://dbpedia.org/resource/Fatimiyya', 'http://dbpedia.org/resource/Feast_of_Ezid', 'http://dbpedia.org/resource/Feast_of_Saint_George_(Palestine)', 'http://dbpedia.org/resource/Feast_of_Saints_Francis_and_Catherine', 'http://dbpedia.org/resource/Feast_of_Saints_Peter_and_Paul', 'http://dbpedia.org/resource/Feast_of_the_Annunciation', 'http://dbpedia.org/resource/Feast_of_the_Ass', 'http://dbpedia.org/resource/Feast_of_the_Assembly', 'http://dbpedia.org/resource/Feast_of_the_Black_Nazarene', 'http://dbpedia.org/resource/Feast_of_the_Great_Shishlam', 'http://dbpedia.org/resource/Feast_of_the_Immaculate_Conception', 'http://dbpedia.org/resource/Federal_Day_of_Thanksgiving,_Repentance_and_Prayer', 'http://dbpedia.org/resource/Federal_holidays_in_the_United_States', 'http://dbpedia.org/resource/Federal_Territory_Day', 'http://dbpedia.org/resource/Feralia', 'http://dbpedia.org/resource/Feria_de_Artesanías_de_Ponce', 'http://dbpedia.org/resource/Feriae_Latinae', 'http://dbpedia.org/resource/Ferragosto', 'http://dbpedia.org/resource/Festa_de_São_João_do_Porto', 'http://dbpedia.org/resource/Festa_della_Repubblica', 'http://dbpedia.org/resource/Festival_de_Bomba_y_Plena_de_San_Antón', 'http://dbpedia.org/resource/Festival_Folclórico_y_Reinado_Nacional_del_Bambuco', 'http://dbpedia.org/resource/Festival_Nacional_Afrocaribeño', 'http://dbpedia.org/resource/Festival_Nacional_de_la_Quenepa', 'http://dbpedia.org/resource/Festival_of_Lights_(Lyon)', 'http://dbpedia.org/resource/Festival_of_Perun', 'http://dbpedia.org/resource/Festival_of_Veles', 'http://dbpedia.org/resource/Festivus', 'http://dbpedia.org/resource/Festum_Ovorum', 'http://dbpedia.org/resource/Fiesta_Nacional_de_la_Danza', 'http://dbpedia.org/resource/Fiestas_de_Santa_Fe', 'http://dbpedia.org/resource/Fiestas_del_Pilar', 'http://dbpedia.org/resource/Fiestas_Patrias_(Chile)', 'http://dbpedia.org/resource/Fiestas_Patrias_(Peru)', 'http://dbpedia.org/resource/Fiestas_patronales_de_Ponce', 'http://dbpedia.org/resource/Fiji_Week', 'http://dbpedia.org/resource/Filipino_American_History_Month', 'http://dbpedia.org/resource/Filipino_Heritage_Month', 'http://dbpedia.org/resource/Filseta', 'http://dbpedia.org/resource/Finnish_Swedish_Heritage_Day', 'http://dbpedia.org/resource/First_day_of_summer_(Iceland)', 'http://dbpedia.org/resource/First_National_Government', 'http://dbpedia.org/resource/Flag_Day_(Albania)', 'http://dbpedia.org/resource/Flag_Day_(Argentina)', 'http://dbpedia.org/resource/Flag_Day_(Australia)', 'http://dbpedia.org/resource/Flag_Day_(United_Arab_Emirates)', 'http://dbpedia.org/resource/Flag_Day_(United_States)', 'http://dbpedia.org/resource/Flag_Day_in_Mexico', 'http://dbpedia.org/resource/Floralia', 'http://dbpedia.org/resource/Fordicidia', 'http://dbpedia.org/resource/Fossil_Fools_Day', 'http://dbpedia.org/resource/Fössta_tossdan_i_mass', "http://dbpedia.org/resource/Founders'_Day_(Ghana)", 'http://dbpedia.org/resource/Frankenstein_Day', 'http://dbpedia.org/resource/Fraternal_Day', 'http://dbpedia.org/resource/Freedom_and_Democracy_Day', 'http://dbpedia.org/resource/Freedom_Day_(Belarus)', 'http://dbpedia.org/resource/Freedom_Day_(Malta)', 'http://dbpedia.org/resource/Freedom_Day_(South_Africa)', 'http://dbpedia.org/resource/French_Community_Holiday', 'http://dbpedia.org/resource/Friendship_Day', 'http://dbpedia.org/resource/Fukagawa_Matsuri', 'http://dbpedia.org/resource/Funeral_prayer_(Islam)', 'http://dbpedia.org/resource/Gaan-Ngai', 'http://dbpedia.org/resource/Gaecheonjeol', 'http://dbpedia.org/resource/Gai_Jatra', 'http://dbpedia.org/resource/Gajan_(festival)', 'http://dbpedia.org/resource/Galdan_Namchot', 'http://dbpedia.org/resource/Galician_Literature_Day', 'http://dbpedia.org/resource/Galungan', 'http://dbpedia.org/resource/Gandhi_Jayanti', 'http://dbpedia.org/resource/Ganesh_Chaturthi', 'http://dbpedia.org/resource/Ganesh_Jayanti', 'http://dbpedia.org/resource/Ganga_Dussehra', 'http://dbpedia.org/resource/Ganga_puja', 'http://dbpedia.org/resource/Gangamma_Jatara', 'http://dbpedia.org/resource/Gangaur', 'http://dbpedia.org/resource/Garifuna_Settlement_Day', 'http://dbpedia.org/resource/Gasparilla_Pirate_Festival', 'http://dbpedia.org/resource/Gaudete_Sunday', 'http://dbpedia.org/resource/Gaura_(festival)', 'http://dbpedia.org/resource/Gawai_Dayak', 'http://dbpedia.org/resource/Geek_Pride_Day', 'http://dbpedia.org/resource/General_Pulaski_Memorial_Day', "http://dbpedia.org/resource/George's_Day_in_Autumn", "http://dbpedia.org/resource/George's_Day_in_Spring", 'http://dbpedia.org/resource/Georgia_Day', 'http://dbpedia.org/resource/German_Unity_Day', 'http://dbpedia.org/resource/German-American_Day', 'http://dbpedia.org/resource/Ghanta_Karna', 'http://dbpedia.org/resource/Ghost_Festival', 'http://dbpedia.org/resource/Giant_Lantern_Festival', 'http://dbpedia.org/resource/Gibraltar_National_Day', 'http://dbpedia.org/resource/Gifaata', 'http://dbpedia.org/resource/Gilgit-Baltistan_Independence_Day', 'http://dbpedia.org/resource/Gion_Matsuri', 'http://dbpedia.org/resource/Giving_Tuesday', 'http://dbpedia.org/resource/GivingTuesday', 'http://dbpedia.org/resource/Glasgow_Fair', 'http://dbpedia.org/resource/Global_Accessibility_Awareness_Day', 'http://dbpedia.org/resource/Global_Day_of_Action_on_Military_Spending', 'http://dbpedia.org/resource/Global_Handwashing_Day', 'http://dbpedia.org/resource/Global_Information_Governance_Day', 'http://dbpedia.org/resource/Global_Money_Week', 'http://dbpedia.org/resource/Global_Running_Day', 'http://dbpedia.org/resource/Global_Wind_Day', 'http://dbpedia.org/resource/Goa_Liberation_Day', 'http://dbpedia.org/resource/Golden_Week_(Japan)', 'http://dbpedia.org/resource/Golu', 'http://dbpedia.org/resource/Good_Friday', 'http://dbpedia.org/resource/Good_Governance_Day', 'http://dbpedia.org/resource/Gopastami', 'http://dbpedia.org/resource/Govatsa_Dwadashi', 'http://dbpedia.org/resource/Gowri_Habba', "http://dbpedia.org/resource/Grand_Duke's_Official_Birthday", "http://dbpedia.org/resource/Grandparents'_Day", 'http://dbpedia.org/resource/Great_Union_Day', 'http://dbpedia.org/resource/Green_Monday', 'http://dbpedia.org/resource/Green_week', 'http://dbpedia.org/resource/Greenery_Day', 'http://dbpedia.org/resource/Groundhog_Day', 'http://dbpedia.org/resource/Guam_Discovery_Day', 'http://dbpedia.org/resource/Guanacaste_Day', 'http://dbpedia.org/resource/Gudi_Padwa', 'http://dbpedia.org/resource/Gunla', 'http://dbpedia.org/resource/Guru_Nanak_Gurpurab', 'http://dbpedia.org/resource/Guru_Purnima', 'http://dbpedia.org/resource/Gustavus_Adolphus_Day', 'http://dbpedia.org/resource/Gustor_Festival', 'http://dbpedia.org/resource/Hadaka_Matsuri', 'http://dbpedia.org/resource/Haitian_Heritage_Month', 'http://dbpedia.org/resource/Hakata_Dontaku', 'http://dbpedia.org/resource/Hakata_Gion_Yamakasa', 'http://dbpedia.org/resource/Halloween', 'http://dbpedia.org/resource/Handsel_Monday', 'http://dbpedia.org/resource/Hangul_Day', 'http://dbpedia.org/resource/Hanukkah', 'http://dbpedia.org/resource/Hanuman_Jayanti', 'http://dbpedia.org/resource/Harela_Mela', 'http://dbpedia.org/resource/Harriet_Tubman_Day', 'http://dbpedia.org/resource/Harvey_Milk_Day', 'http://dbpedia.org/resource/Haya_Day', 'http://dbpedia.org/resource/Heikru_Hidongba', 'http://dbpedia.org/resource/Helen_Keller_Day', 'http://dbpedia.org/resource/Heritage_Day_(South_Africa)', "http://dbpedia.org/resource/Heroes'_Day_(Namibia)", "http://dbpedia.org/resource/Heroes'_Day", 'http://dbpedia.org/resource/Herzl_Day', 'http://dbpedia.org/resource/Higalaay_Festival', 'http://dbpedia.org/resource/Higantes_Festival', 'http://dbpedia.org/resource/Hilaria', 'http://dbpedia.org/resource/Hillbilly_Days', 'http://dbpedia.org/resource/Hiloula_of_Rabbi_Haim_Pinto', 'http://dbpedia.org/resource/Hinamatsuri', 'http://dbpedia.org/resource/Hindi_Day', 'http://dbpedia.org/resource/History_of_lysergic_acid_diethylamide', 'http://dbpedia.org/resource/Hizb_Rateb', 'http://dbpedia.org/resource/Hıdırellez', 'http://dbpedia.org/resource/Hobiyee', 'http://dbpedia.org/resource/Hogmanay', 'http://dbpedia.org/resource/Hola_Mohalla', 'http://dbpedia.org/resource/Holi', 'http://dbpedia.org/resource/Holidays_with_paid_time_off_in_the_United_States', 'http://dbpedia.org/resource/Holika_Dahan', 'http://dbpedia.org/resource/Holy_Saturday', 'http://dbpedia.org/resource/Holy_Week_in_Ruvo_di_Puglia', 'http://dbpedia.org/resource/Hōnensai', 'http://dbpedia.org/resource/Honey_Feast_of_the_Saviour', 'http://dbpedia.org/resource/Hong_Kong_Foundation_Day', 'http://dbpedia.org/resource/Hong_Kong_Special_Administrative_Region_Establishment_Day', 'http://dbpedia.org/resource/Honor_America_Days', 'http://dbpedia.org/resource/Hop-tu-Naa', 'http://dbpedia.org/resource/Hosay', 'http://dbpedia.org/resource/Human_Rights_Day', 'http://dbpedia.org/resource/HumanLight', "http://dbpedia.org/resource/Hùng_Kings'_Festival", 'http://dbpedia.org/resource/Hyderabad-Karnataka_Liberation_Day', 'http://dbpedia.org/resource/Icelandic_National_Day', 'http://dbpedia.org/resource/Imbolc', 'http://dbpedia.org/resource/Imoinu_Iratpa', 'http://dbpedia.org/resource/In_town,_without_my_car!', 'http://dbpedia.org/resource/Independence_and_Unity_Day_(Slovenia)', 'http://dbpedia.org/resource/Independence_Day_(Abkhazia)', 'http://dbpedia.org/resource/Independence_Day_(Algeria)', 'http://dbpedia.org/resource/Independence_Day_(Armenia)', 'http://dbpedia.org/resource/Independence_Day_(Bahrain)', 'http://dbpedia.org/resource/Independence_Day_(Bangladesh)', 'http://dbpedia.org/resource/Independence_Day_(Belarus)', 'http://dbpedia.org/resource/Independence_Day_(Bosnia_and_Herzegovina)', 'http://dbpedia.org/resource/Independence_Day_(Botswana)', 'http://dbpedia.org/resource/Independence_Day_(Brazil)', 'http://dbpedia.org/resource/Independence_Day_(Croatia)', 'http://dbpedia.org/resource/Independence_Day_(Cyprus)', 'http://dbpedia.org/resource/Independence_Day_(Djibouti)', 'http://dbpedia.org/resource/Independence_Day_(Eritrea)', 'http://dbpedia.org/resource/Independence_Day_(Estonia)', 'http://dbpedia.org/resource/Independence_Day_(Finland)', 'http://dbpedia.org/resource/Independence_Day_(Georgia)', 'http://dbpedia.org/resource/Independence_Day_(Ghana)', 'http://dbpedia.org/resource/Independence_Day_(Grenada)', 'http://dbpedia.org/resource/Independence_Day_(Hawaii)', 'http://dbpedia.org/resource/Independence_Day_(India)', 'http://dbpedia.org/resource/Independence_Day_(Indonesia)', 'http://dbpedia.org/resource/Independence_Day_(Jamaica)', 'http://dbpedia.org/resource/Independence_Day_(Jordan)', 'http://dbpedia.org/resource/Independence_Day_(Kazakhstan)', 'http://dbpedia.org/resource/Independence_Day_(Kyrgyzstan)', 'http://dbpedia.org/resource/Independence_Day_(Malaysia)', 'http://dbpedia.org/resource/Independence_Day_(Malta)', 'http://dbpedia.org/resource/Independence_Day_(Myanmar)', 'http://dbpedia.org/resource/Independence_Day_(Niger)', 'http://dbpedia.org/resource/Independence_Day_(North_Macedonia)', 'http://dbpedia.org/resource/Independence_Day_(Pakistan)', 'http://dbpedia.org/resource/Independence_Day_(Philippines)', 'http://dbpedia.org/resource/Independence_Day_(Somalia)', 'http://dbpedia.org/resource/Independence_Day_(Somaliland)', 'http://dbpedia.org/resource/Independence_Day_(South_Ossetia)', 'http://dbpedia.org/resource/Independence_Day_(Sri_Lanka)', 'http://dbpedia.org/resource/Independence_Day_(State_of_Somaliland)', 'http://dbpedia.org/resource/Independence_Day_(Tajikistan)', 'http://dbpedia.org/resource/Independence_Day_(Turkmenistan)', 'http://dbpedia.org/resource/Independence_Day_(Uganda)', 'http://dbpedia.org/resource/Independence_Day_(United_States)', 'http://dbpedia.org/resource/Independence_Day_(Uzbekistan)', 'http://dbpedia.org/resource/Independence_Day_of_Cambodia', 'http://dbpedia.or</t>
+          <t>['http://dbpedia.org/resource/Washington,_D.C.']</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/140th_Anniversary_Celebration_of_the_Emancipation_Proclamation', 'http://dbpedia.org/resource/19_Kislev', "http://dbpedia.org/resource/21_July_Martyr's_Day_Rally", 'http://dbpedia.org/resource/3_May_Constitution_Day', 'http://dbpedia.org/resource/420_(cannabis_culture)', 'http://dbpedia.org/resource/75th_Anniversary_of_Indian_Independence', 'http://dbpedia.org/resource/Aadi_Perukku', 'http://dbpedia.org/resource/Abaca_Festival', 'http://dbpedia.org/resource/Aberri_Eguna', 'http://dbpedia.org/resource/Absentee_funeral_prayer_(Islam)', 'http://dbpedia.org/resource/Accession_Day_(Jammu_and_Kashmir)', 'http://dbpedia.org/resource/Adae_Festival', 'http://dbpedia.org/resource/Advent_Sunday', 'http://dbpedia.org/resource/Advent', 'http://dbpedia.org/resource/Adwa_Victory_Day', 'http://dbpedia.org/resource/Afghan_Independence_Day', 'http://dbpedia.org/resource/Africa_Day', 'http://dbpedia.org/resource/Afro-Colombian_Day', 'http://dbpedia.org/resource/Agawan_Festival', 'http://dbpedia.org/resource/Agonalia', 'http://dbpedia.org/resource/Agrasen_Jayanti', 'http://dbpedia.org/resource/Ahoi_Ashtami', 'http://dbpedia.org/resource/Air_Force_Day_(Pakistan)', 'http://dbpedia.org/resource/Airborne_March', 'http://dbpedia.org/resource/Akita_Kantō', 'http://dbpedia.org/resource/Akitu', 'http://dbpedia.org/resource/Akshaya_Tritiya', 'http://dbpedia.org/resource/Akwasidae_Festival', 'http://dbpedia.org/resource/Alabama_Day', "http://dbpedia.org/resource/Åland's_Autonomy_Day", 'http://dbpedia.org/resource/Alaska_Day', 'http://dbpedia.org/resource/Aldersgate_Day', 'http://dbpedia.org/resource/Alexandra_Rose_Day', "http://dbpedia.org/resource/All_Saints'_Day", "http://dbpedia.org/resource/All_Souls'_Day", 'http://dbpedia.org/resource/Allantide', 'http://dbpedia.org/resource/Allhallowtide', 'http://dbpedia.org/resource/Amalaka_Ekadashi', 'http://dbpedia.org/resource/Ambedkar_Jayanti', 'http://dbpedia.org/resource/Ambubachi_Mela', 'http://dbpedia.org/resource/Amburbium', 'http://dbpedia.org/resource/America_Recycles_Day', "http://dbpedia.org/resource/American_Business_Women's_Day", 'http://dbpedia.org/resource/American_Family_Day', 'http://dbpedia.org/resource/American_Heart_Month', 'http://dbpedia.org/resource/An_Act_for_the_Admission_of_the_State_of_California', 'http://dbpedia.org/resource/Anant_Chaturdashi', 'http://dbpedia.org/resource/Angam_Day', 'http://dbpedia.org/resource/Angarki_Sankashti_Chaturthi', 'http://dbpedia.org/resource/Anishinaabe_Giizhigad', 'http://dbpedia.org/resource/Anniversary_of_the_Unification_of_Italy', 'http://dbpedia.org/resource/Antarctica_Day', 'http://dbpedia.org/resource/Anti-Bullying_Day', 'http://dbpedia.org/resource/Anti-Fascist_Struggle_Day', 'http://dbpedia.org/resource/Anzac_Day', 'http://dbpedia.org/resource/Apple_Feast_of_the_Saviour', "http://dbpedia.org/resource/April_Fools'_Day", 'http://dbpedia.org/resource/Arattupuzha_Pooram', 'http://dbpedia.org/resource/Aravan_Festival_in_Coimbatore', "http://dbpedia.org/resource/Arba'een", 'http://dbpedia.org/resource/Arbor_Day', 'http://dbpedia.org/resource/Armed_Forces_Day_(Bangladesh)', 'http://dbpedia.org/resource/Armed_Forces_Day_(Poland)', 'http://dbpedia.org/resource/Armed_Forces_Day_(South_Korea)', 'http://dbpedia.org/resource/Armed_Forces_Day_(Tajikistan)', 'http://dbpedia.org/resource/Armed_Forces_Day_(United_Kingdom)', 'http://dbpedia.org/resource/Armenian_Genocide_Remembrance_Day', 'http://dbpedia.org/resource/Armilustrium', 'http://dbpedia.org/resource/Armistice_Day', 'http://dbpedia.org/resource/Army_Day_(Armenia)', 'http://dbpedia.org/resource/Aromanian_National_Day', 'http://dbpedia.org/resource/Artsakh_Revival_Day', 'http://dbpedia.org/resource/Asalha_Puja', 'http://dbpedia.org/resource/Ash_Wednesday', 'http://dbpedia.org/resource/Ashadhi_Puja', 'http://dbpedia.org/resource/Ashanti_Yam_Festival', 'http://dbpedia.org/resource/Ashenda', 'http://dbpedia.org/resource/Ashtimki', 'http://dbpedia.org/resource/Ashura', 'http://dbpedia.org/resource/Asian_American_and_Pacific_Islander_Heritage_Month', 'http://dbpedia.org/resource/Ask_a_Stupid_Question_Day', 'http://dbpedia.org/resource/Asr_prayer', 'http://dbpedia.org/resource/Assumption_of_Mary', 'http://dbpedia.org/resource/Astan_Bandar', 'http://dbpedia.org/resource/Asteroid_Day', 'http://dbpedia.org/resource/Astronauts_Day', 'http://dbpedia.org/resource/Ati-Atihan_festival', 'http://dbpedia.org/resource/Atla_Tadde', 'http://dbpedia.org/resource/Attukal_Pongala', 'http://dbpedia.org/resource/Auckland_Anniversary_Day', 'http://dbpedia.org/resource/August_Holiday', 'http://dbpedia.org/resource/Australia_Day', 'http://dbpedia.org/resource/Australian_Citizenship_Day', 'http://dbpedia.org/resource/Autism_Sunday', 'http://dbpedia.org/resource/Autumnal_Equinox_Day', 'http://dbpedia.org/resource/Awukudae_Festival', 'http://dbpedia.org/resource/Ayudha_Puja', 'http://dbpedia.org/resource/Ayurveda_Day', 'http://dbpedia.org/resource/Azad_Kashmir_Day', 'http://dbpedia.org/resource/Azores_Day', 'http://dbpedia.org/resource/Baba_Marta_Day', 'http://dbpedia.org/resource/Babinden', 'http://dbpedia.org/resource/Baci', 'http://dbpedia.org/resource/Bali_Jatra', 'http://dbpedia.org/resource/Balipratipada', 'http://dbpedia.org/resource/Ballarat_Show', 'http://dbpedia.org/resource/Baltic_Freedom_Day', 'http://dbpedia.org/resource/Baltic_Unity_Day', 'http://dbpedia.org/resource/Bandi_Chhor_Divas', 'http://dbpedia.org/resource/Bandna', 'http://dbpedia.org/resource/Banned_Books_Week', 'http://dbpedia.org/resource/Barack_Obama_Day', 'http://dbpedia.org/resource/Basant_(festival)', 'http://dbpedia.org/resource/Bastille_Day_military_parade', 'http://dbpedia.org/resource/Bastille_Day', 'http://dbpedia.org/resource/Batakari_Day', 'http://dbpedia.org/resource/Bathukamma', 'http://dbpedia.org/resource/Batik_Day', 'http://dbpedia.org/resource/Battle_of_Saragarhi__Day__1', 'http://dbpedia.org/resource/Bauernfest', 'http://dbpedia.org/resource/Belgian_National_Day', 'http://dbpedia.org/resource/Beltane', 'http://dbpedia.org/resource/Ben-Gurion_Day', 'http://dbpedia.org/resource/Beñesmen', 'http://dbpedia.org/resource/Bengali_Genocide_Remembrance_Day', 'http://dbpedia.org/resource/Bennington_Battle_Day', 'http://dbpedia.org/resource/Berchtoldstag', 'http://dbpedia.org/resource/Bhai_Dooj', 'http://dbpedia.org/resource/Bhairava_Ashtami', 'http://dbpedia.org/resource/Bhimana_Amavasya', 'http://dbpedia.org/resource/Bhogi', 'http://dbpedia.org/resource/Bhumchu', 'http://dbpedia.org/resource/Bhume_Naach', 'http://dbpedia.org/resource/Bibi-Ka-Alam', 'http://dbpedia.org/resource/Bihar_Day', 'http://dbpedia.org/resource/Bihu', 'http://dbpedia.org/resource/Binirayan_festival', 'http://dbpedia.org/resource/Birkat_Hachama', "http://dbpedia.org/resource/Birth_of_Baháʼu'lláh", 'http://dbpedia.org/resource/Bisexual_Awareness_Week', 'http://dbpedia.org/resource/Bisu_Parba', 'http://dbpedia.org/resource/Bizhu', 'http://dbpedia.org/resource/Black_Day_(South_Korea)', 'http://dbpedia.org/resource/Black_Friday_(partying)', 'http://dbpedia.org/resource/Black_Friday_(shopping)', 'http://dbpedia.org/resource/Black_History_Month', 'http://dbpedia.org/resource/Black_Ribbon_Day', 'http://dbpedia.org/resource/Blackout_Wednesday', "http://dbpedia.org/resource/Blacks_and_Whites'_Carnival", 'http://dbpedia.org/resource/Blasphemy_Day', 'http://dbpedia.org/resource/Blessed_Rainy_Day', 'http://dbpedia.org/resource/Blue_Beanie_Day', 'http://dbpedia.org/resource/Blue_Christmas_(holiday)', 'http://dbpedia.org/resource/Blue_Mass', 'http://dbpedia.org/resource/Bodhi_Day', 'http://dbpedia.org/resource/Bohag_Bihu', 'http://dbpedia.org/resource/Boishakhi_Mela', 'http://dbpedia.org/resource/Boita_Bandana', 'http://dbpedia.org/resource/Bon_(festival)', 'http://dbpedia.org/resource/Bon_Festival', 'http://dbpedia.org/resource/Bon_Om_Touk', 'http://dbpedia.org/resource/Bonalu', 'http://dbpedia.org/resource/Bonifacio_Day', 'http://dbpedia.org/resource/Book_Lovers_Day', 'http://dbpedia.org/resource/Border_Guards_Day', "http://dbpedia.org/resource/Boss's_Day", 'http://dbpedia.org/resource/Boun_Suang_Huea', 'http://dbpedia.org/resource/Boxing_Day', 'http://dbpedia.org/resource/Boxing_Week', 'http://dbpedia.org/resource/Brain_Tumor_Awareness_Month', "http://dbpedia.org/resource/Buddha's_Birthday", 'http://dbpedia.org/resource/Buhe', 'http://dbpedia.org/resource/Buisu', 'http://dbpedia.org/resource/Bukovina_Day', 'http://dbpedia.org/resource/Bulgarian_Armed_Forces_Day', "http://dbpedia.org/resource/Burmese_Martyrs'_Day", 'http://dbpedia.org/resource/Burns_supper', 'http://dbpedia.org/resource/Buß-_und_Bettag', 'http://dbpedia.org/resource/Busu_Dima', 'http://dbpedia.org/resource/Buwan_ng_Wika', 'http://dbpedia.org/resource/Buy_Nothing_Day', 'http://dbpedia.org/resource/Bwisagu', 'http://dbpedia.org/resource/Cake_and_Cunnilingus_Day', 'http://dbpedia.org/resource/Calan_Gaeaf', 'http://dbpedia.org/resource/Cambodian_New_Year', 'http://dbpedia.org/resource/Canada_Day', 'http://dbpedia.org/resource/Canberra_Day', 'http://dbpedia.org/resource/Cancer_Control_Month', 'http://dbpedia.org/resource/Candlemas', 'http://dbpedia.org/resource/Caribbean-American_Heritage_Month', 'http://dbpedia.org/resource/Caristia', 'http://dbpedia.org/resource/Carl_Garner_Federal_Lands_Cleanup_Day', 'http://dbpedia.org/resource/Carmentalia', 'http://dbpedia.org/resource/Carnaval_de_Ponce', 'http://dbpedia.org/resource/Carnaval_de_Vejigantes', 'http://dbpedia.org/resource/Carnival_in_Belize', 'http://dbpedia.org/resource/Carnival_of_Madeira', 'http://dbpedia.org/resource/Carnival_of_Ovar', 'http://dbpedia.org/resource/Carnival_of_Santa_Cruz_de_Tenerife', 'http://dbpedia.org/resource/Casimir_Pulaski_Day', 'http://dbpedia.org/resource/Cassette_Store_Day', 'http://dbpedia.org/resource/Cassinga_Day', 'http://dbpedia.org/resource/Castile_and_León_Day', 'http://dbpedia.org/resource/Castleton_Garland_Day', 'http://dbpedia.org/resource/Catandungan_Festival', 'http://dbpedia.org/resource/Celebrate_Bisexuality_Day', 'http://dbpedia.org/resource/Ceremony_of_the_Keys_(London)', 'http://dbpedia.org/resource/Cesar_Chavez_Day', 'http://dbpedia.org/resource/Ceuta_Day', 'http://dbpedia.org/resource/Chaand_Raat', "http://dbpedia.org/resource/Chafa'a", 'http://dbpedia.org/resource/Chaharshanbe_Suri', 'http://dbpedia.org/resource/Chaiti_Festival,_Rayagada', 'http://dbpedia.org/resource/Chak_Phra', 'http://dbpedia.org/resource/Chandeshwori_Jatra', 'http://dbpedia.org/resource/Chapchar_Kut', 'http://dbpedia.org/resource/Charak_Puja', 'http://dbpedia.org/resource/Charro_Days', 'http://dbpedia.org/resource/Chasok_Tangnam', 'http://dbpedia.org/resource/Chatar_jatra', 'http://dbpedia.org/resource/Chaturmasya', 'http://dbpedia.org/resource/Cheti_Chand', 'http://dbpedia.org/resource/Chhadakhai', 'http://dbpedia.org/resource/Chhath', 'http://dbpedia.org/resource/Child_Health_Day', 'http://dbpedia.org/resource/Childbirth_Masses', "http://dbpedia.org/resource/Children's_Day_(India)", "http://dbpedia.org/resource/Children's_Day_(Japan)", "http://dbpedia.org/resource/Children's_Day", 'http://dbpedia.org/resource/Chilseok', "http://dbpedia.org/resource/Chinese_New_Year's_Eve", 'http://dbpedia.org/resource/Chinese_New_Year', 'http://dbpedia.org/resource/Chitra_Pournami_(festival)', 'http://dbpedia.org/resource/Chocolate_Day_(Ghana)', 'http://dbpedia.org/resource/Christmas_and_holiday_season', 'http://dbpedia.org/resource/Christmas_Eve', 'http://dbpedia.org/resource/Christmas_in_Ireland', 'http://dbpedia.org/resource/Christmas_in_Romania', 'http://dbpedia.org/resource/Christmas_in_Russia', 'http://dbpedia.org/resource/Christmas_in_Sweden', 'http://dbpedia.org/resource/Christmas_in_Ukraine', 'http://dbpedia.org/resource/Christmas_lights_in_Medellín', 'http://dbpedia.org/resource/Christmas_pageant', 'http://dbpedia.org/resource/Christmas_Sunday', 'http://dbpedia.org/resource/Christmas_traditions', 'http://dbpedia.org/resource/Christmas', 'http://dbpedia.org/resource/Christmastide', 'http://dbpedia.org/resource/Cimarrones_Festival', 'http://dbpedia.org/resource/Cinco_de_Mayo', 'http://dbpedia.org/resource/Cinnamon_Roll_Day', 'http://dbpedia.org/resource/Civic_Holiday', 'http://dbpedia.org/resource/Classics_Day', 'http://dbpedia.org/resource/Coast_Guard_Day', 'http://dbpedia.org/resource/Cold_Food_Festival', 'http://dbpedia.org/resource/Coming_of_Age_Day', 'http://dbpedia.org/resource/Commemoration_Day_of_Fallen_Soldiers', 'http://dbpedia.org/resource/Commemoration_Day', 'http://dbpedia.org/resource/Commemoration_of_Atatürk,_Youth_and_Sports_Day', 'http://dbpedia.org/resource/Commonwealth_Day', 'http://dbpedia.org/resource/Concord_Day', 'http://dbpedia.org/resource/Confederate_Memorial_Day', 'http://dbpedia.org/resource/Constitution_Day_(Denmark)', 'http://dbpedia.org/resource/Constitution_Day_(Ghana)', 'http://dbpedia.org/resource/Constitution_Day_(India)', 'http://dbpedia.org/resource/Constitution_Day_(Kazakhstan)', 'http://dbpedia.org/resource/Constitution_Day_(Norway)', 'http://dbpedia.org/resource/Constitution_Day_(Russia)', 'http://dbpedia.org/resource/Constitution_Day_(South_Korea)', 'http://dbpedia.org/resource/Constitution_Day_(Ukraine)', 'http://dbpedia.org/resource/Constitution_Day_(United_States)', 'http://dbpedia.org/resource/Constitution_Memorial_Day', 'http://dbpedia.org/resource/Constitution_Week', 'http://dbpedia.org/resource/Consualia', 'http://dbpedia.org/resource/Contraband_Days', 'http://dbpedia.org/resource/COPD_Awareness_Month', 'http://dbpedia.org/resource/Coral_Triangle_Day', 'http://dbpedia.org/resource/Cosmonautics_Day', 'http://dbpedia.org/resource/Côte-Rôtie', 'http://dbpedia.org/resource/Courir_de_Mardi_Gras', 'http://dbpedia.org/resource/Cow_Harbor_Day', 'http://dbpedia.org/resource/Crop_Over', "http://dbpedia.org/resource/Cruisin'_Downriver", 'http://dbpedia.org/resource/Cry_of_Dolores', 'http://dbpedia.org/resource/Culture_Day', 'http://dbpedia.org/resource/Čuvari_Hristovog_groba', 'http://dbpedia.org/resource/Cyber_Monday', 'http://dbpedia.org/resource/Daeboreum', 'http://dbpedia.org/resource/Dahi_Handi', 'http://dbpedia.org/resource/Dahi_Jatra', 'http://dbpedia.org/resource/Dalit_History_Month', 'http://dbpedia.org/resource/Dano_(festival)', 'http://dbpedia.org/resource/Dano_(Korean_festival)', 'http://dbpedia.org/resource/Darwin_Day', 'http://dbpedia.org/resource/Dashain', 'http://dbpedia.org/resource/Data_Privacy_Day', 'http://dbpedia.org/resource/Datta_Jayanti', 'http://dbpedia.org/resource/Davao_City_Torotot_Festival', 'http://dbpedia.org/resource/Day_of_Arafah', 'http://dbpedia.org/resource/Day_of_Conception', 'http://dbpedia.org/resource/Day_of_Missile_Forces_and_Artillery', 'http://dbpedia.org/resource/Day_of_National_Dignity', 'http://dbpedia.org/resource/Day_of_Neutrality', 'http://dbpedia.org/resource/Day_of_Prayer', 'http://dbpedia.org/resource/Day_of_Reconciliation', 'http://dbpedia.org/resource/Day_of_Remembrance_for_All_Victims_of_Chemical_Warfare', 'http://dbpedia.org/resource/Day_of_Remembrance_for_Truth_and_Justice', 'http://dbpedia.org/resource/Day_of_Remembrance_of_the_Victims_of_Political_Repressions', 'http://dbpedia.org/resource/Day_of_Republika_Srpska', 'http://dbpedia.org/resource/Day_of_Restoration_of_Independence_(Azerbaijan)', 'http://dbpedia.org/resource/Day_of_Silence', 'http://dbpedia.org/resource/Day_of_Songun', 'http://dbpedia.org/resource/Day_of_the_Armed_Forces_(Kyrgyzstan)', 'http://dbpedia.org/resource/Day_of_the_Armed_Forces_of_Azerbaijan', 'http://dbpedia.org/resource/Day_of_the_Canary_Islands', 'http://dbpedia.org/resource/Day_of_the_Cuban_Armed_Forces', 'http://dbpedia.org/resource/Day_of_the_Dead', 'http://dbpedia.org/resource/Day_of_the_Flemish_Community', 'http://dbpedia.org/resource/Day_of_the_Foundation_of_the_Republic', 'http://dbpedia.org/resource/Day_of_the_founding_of_the_German_Empire', 'http://dbpedia.org/resource/Day_of_the_German-speaking_Community_of_Belgium', 'http://dbpedia.org/resource/Day_of_the_German-speaking_Community', 'http://dbpedia.org/resource/Day_of_the_Little_Candles', 'http://dbpedia.org/resource/Day_of_the_National_Flag_(Ukraine)', 'http://dbpedia.org/resource/Day_of_the_Shining_Star', 'http://dbpedia.org/resource/Day_of_the_Sun', 'http://dbpedia.org/resource/Day_of_the_Unification_of_the_Romanian_Principalities', 'http://dbpedia.org/resource/Day_of_the_Union_of_Bessarabia_with_Romania', 'http://dbpedia.org/resource/Day_of_the_Walloon_Region', 'http://dbpedia.org/resource/Day_of_the_Young_Combatant', 'http://dbpedia.org/resource/Day_of_Ukrainian_Literature_and_Language', 'http://dbpedia.org/resource/Day_of_Valor', 'http://dbpedia.org/resource/Day_of_Victory_in_the_Great_Fatherland_Liberation_War', 'http://dbpedia.org/resource/Daylight_saving_time_in_Canada', 'http://dbpedia.org/resource/Deepothsavam', 'http://dbpedia.org/resource/Defence_Day', 'http://dbpedia.org/resource/Defender_of_the_Fatherland_Day_(Kazakhstan)', 'http://dbpedia.org/resource/Defender_of_the_Fatherland_Day', 'http://dbpedia.org/resource/Defender_of_the_Motherland_Day', 'http://dbpedia.org/resource/Defenders_Day_(Maryland)', 'http://dbpedia.org/resource/Defenders_Day_(Ukraine)', 'http://dbpedia.org/resource/Dehwa_Daimana', 'http://dbpedia.org/resource/Dehwa_Hanina', 'http://dbpedia.org/resource/Dehwa_Rabba', 'http://dbpedia.org/resource/Democracy_and_National_Unity_Day', 'http://dbpedia.org/resource/Dev_Deepawali_(Varanasi)', 'http://dbpedia.org/resource/Dhammachakra_Pravartan_Din', 'http://dbpedia.org/resource/Dhanteras', 'http://dbpedia.org/resource/Dhanu_jatra', 'http://dbpedia.org/resource/Dhodha', 'http://dbpedia.org/resource/Día_de_la_Altagracia', 'http://dbpedia.org/resource/Día_Mundial_de_Ponce', 'http://dbpedia.org/resource/Día_Nacional_de_Galicia', 'http://dbpedia.org/resource/Días_Patrios_(Guatemala)', 'http://dbpedia.org/resource/Dinagyang', 'http://dbpedia.org/resource/Dinamulag_Festival', 'http://dbpedia.org/resource/Disabled_Access_Day', 'http://dbpedia.org/resource/Distaff_Day', 'http://dbpedia.org/resource/Dita_e_Verës', 'http://dbpedia.org/resource/Diwali_(Jainism)', 'http://dbpedia.org/resource/Diwali', 'http://dbpedia.org/resource/DNA_Day', 'http://dbpedia.org/resource/Dobruja_Day', 'http://dbpedia.org/resource/Dongzhi_Festival', 'http://dbpedia.org/resource/Dormition_of_the_Mother_of_God', 'http://dbpedia.org/resource/Dosmoche', 'http://dbpedia.org/resource/Double_Sixth_Festival', 'http://dbpedia.org/resource/Double_Third_Festival', 'http://dbpedia.org/resource/Downfall_of_the_Derg_(holiday)', 'http://dbpedia.org/resource/Dożynki', 'http://dbpedia.org/resource/Dragon_Boat_Festival', 'http://dbpedia.org/resource/Drupka_Teshi', 'http://dbpedia.org/resource/Duanwu_Festival', 'http://dbpedia.org/resource/Duha', 'http://dbpedia.org/resource/Dundee_Fortnight', 'http://dbpedia.org/resource/Durga_Puja', 'http://dbpedia.org/resource/Durgapur_Free_Day', 'http://dbpedia.org/resource/Dziady', 'http://dbpedia.org/resource/Earth_Day', 'http://dbpedia.org/resource/Earth_Hour', 'http://dbpedia.org/resource/Easter', 'http://dbpedia.org/resource/Economics_of_Christmas', 'http://dbpedia.org/resource/Eid_al-Adha', 'http://dbpedia.org/resource/Eid_al-Fitr', 'http://dbpedia.org/resource/Eid_al-Ghadir', 'http://dbpedia.org/resource/Eid_il-Burbara', 'http://dbpedia.org/resource/Eid_prayers', 'http://dbpedia.org/resource/El_Buen_Fin', 'http://dbpedia.org/resource/Ely_Eel_Day', 'http://dbpedia.org/resource/Emergency_Services_Day_(United_Kingdom)', 'http://dbpedia.org/resource/Employee_Appreciation_Day', 'http://dbpedia.org/resource/Enkutatash', 'http://dbpedia.org/resource/Epiphany_(Christian)', 'http://dbpedia.org/resource/Epiphany_(holiday)', 'http://dbpedia.org/resource/Epiphanytide', 'http://dbpedia.org/resource/Errol_Barrow_Day', 'http://dbpedia.org/resource/Erzya_Language_Day', 'http://dbpedia.org/resource/Ethiopian_Christmas', "http://dbpedia.org/resource/Ethiopian_Patriots'_Victory_Day", 'http://dbpedia.org/resource/Ettu_Nombu', 'http://dbpedia.org/resource/Europe_Day', 'http://dbpedia.org/resource/European_Day_of_the_Righteous', 'http://dbpedia.org/resource/Evacuation_Day_(Massachusetts)', 'http://dbpedia.org/resource/Evacuation_Day_(New_York)', 'http://dbpedia.org/resource/Evacuation_Day_(Syria)', 'http://dbpedia.org/resource/Evelio_Javier_Day', 'http://dbpedia.org/resource/Evolution_Day', 'http://dbpedia.org/resource/Execution_of_the_Báb', 'http://dbpedia.org/resource/Fajr_nafl_prayer', 'http://dbpedia.org/resource/Fajr_prayer', 'http://dbpedia.org/resource/Falklands_Day', 'http://dbpedia.org/resource/Family_Day_(Canada)', "http://dbpedia.org/resource/Farmers'_Day", 'http://dbpedia.org/resource/Fast_of_Esther', 'http://dbpedia.org/resource/Fast_of_Gedalia', 'http://dbpedia.org/resource/Fast_of_Nineveh', 'http://dbpedia.org/resource/Fast_of_the_Firstborn', 'http://dbpedia.org/resource/Father–Daughter_Day', "http://dbpedia.org/resource/Father's_Day_(United_States)", "http://dbpedia.org/resource/Father's_Day", 'http://dbpedia.org/resource/Fatimiyya', 'http://dbpedia.org/resource/Feast_of_Ezid', 'http://dbpedia.org/resource/Feast_of_Saint_George_(Palestine)', 'http://dbpedia.org/resource/Feast_of_Saints_Francis_and_Catherine', 'http://dbpedia.org/resource/Feast_of_Saints_Peter_and_Paul', 'http://dbpedia.org/resource/Feast_of_the_Annunciation', 'http://dbpedia.org/resource/Feast_of_the_Ass', 'http://dbpedia.org/resource/Feast_of_the_Assembly', 'http://dbpedia.org/resource/Feast_of_the_Black_Nazarene', 'http://dbpedia.org/resource/Feast_of_the_Great_Shishlam', 'http://dbpedia.org/resource/Feast_of_the_Immaculate_Conception', 'http://dbpedia.org/resource/Federal_Day_of_Thanksgiving,_Repentance_and_Prayer', 'http://dbpedia.org/resource/Federal_holidays_in_the_United_States', 'http://dbpedia.org/resource/Federal_Territory_Day', 'http://dbpedia.org/resource/Feralia', 'http://dbpedia.org/resource/Feria_de_Artesanías_de_Ponce', 'http://dbpedia.org/resource/Feriae_Latinae', 'http://dbpedia.org/resource/Ferragosto', 'http://dbpedia.org/resource/Festa_de_São_João_do_Porto', 'http://dbpedia.org/resource/Festa_della_Repubblica', 'http://dbpedia.org/resource/Festival_de_Bomba_y_Plena_de_San_Antón', 'http://dbpedia.org/resource/Festival_Folclórico_y_Reinado_Nacional_del_Bambuco', 'http://dbpedia.org/resource/Festival_Nacional_Afrocaribeño', 'http://dbpedia.org/resource/Festival_Nacional_de_la_Quenepa', 'http://dbpedia.org/resource/Festival_of_Lights_(Lyon)', 'http://dbpedia.org/resource/Festival_of_Perun', 'http://dbpedia.org/resource/Festival_of_Veles', 'http://dbpedia.org/resource/Festivus', 'http://dbpedia.org/resource/Festum_Ovorum', 'http://dbpedia.org/resource/Fiesta_Nacional_de_la_Danza', 'http://dbpedia.org/resource/Fiestas_de_Santa_Fe', 'http://dbpedia.org/resource/Fiestas_del_Pilar', 'http://dbpedia.org/resource/Fiestas_Patrias_(Chile)', 'http://dbpedia.org/resource/Fiestas_Patrias_(Peru)', 'http://dbpedia.org/resource/Fiestas_patronales_de_Ponce', 'http://dbpedia.org/resource/Fiji_Week', 'http://dbpedia.org/resource/Filipino_American_History_Month', 'http://dbpedia.org/resource/Filipino_Heritage_Month', 'http://dbpedia.org/resource/Filseta', 'http://dbpedia.org/resource/Finnish_Swedish_Heritage_Day', 'http://dbpedia.org/resource/First_day_of_summer_(Iceland)', 'http://dbpedia.org/resource/First_National_Government', 'http://dbpedia.org/resource/Flag_Day_(Albania)', 'http://dbpedia.org/resource/Flag_Day_(Argentina)', 'http://dbpedia.org/resource/Flag_Day_(Australia)', 'http://dbpedia.org/resource/Flag_Day_(United_Arab_Emirates)', 'http://dbpedia.org/resource/Flag_Day_(United_States)', 'http://dbpedia.org/resource/Flag_Day_in_Mexico', 'http://dbpedia.org/resource/Floralia', 'http://dbpedia.org/resource/Fordicidia', 'http://dbpedia.org/resource/Fossil_Fools_Day', 'http://dbpedia.org/resource/Fössta_tossdan_i_mass', "http://dbpedia.org/resource/Founders'_Day_(Ghana)", 'http://dbpedia.org/resource/Frankenstein_Day', 'http://dbpedia.org/resource/Fraternal_Day', 'http://dbpedia.org/resource/Freedom_and_Democracy_Day', 'http://dbpedia.org/resource/Freedom_Day_(Belarus)', 'http://dbpedia.org/resource/Freedom_Day_(Malta)', 'http://dbpedia.org/resource/Freedom_Day_(South_Africa)', 'http://dbpedia.org/resource/French_Community_Holiday', 'http://dbpedia.org/resource/Friendship_Day', 'http://dbpedia.org/resource/Fukagawa_Matsuri', 'http://dbpedia.org/resource/Funeral_prayer_(Islam)', 'http://dbpedia.org/resource/Gaan-Ngai', 'http://dbpedia.org/resource/Gaecheonjeol', 'http://dbpedia.org/resource/Gai_Jatra', 'http://dbpedia.org/resource/Gajan_(festival)', 'http://dbpedia.org/resource/Galdan_Namchot', 'http://dbpedia.org/resource/Galician_Literature_Day', 'http://dbpedia.org/resource/Galungan', 'http://dbpedia.org/resource/Gandhi_Jayanti', 'http://dbpedia.org/resource/Ganesh_Chaturthi', 'http://dbpedia.org/resource/Ganesh_Jayanti', 'http://dbpedia.org/resource/Ganga_Dussehra', 'http://dbpedia.org/resource/Ganga_puja', 'http://dbpedia.org/resource/Gangamma_Jatara', 'http://dbpedia.org/resource/Gangaur', 'http://dbpedia.org/resource/Garifuna_Settlement_Day', 'http://dbpedia.org/resource/Gasparilla_Pirate_Festival', 'http://dbpedia.org/resource/Gaudete_Sunday', 'http://dbpedia.org/resource/Gaura_(festival)', 'http://dbpedia.org/resource/Gawai_Dayak', 'http://dbpedia.org/resource/Geek_Pride_Day', 'http://dbpedia.org/resource/General_Pulaski_Memorial_Day', "http://dbpedia.org/resource/George's_Day_in_Autumn", "http://dbpedia.org/resource/George's_Day_in_Spring", 'http://dbpedia.org/resource/Georgia_Day', 'http://dbpedia.org/resource/German_Unity_Day', 'http://dbpedia.org/resource/German-American_Day', 'http://dbpedia.org/resource/Ghanta_Karna', 'http://dbpedia.org/resource/Ghost_Festival', 'http://dbpedia.org/resource/Giant_Lantern_Festival', 'http://dbpedia.org/resource/Gibraltar_National_Day', 'http://dbpedia.org/resource/Gifaata', 'http://dbpedia.org/resource/Gilgit-Baltistan_Independence_Day', 'http://dbpedia.org/resource/Gion_Matsuri', 'http://dbpedia.org/resource/Giving_Tuesday', 'http://dbpedia.org/resource/GivingTuesday', 'http://dbpedia.org/resource/Glasgow_Fair', 'http://dbpedia.org/resource/Global_Accessibility_Awareness_Day', 'http://dbpedia.org/resource/Global_Day_of_Action_on_Military_Spending', 'http://dbpedia.org/resource/Global_Handwashing_Day', 'http://dbpedia.org/resource/Global_Information_Governance_Day', 'http://dbpedia.org/resource/Global_Money_Week', 'http://dbpedia.org/resource/Global_Running_Day', 'http://dbpedia.org/resource/Global_Wind_Day', 'http://dbpedia.org/resource/Goa_Liberation_Day', 'http://dbpedia.org/resource/Golden_Week_(Japan)', 'http://dbpedia.org/resource/Golu', 'http://dbpedia.org/resource/Good_Friday', 'http://dbpedia.org/resource/Good_Governance_Day', 'http://dbpedia.org/resource/Gopastami', 'http://dbpedia.org/resource/Govatsa_Dwadashi', 'http://dbpedia.org/resource/Gowri_Habba', "http://dbpedia.org/resource/Grand_Duke's_Official_Birthday", "http://dbpedia.org/resource/Grandparents'_Day", 'http://dbpedia.org/resource/Great_Union_Day', 'http://dbpedia.org/resource/Green_Monday', 'http://dbpedia.org/resource/Green_week', 'http://dbpedia.org/resource/Greenery_Day', 'http://dbpedia.org/resource/Groundhog_Day', 'http://dbpedia.org/resource/Guam_Discovery_Day', 'http://dbpedia.org/resource/Guanacaste_Day', 'http://dbpedia.org/resource/Gudi_Padwa', 'http://dbpedia.org/resource/Gunla', 'http://dbpedia.org/resource/Guru_Nanak_Gurpurab', 'http://dbpedia.org/resource/Guru_Purnima', 'http://dbpedia.org/resource/Gustavus_Adolphus_Day', 'http://dbpedia.org/resource/Gustor_Festival', 'http://dbpedia.org/resource/Hadaka_Matsuri', 'http://dbpedia.org/resource/Haitian_Heritage_Month', 'http://dbpedia.org/resource/Hakata_Dontaku', 'http://dbpedia.org/resource/Hakata_Gion_Yamakasa', 'http://dbpedia.org/resource/Halloween', 'http://dbpedia.org/resource/Handsel_Monday', 'http://dbpedia.org/resource/Hangul_Day', 'http://dbpedia.org/resource/Hanukkah', 'http://dbpedia.org/resource/Hanuman_Jayanti', 'http://dbpedia.org/resource/Harela_Mela', 'http://dbpedia.org/resource/Harriet_Tubman_Day', 'http://dbpedia.org/resource/Harvey_Milk_Day', 'http://dbpedia.org/resource/Haya_Day', 'http://dbpedia.org/resource/Heikru_Hidongba', 'http://dbpedia.org/resource/Helen_Keller_Day', 'http://dbpedia.org/resource/Heritage_Day_(South_Africa)', "http://dbpedia.org/resource/Heroes'_Day_(Namibia)", "http://dbpedia.org/resource/Heroes'_Day", 'http://dbpedia.org/resource/Herzl_Day', 'http://dbpedia.org/resource/Higalaay_Festival', 'http://dbpedia.org/resource/Higantes_Festival', 'http://dbpedia.org/resource/Hilaria', 'http://dbpedia.org/resource/Hillbilly_Days', 'http://dbpedia.org/resource/Hiloula_of_Rabbi_Haim_Pinto', 'http://dbpedia.org/resource/Hinamatsuri', 'http://dbpedia.org/resource/Hindi_Day', 'http://dbpedia.org/resource/History_of_lysergic_acid_diethylamide', 'http://dbpedia.org/resource/Hizb_Rateb', 'http://dbpedia.org/resource/Hıdırellez', 'http://dbpedia.org/resource/Hobiyee', 'http://dbpedia.org/resource/Hogmanay', 'http://dbpedia.org/resource/Hola_Mohalla', 'http://dbpedia.org/resource/Holi', 'http://dbpedia.org/resource/Holidays_with_paid_time_off_in_the_United_States', 'http://dbpedia.org/resource/Holika_Dahan', 'http://dbpedia.org/resource/Holy_Saturday', 'http://dbpedia.org/resource/Holy_Week_in_Ruvo_di_Puglia', 'http://dbpedia.org/resource/Hōnensai', 'http://dbpedia.org/resource/Honey_Feast_of_the_Saviour', 'http://dbpedia.org/resource/Hong_Kong_Foundation_Day', 'http://dbpedia.org/resource/Hong_Kong_Special_Administrative_Region_Establishment_Day', 'http://dbpedia.org/resource/Honor_America_Days', 'http://dbpedia.org/resource/Hop-tu-Naa', 'http://dbpedia.org/resource/Hosay', 'http://dbpedia.org/resource/Human_Rights_Day', 'http://dbpedia.org/resource/HumanLight', "http://dbpedia.org/resource/Hùng_Kings'_Festival", 'http://dbpedia.org/resource/Hyderabad-Karnataka_Liberation_Day', 'http://dbpedia.org/resource/Icelandic_National_Day', 'http://dbpedia.org/resource/Imbolc', 'http://dbpedia.org/resource/Imoinu_Iratpa', 'http://dbpedia.org/resource/In_town,_without_my_car!', 'http://dbpedia.org/resource/Independence_and_Unity_Day_(Slovenia)', 'http://dbpedia.org/resource/Independence_Day_(Abkhazia)', 'http://dbpedia.org/resource/Independence_Day_(Algeria)', 'http://dbpedia.org/resource/Independence_Day_(Armenia)', 'http://dbpedia.org/resource/Independence_Day_(Bahrain)', 'http://dbpedia.org/resource/Independence_Day_(Bangladesh)', 'http://dbpedia.org/resource/Independence_Day_(Belarus)', 'http://dbpedia.org/resource/Independence_Day_(Bosnia_and_Herzegovina)', 'http://dbpedia.org/resource/Independence_Day_(Botswana)', 'http://dbpedia.org/resource/Independence_Day_(Brazil)', 'http://dbpedia.org/resource/Independence_Day_(Croatia)', 'http://dbpedia.org/resource/Independence_Day_(Cyprus)', 'http://dbpedia.org/resource/Independence_Day_(Djibouti)', 'http://dbpedia.org/resource/Independence_Day_(Eritrea)', 'http://dbpedia.org/resource/Independence_Day_(Estonia)', 'http://dbpedia.org/resource/Independence_Day_(Finland)', 'http://dbpedia.org/resource/Independence_Day_(Georgia)', 'http://dbpedia.org/resource/Independence_Day_(Ghana)', 'http://dbpedia.org/resource/Independence_Day_(Grenada)', 'http://dbpedia.org/resource/Independence_Day_(Hawaii)', 'http://dbpedia.org/resource/Independence_Day_(India)', 'http://dbpedia.org/resource/Independence_Day_(Indonesia)', 'http://dbpedia.org/resource/Independence_Day_(Jamaica)', 'http://dbpedia.org/resource/Independence_Day_(Jordan)', 'http://dbpedia.org/resource/Independence_Day_(Kazakhstan)', 'http://dbpedia.org/resource/Independence_Day_(Kyrgyzstan)', 'http://dbpedia.org/resource/Independence_Day_(Malaysia)', 'http://dbpedia.org/resource/Independence_Day_(Malta)', 'http://dbpedia.org/resource/Independence_Day_(Myanmar)', 'http://dbpedia.org/resource/Independence_Day_(Niger)', 'http://dbpedia.org/resource/Independence_Day_(North_Macedonia)', 'http://dbpedia.org/resource/Independence_Day_(Pakistan)', 'http://dbpedia.org/resource/Independence_Day_(Philippines)', 'http://dbpedia.org/resource/Independence_Day_(Somalia)', 'http://dbpedia.org/resource/Independence_Day_(Somaliland)', 'http://dbpedia.org/resource/Independence_Day_(South_Ossetia)', 'http://dbpedia.org/resource/Independence_Day_(Sri_Lanka)', 'http://dbpedia.org/resource/Independence_Day_(State_of_Somaliland)', 'http://dbpedia.org/resource/Independence_Day_(Tajikistan)', 'http://dbpedia.org/resource/Independence_Day_(Turkmenistan)', 'http://dbpedia.org/resource/Independence_Day_(Uganda)', 'http://dbpedia.org/resource/Independence_Day_(United_States)', 'http://dbpedia.org/resource/Independence_Day_(Uzbekistan)', 'http://dbpedia.org/resource/Independence_Day_of_Cambodia', 'http://dbpedia.or</t>
+          <t>['http://dbpedia.org/resource/Washington,_D.C.']</t>
         </is>
       </c>
       <c r="D20" t="b">
@@ -838,17 +838,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>What kind of music did Lou Reed play?</t>
+          <t>In which country is the Limerick Lake?</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Art_rock', 'http://dbpedia.org/resource/Experimental_music', 'http://dbpedia.org/resource/Glam_rock', 'http://dbpedia.org/resource/Noise_rock', 'http://dbpedia.org/resource/Proto-punk', 'http://dbpedia.org/resource/Rock_music']</t>
+          <t>['http://dbpedia.org/resource/Canada']</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Art_rock', 'http://dbpedia.org/resource/Experimental_music', 'http://dbpedia.org/resource/Glam_rock', 'http://dbpedia.org/resource/Noise_rock', 'http://dbpedia.org/resource/Proto-punk', 'http://dbpedia.org/resource/Rock_music']</t>
+          <t>['http://dbpedia.org/resource/Canada']</t>
         </is>
       </c>
       <c r="D21" t="b">
@@ -858,17 +858,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Give me the birth place of Frank Sinatra.</t>
+          <t>In which countries can you pay using the West African CFA franc?</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Hoboken,_New_Jersey']</t>
+          <t>['http://dbpedia.org/resource/Benin', 'http://dbpedia.org/resource/Burkina_Faso', 'http://dbpedia.org/resource/Colonial_Mauritania', 'http://dbpedia.org/resource/Colony_of_Niger', 'http://dbpedia.org/resource/Economic_Community_of_West_African_States', 'http://dbpedia.org/resource/French_Dahomey', 'http://dbpedia.org/resource/French_Togoland', 'http://dbpedia.org/resource/Guinea-Bissau', 'http://dbpedia.org/resource/History_of_Togo', 'http://dbpedia.org/resource/Ivory_Coast', 'http://dbpedia.org/resource/Mali', 'http://dbpedia.org/resource/Niger', "http://dbpedia.org/resource/People's_Republic_of_Benin", 'http://dbpedia.org/resource/Republic_of_Dahomey', 'http://dbpedia.org/resource/Republic_of_Upper_Volta', 'http://dbpedia.org/resource/Senegal', 'http://dbpedia.org/resource/Senegambia_Confederation', 'http://dbpedia.org/resource/Togo']</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Hoboken,_New_Jersey']</t>
+          <t>['http://dbpedia.org/resource/Benin', 'http://dbpedia.org/resource/Burkina_Faso', 'http://dbpedia.org/resource/Colonial_Mauritania', 'http://dbpedia.org/resource/Colony_of_Niger', 'http://dbpedia.org/resource/Economic_Community_of_West_African_States', 'http://dbpedia.org/resource/French_Dahomey', 'http://dbpedia.org/resource/French_Togoland', 'http://dbpedia.org/resource/Guinea-Bissau', 'http://dbpedia.org/resource/History_of_Togo', 'http://dbpedia.org/resource/Ivory_Coast', 'http://dbpedia.org/resource/Mali', 'http://dbpedia.org/resource/Niger', "http://dbpedia.org/resource/People's_Republic_of_Benin", 'http://dbpedia.org/resource/Republic_of_Dahomey', 'http://dbpedia.org/resource/Republic_of_Upper_Volta', 'http://dbpedia.org/resource/Senegal', 'http://dbpedia.org/resource/Senegambia_Confederation', 'http://dbpedia.org/resource/Togo']</t>
         </is>
       </c>
       <c r="D22" t="b">
@@ -878,17 +878,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Where did Abraham Lincoln die?</t>
+          <t>What is the capital of Canada?</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Washington,_D.C.']</t>
+          <t>['http://dbpedia.org/resource/Ottawa']</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Washington,_D.C.']</t>
+          <t>['http://dbpedia.org/resource/Ottawa']</t>
         </is>
       </c>
       <c r="D23" t="b">
@@ -898,17 +898,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>How tall is Michael Jordan?</t>
+          <t>What is the capital of Cameroon?</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>['1.9812']</t>
+          <t>['http://dbpedia.org/resource/Yaoundé']</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>['1.9812']</t>
+          <t>['http://dbpedia.org/resource/Yaoundé']</t>
         </is>
       </c>
       <c r="D24" t="b">
@@ -918,17 +918,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>In which countries can you pay using the West African CFA franc?</t>
+          <t>Give me all cosmonauts.</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Benin', 'http://dbpedia.org/resource/Burkina_Faso', 'http://dbpedia.org/resource/Colonial_Mauritania', 'http://dbpedia.org/resource/Colony_of_Niger', 'http://dbpedia.org/resource/Economic_Community_of_West_African_States', 'http://dbpedia.org/resource/French_Dahomey', 'http://dbpedia.org/resource/French_Togoland', 'http://dbpedia.org/resource/Guinea-Bissau', 'http://dbpedia.org/resource/History_of_Togo', 'http://dbpedia.org/resource/Ivory_Coast', 'http://dbpedia.org/resource/Mali', 'http://dbpedia.org/resource/Niger', "http://dbpedia.org/resource/People's_Republic_of_Benin", 'http://dbpedia.org/resource/Republic_of_Dahomey', 'http://dbpedia.org/resource/Republic_of_Upper_Volta', 'http://dbpedia.org/resource/Senegal', 'http://dbpedia.org/resource/Senegambia_Confederation', 'http://dbpedia.org/resource/Togo']</t>
+          <t>['http://dbpedia.org/resource/Aleksandr_Aleksandrovich_Volkov', 'http://dbpedia.org/resource/Aleksandr_Ivanchenkov', 'http://dbpedia.org/resource/Aleksandr_Laveykin', 'http://dbpedia.org/resource/Aleksandr_Nikolayevich_Balandin', 'http://dbpedia.org/resource/Aleksandr_Pavlovich_Aleksandrov__Aleksandr_Pavlovich_Aleksandrov__1', 'http://dbpedia.org/resource/Aleksandr_Serebrov', 'http://dbpedia.org/resource/Aleksandr_Viktorenko', 'http://dbpedia.org/resource/Aleksei_Gubarev', 'http://dbpedia.org/resource/Aleksei_Yeliseyev', 'http://dbpedia.org/resource/Anatoly_Berezovoy', 'http://dbpedia.org/resource/Anatoly_Filipchenko', 'http://dbpedia.org/resource/Anatoly_Levchenko__Anatoly_Semyonovich_Levchenko__1', 'http://dbpedia.org/resource/Andriyan_Nikolayev', 'http://dbpedia.org/resource/Boris_Andreyev_(cosmonaut)', 'http://dbpedia.org/resource/Boris_Volynov', 'http://dbpedia.org/resource/Boris_Yegorov', 'http://dbpedia.org/resource/Gennady_Manakov', 'http://dbpedia.org/resource/Gennady_Sarafanov', 'http://dbpedia.org/resource/Gennady_Strekalov', 'http://dbpedia.org/resource/Georgy_Dobrovolsky', 'http://dbpedia.org/resource/Georgy_Grechko', 'http://dbpedia.org/resource/Ivan_Anikeyev', 'http://dbpedia.org/resource/Konstantin_Feoktistov', 'http://dbpedia.org/resource/Leonid_Ivanov_(test_pilot)', 'http://dbpedia.org/resource/Leonid_Kizim', 'http://dbpedia.org/resource/Leonid_Popov', 'http://dbpedia.org/resource/Lev_Dyomin', 'http://dbpedia.org/resource/Mars_Rafikov', 'http://dbpedia.org/resource/Nikolai_Rukavishnikov', 'http://dbpedia.org/resource/Oleg_Atkov', 'http://dbpedia.org/resource/Oleg_Grigoriyevich_Kononenko', 'http://dbpedia.org/resource/Oleg_Makarov_(cosmonaut)', 'http://dbpedia.org/resource/Pavel_Belyayev', 'http://dbpedia.org/resource/Sergey_Volkov_(cosmonaut)', 'http://dbpedia.org/resource/Sergey_Vozovikov', 'http://dbpedia.org/resource/Valentin_Bondarenko', 'http://dbpedia.org/resource/Valentin_Lebedev', 'http://dbpedia.org/resource/Valery_Bykovsky', 'http://dbpedia.org/resource/Valery_Kubasov', 'http://dbpedia.org/resource/Valery_Rozhdestvensky', 'http://dbpedia.org/resource/Valery_Ryumin', 'http://dbpedia.org/resource/Vasily_Lazarev', 'http://dbpedia.org/resource/Viktor_Gorbatko', 'http://dbpedia.org/resource/Viktor_Patsayev', 'http://dbpedia.org/resource/Viktor_Savinykh', 'http://dbpedia.org/resource/Vitaly_Sevastyanov', 'http://dbpedia.org/resource/Vladimir_Aksyonov', 'http://dbpedia.org/resource/Vladimir_Dzhanibekov', 'http://dbpedia.org/resource/Vladimir_Shatalov', 'http://dbpedia.org/resource/Vladimir_Solovyov_(cosmonaut)', 'http://dbpedia.org/resource/Vladimir_Vasyutin', 'http://dbpedia.org/resource/Vladislav_Volkov', 'http://dbpedia.org/resource/Vyacheslav_Zudov', 'http://dbpedia.org/resource/Yevgeny_Khrunov', 'http://dbpedia.org/resource/Yuri_Artyukhin', 'http://dbpedia.org/resource/Yuri_Glazkov', 'http://dbpedia.org/resource/Yuri_Malyshev_(cosmonaut)', 'http://dbpedia.org/resource/Yuri_Romanenko']</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Benin', 'http://dbpedia.org/resource/Burkina_Faso', 'http://dbpedia.org/resource/Colonial_Mauritania', 'http://dbpedia.org/resource/Colony_of_Niger', 'http://dbpedia.org/resource/Economic_Community_of_West_African_States', 'http://dbpedia.org/resource/French_Dahomey', 'http://dbpedia.org/resource/French_Togoland', 'http://dbpedia.org/resource/Guinea-Bissau', 'http://dbpedia.org/resource/History_of_Togo', 'http://dbpedia.org/resource/Ivory_Coast', 'http://dbpedia.org/resource/Mali', 'http://dbpedia.org/resource/Niger', "http://dbpedia.org/resource/People's_Republic_of_Benin", 'http://dbpedia.org/resource/Republic_of_Dahomey', 'http://dbpedia.org/resource/Republic_of_Upper_Volta', 'http://dbpedia.org/resource/Senegal', 'http://dbpedia.org/resource/Senegambia_Confederation', 'http://dbpedia.org/resource/Togo']</t>
+          <t>['http://dbpedia.org/resource/Aleksandr_Aleksandrovich_Volkov', 'http://dbpedia.org/resource/Aleksandr_Ivanchenkov', 'http://dbpedia.org/resource/Aleksandr_Laveykin', 'http://dbpedia.org/resource/Aleksandr_Nikolayevich_Balandin', 'http://dbpedia.org/resource/Aleksandr_Pavlovich_Aleksandrov__Aleksandr_Pavlovich_Aleksandrov__1', 'http://dbpedia.org/resource/Aleksandr_Serebrov', 'http://dbpedia.org/resource/Aleksandr_Viktorenko', 'http://dbpedia.org/resource/Aleksei_Gubarev', 'http://dbpedia.org/resource/Aleksei_Yeliseyev', 'http://dbpedia.org/resource/Anatoly_Berezovoy', 'http://dbpedia.org/resource/Anatoly_Filipchenko', 'http://dbpedia.org/resource/Anatoly_Levchenko__Anatoly_Semyonovich_Levchenko__1', 'http://dbpedia.org/resource/Andriyan_Nikolayev', 'http://dbpedia.org/resource/Boris_Andreyev_(cosmonaut)', 'http://dbpedia.org/resource/Boris_Volynov', 'http://dbpedia.org/resource/Boris_Yegorov', 'http://dbpedia.org/resource/Gennady_Manakov', 'http://dbpedia.org/resource/Gennady_Sarafanov', 'http://dbpedia.org/resource/Gennady_Strekalov', 'http://dbpedia.org/resource/Georgy_Dobrovolsky', 'http://dbpedia.org/resource/Georgy_Grechko', 'http://dbpedia.org/resource/Ivan_Anikeyev', 'http://dbpedia.org/resource/Konstantin_Feoktistov', 'http://dbpedia.org/resource/Leonid_Ivanov_(test_pilot)', 'http://dbpedia.org/resource/Leonid_Kizim', 'http://dbpedia.org/resource/Leonid_Popov', 'http://dbpedia.org/resource/Lev_Dyomin', 'http://dbpedia.org/resource/Mars_Rafikov', 'http://dbpedia.org/resource/Nikolai_Rukavishnikov', 'http://dbpedia.org/resource/Oleg_Atkov', 'http://dbpedia.org/resource/Oleg_Grigoriyevich_Kononenko', 'http://dbpedia.org/resource/Oleg_Makarov_(cosmonaut)', 'http://dbpedia.org/resource/Pavel_Belyayev', 'http://dbpedia.org/resource/Sergey_Volkov_(cosmonaut)', 'http://dbpedia.org/resource/Sergey_Vozovikov', 'http://dbpedia.org/resource/Valentin_Bondarenko', 'http://dbpedia.org/resource/Valentin_Lebedev', 'http://dbpedia.org/resource/Valery_Bykovsky', 'http://dbpedia.org/resource/Valery_Kubasov', 'http://dbpedia.org/resource/Valery_Rozhdestvensky', 'http://dbpedia.org/resource/Valery_Ryumin', 'http://dbpedia.org/resource/Vasily_Lazarev', 'http://dbpedia.org/resource/Viktor_Gorbatko', 'http://dbpedia.org/resource/Viktor_Patsayev', 'http://dbpedia.org/resource/Viktor_Savinykh', 'http://dbpedia.org/resource/Vitaly_Sevastyanov', 'http://dbpedia.org/resource/Vladimir_Aksyonov', 'http://dbpedia.org/resource/Vladimir_Dzhanibekov', 'http://dbpedia.org/resource/Vladimir_Shatalov', 'http://dbpedia.org/resource/Vladimir_Solovyov_(cosmonaut)', 'http://dbpedia.org/resource/Vladimir_Vasyutin', 'http://dbpedia.org/resource/Vladislav_Volkov', 'http://dbpedia.org/resource/Vyacheslav_Zudov', 'http://dbpedia.org/resource/Yevgeny_Khrunov', 'http://dbpedia.org/resource/Yuri_Artyukhin', 'http://dbpedia.org/resource/Yuri_Glazkov', 'http://dbpedia.org/resource/Yuri_Malyshev_(cosmonaut)', 'http://dbpedia.org/resource/Yuri_Romanenko']</t>
         </is>
       </c>
       <c r="D25" t="b">
@@ -938,17 +938,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Which Greek parties are pro-European?</t>
+          <t>Who created Family Guy?</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Democratic_Alignment_(2015)', 'http://dbpedia.org/resource/Movement_of_Democratic_Socialists', 'http://dbpedia.org/resource/Movement_of_Free_Citizens_(Greece)', 'http://dbpedia.org/resource/PASOK_–_Movement_for_Change', 'http://dbpedia.org/resource/PASOK', 'http://dbpedia.org/resource/Radical_Movement_of_Social_Democratic_Alliance']</t>
+          <t>['http://dbpedia.org/resource/Seth_MacFarlane']</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Democratic_Alignment_(2015)', 'http://dbpedia.org/resource/Movement_of_Democratic_Socialists', 'http://dbpedia.org/resource/Movement_of_Free_Citizens_(Greece)', 'http://dbpedia.org/resource/PASOK_–_Movement_for_Change', 'http://dbpedia.org/resource/PASOK', 'http://dbpedia.org/resource/Radical_Movement_of_Social_Democratic_Alliance']</t>
+          <t>['http://dbpedia.org/resource/Seth_MacFarlane']</t>
         </is>
       </c>
       <c r="D26" t="b">
@@ -958,17 +958,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Who wrote the Game of Thrones theme?</t>
+          <t>How much is the population of mexico city ?</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Ramin_Djawadi']</t>
+          <t>['9209944']</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Ramin_Djawadi']</t>
+          <t>['9209944']</t>
         </is>
       </c>
       <c r="D27" t="b">
@@ -978,140 +978,60 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Which bridges cross the Seine?</t>
+          <t>How many people live in the capital of Australia?</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Passerelle_Debilly', 'http://dbpedia.org/resource/Passerelle_Simone-de-Beauvoir', 'http://dbpedia.org/resource/Pont_Alexandre_III', 'http://dbpedia.org/resource/Pont_amont', 'http://dbpedia.org/resource/Pont_au_Change', 'http://dbpedia.org/resource/Pont_au_Double', 'http://dbpedia.org/resource/Pont_aval', 'http://dbpedia.org/resource/Pont_Charles-de-Gaulle', "http://dbpedia.org/resource/Pont_d'Austerlitz", "http://dbpedia.org/resource/Pont_d'Iéna", 'http://dbpedia.org/resource/Pont_de_Bercy', 'http://dbpedia.org/resource/Pont_de_Bir-Hakeim', 'http://dbpedia.org/resource/Pont_de_Brotonne', 'http://dbpedia.org/resource/Pont_de_Grenelle', "http://dbpedia.org/resource/Pont_de_l'Alma", "http://dbpedia.org/resource/Pont_de_l'Archevêché", 'http://dbpedia.org/resource/Pont_de_la_Concorde_(Paris)', 'http://dbpedia.org/resource/Pont_de_la_Tournelle', 'http://dbpedia.org/resource/Pont_de_Neuilly', 'http://dbpedia.org/resource/Pont_de_Normandie', 'http://dbpedia.org/resource/Pont_de_Sully', 'http://dbpedia.org/resource/Pont_de_Tolbiac', 'http://dbpedia.org/resource/Pont_des_Invalides', 'http://dbpedia.org/resource/Pont_du_Carrousel', 'http://dbpedia.org/resource/Pont_du_Garigliano', 'http://dbpedia.org/resource/Pont_Gustave-Flaubert', 'http://dbpedia.org/resource/Pont_Louis-Philippe', 'http://dbpedia.org/resource/Pont_Marie', 'http://dbpedia.org/resource/Pont_National', 'http://dbpedia.org/resource/Pont_Neuf', 'http://dbpedia.org/resource/Pont_Notre-Dame', 'http://dbpedia.org/resource/Pont_Rouelle', 'http://dbpedia.org/resource/Pont_Royal', "http://dbpedia.org/resource/Port_à_l'Anglais_Bridge", "http://dbpedia.org/resource/Viaduc_d'Austerlitz"]</t>
+          <t>['453558']</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Passerelle_Debilly', 'http://dbpedia.org/resource/Passerelle_Simone-de-Beauvoir', 'http://dbpedia.org/resource/Pont_Alexandre_III', 'http://dbpedia.org/resource/Pont_amont', 'http://dbpedia.org/resource/Pont_au_Change', 'http://dbpedia.org/resource/Pont_au_Double', 'http://dbpedia.org/resource/Pont_aval', 'http://dbpedia.org/resource/Pont_Charles-de-Gaulle', "http://dbpedia.org/resource/Pont_d'Austerlitz", "http://dbpedia.org/resource/Pont_d'Iéna", 'http://dbpedia.org/resource/Pont_de_Bercy', 'http://dbpedia.org/resource/Pont_de_Bir-Hakeim', 'http://dbpedia.org/resource/Pont_de_Brotonne', 'http://dbpedia.org/resource/Pont_de_Grenelle', "http://dbpedia.org/resource/Pont_de_l'Alma", "http://dbpedia.org/resource/Pont_de_l'Archevêché", 'http://dbpedia.org/resource/Pont_de_la_Concorde_(Paris)', 'http://dbpedia.org/resource/Pont_de_la_Tournelle', 'http://dbpedia.org/resource/Pont_de_Neuilly', 'http://dbpedia.org/resource/Pont_de_Normandie', 'http://dbpedia.org/resource/Pont_de_Sully', 'http://dbpedia.org/resource/Pont_de_Tolbiac', 'http://dbpedia.org/resource/Pont_des_Invalides', 'http://dbpedia.org/resource/Pont_du_Carrousel', 'http://dbpedia.org/resource/Pont_du_Garigliano', 'http://dbpedia.org/resource/Pont_Gustave-Flaubert', 'http://dbpedia.org/resource/Pont_Louis-Philippe', 'http://dbpedia.org/resource/Pont_Marie', 'http://dbpedia.org/resource/Pont_National', 'http://dbpedia.org/resource/Pont_Neuf', 'http://dbpedia.org/resource/Pont_Notre-Dame', 'http://dbpedia.org/resource/Pont_Rouelle', 'http://dbpedia.org/resource/Pont_Royal', "http://dbpedia.org/resource/Port_à_l'Anglais_Bridge", "http://dbpedia.org/resource/Viaduc_d'Austerlitz"]</t>
+          <t>['http://dbpedia.org/resource/Canberra', '453558']</t>
         </is>
       </c>
       <c r="D28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Give me a list of all bandleaders that play trumpet.</t>
+          <t>how big is the total area of North Rhine- Westphalia?</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Abatte_Barihun', 'http://dbpedia.org/resource/Alan_Silva', 'http://dbpedia.org/resource/Artie_Fields', 'http://dbpedia.org/resource/Charlie_Spivak', 'http://dbpedia.org/resource/Danny_Davis_(country_musician)', 'http://dbpedia.org/resource/Doc_Cheatham', 'http://dbpedia.org/resource/Ernest_%22Doc%22_Paulin', 'http://dbpedia.org/resource/Jack_Jackson_(radio_personality)', 'http://dbpedia.org/resource/Jacobo_Rubalcaba', 'http://dbpedia.org/resource/Jimmy_Dorsey', 'http://dbpedia.org/resource/Kaj_Backlund', 'http://dbpedia.org/resource/Lloyd_Hunter', 'http://dbpedia.org/resource/Marlon_Jordan', 'http://dbpedia.org/resource/Mick_Mulligan', 'http://dbpedia.org/resource/Ollie_Mitchell', 'http://dbpedia.org/resource/Ovie_Alston', 'http://dbpedia.org/resource/Pacho_Galan', 'http://dbpedia.org/resource/Red_Perkins', 'http://dbpedia.org/resource/Richard_Maltby_Sr.', 'http://dbpedia.org/resource/Steamboat_Willie_(musician)']</t>
+          <t>['34084130000']</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Aaron_Rimbui', 'http://dbpedia.org/resource/Abatte_Barihun', 'http://dbpedia.org/resource/Airto_Moreira', 'http://dbpedia.org/resource/Akira_Ishikawa', 'http://dbpedia.org/resource/Alan_Silva', 'http://dbpedia.org/resource/Alix_Combelle', 'http://dbpedia.org/resource/Ambrose_(bandleader)', 'http://dbpedia.org/resource/Andrew_Cyrille', 'http://dbpedia.org/resource/Anna_Mae_Winburn', 'http://dbpedia.org/resource/Annette_A._Aguilar', 'http://dbpedia.org/resource/Antonio_María_Romeu', 'http://dbpedia.org/resource/Antonio_Morelli', 'http://dbpedia.org/resource/Archie_Semple', 'http://dbpedia.org/resource/Artie_Fields', 'http://dbpedia.org/resource/Assaf_Kehati', 'http://dbpedia.org/resource/Ayinde_Bakare', 'http://dbpedia.org/resource/B._A._Rolfe', 'http://dbpedia.org/resource/Barnabás_von_Géczy', 'http://dbpedia.org/resource/Ben_Selvin', 'http://dbpedia.org/resource/Bernie_Cummins', 'http://dbpedia.org/resource/Bert_Firman', 'http://dbpedia.org/resource/Bert_Kaempfert', 'http://dbpedia.org/resource/Big_George__Big_George__1', 'http://dbpedia.org/resource/Bill_Le_Sage', 'http://dbpedia.org/resource/Billy_Hughes_(musician)', 'http://dbpedia.org/resource/Billy_Jenkins_(musician)', 'http://dbpedia.org/resource/Blaise_Siwula', 'http://dbpedia.org/resource/Bob_Chester', 'http://dbpedia.org/resource/Bob_French_(jazz_musician)', 'http://dbpedia.org/resource/Bobby_Hammack', 'http://dbpedia.org/resource/Branislav_Lala_Kovačev', 'http://dbpedia.org/resource/Brent_Gallaher', 'http://dbpedia.org/resource/Brian_Fahey_(composer)', 'http://dbpedia.org/resource/Buddy_Morrow', 'http://dbpedia.org/resource/Calvin_A._Johnson_Jr.', 'http://dbpedia.org/resource/Carlos_%22Patato%22_Valdes', 'http://dbpedia.org/resource/Carroll_Dickerson', 'http://dbpedia.org/resource/Charles_A._Prince', 'http://dbpedia.org/resource/Charles_Williams_(musician)', 'http://dbpedia.org/resource/Charlie_Kunz', 'http://dbpedia.org/resource/Charlie_Palmieri', 'http://dbpedia.org/resource/Charlie_Spivak', 'http://dbpedia.org/resource/Christoph_Irniger', 'http://dbpedia.org/resource/Chuckii_Booker', 'http://dbpedia.org/resource/Claiborne_Williams', 'http://dbpedia.org/resource/Dajos_Béla', 'http://dbpedia.org/resource/Dana_Hall_(musician)', 'http://dbpedia.org/resource/Danny_Davis_(country_musician)', 'http://dbpedia.org/resource/Dave_Liebman', 'http://dbpedia.org/resource/Dave_Shepherd', 'http://dbpedia.org/resource/Dave_Stogner', 'http://dbpedia.org/resource/Deborah_Weisz', 'http://dbpedia.org/resource/Dennis_Rollins', 'http://dbpedia.org/resource/Desi_Arnaz__Desi_Arnaz__1', 'http://dbpedia.org/resource/Dick_Willebrandts', 'http://dbpedia.org/resource/Doc_Cheatham', 'http://dbpedia.org/resource/Don_Falcone', 'http://dbpedia.org/resource/Doreen_Ketchens', 'http://dbpedia.org/resource/Dylan_Howe', 'http://dbpedia.org/resource/Earl_Hines', 'http://dbpedia.org/resource/Eddy_Howard', 'http://dbpedia.org/resource/Édouard_Ferlet', 'http://dbpedia.org/resource/Edward_Wilkerson', 'http://dbpedia.org/resource/Eric_Dolphy', 'http://dbpedia.org/resource/Eric_Ineke', 'http://dbpedia.org/resource/Eric_Winstone__Eric_Winstone__1', 'http://dbpedia.org/resource/Ernest_%22Doc%22_Paulin', 'http://dbpedia.org/resource/Ernie_Fields', 'http://dbpedia.org/resource/Ernie_Freeman', 'http://dbpedia.org/resource/Ernie_Odoom', 'http://dbpedia.org/resource/Eua_Sunthornsanan', 'http://dbpedia.org/resource/Everett_Robbins', 'http://dbpedia.org/resource/Félix_Reina', 'http://dbpedia.org/resource/Frank_Chacksfield', 'http://dbpedia.org/resource/Fred_Elizalde', 'http://dbpedia.org/resource/Fred_Rich', 'http://dbpedia.org/resource/Freddie_Slack', 'http://dbpedia.org/resource/Freddy_Nagel', 'http://dbpedia.org/resource/Gay_Woods', 'http://dbpedia.org/resource/George_Olsen', 'http://dbpedia.org/resource/Gerald_Danovitch', 'http://dbpedia.org/resource/Gil_Evans', 'http://dbpedia.org/resource/Gilberto_Santa_Rosa', 'http://dbpedia.org/resource/Glen_Gray', 'http://dbpedia.org/resource/Graham_Reynolds_(composer)', 'http://dbpedia.org/resource/Guillermo_Rubalcaba', 'http://dbpedia.org/resource/Hal_Kemp', 'http://dbpedia.org/resource/Harry_Baisden', 'http://dbpedia.org/resource/Harry_Parry', 'http://dbpedia.org/resource/Harry_Robertson_(musician)', 'http://dbpedia.org/resource/Hart_Wand', 'http://dbpedia.org/resource/Helen_May_Butler', 'http://dbpedia.org/resource/Henry_Hall_(bandleader)', 'http://dbpedia.org/resource/Hotep_Idris_Galeta', 'http://dbpedia.org/resource/Howard_Lanin', 'http://dbpedia.org/resource/Hurshul_Clothier', 'http://dbpedia.org/resource/Igor_Butman', 'http://dbpedia.org/resource/Igor_Grigoriev', 'http://dbpedia.org/resource/Isaac_M._Carpenter', 'http://dbpedia.org/resource/Issie_Barratt', 'http://dbpedia.org/resource/Jack_Jackson_(radio_personality)', 'http://dbpedia.org/resource/Jack_McVea', 'http://dbpedia.org/resource/Jacobo_Rubalcaba', 'http://dbpedia.org/resource/James_Mainwaring', 'http://dbpedia.org/resource/Jay_Wilbur', 'http://dbpedia.org/resource/Jerry_Fielding', 'http://dbpedia.org/resource/Jesper_Thilo', 'http://dbpedia.org/resource/Jim_Gailloreto', 'http://dbpedia.org/resource/Jimmy_Dorsey', 'http://dbpedia.org/resource/Joe_Lutcher', 'http://dbpedia.org/resource/John_Coltrane', 'http://dbpedia.org/resource/John_Serry_Jr.', 'http://dbpedia.org/resource/Jose_Vazquez-Cofresi', 'http://dbpedia.org/resource/Juan_García_Esquivel', 'http://dbpedia.org/resource/Julia_Feldman', 'http://dbpedia.org/resource/Julien_Lourau', 'http://dbpedia.org/resource/Kaj_Backlund', 'http://dbpedia.org/resource/Karel_Krautgartner', 'http://dbpedia.org/resource/Karl_E._H._Seigfried', 'http://dbpedia.org/resource/Kay_Kyser', 'http://dbpedia.org/resource/Kenny_Lovelace', 'http://dbpedia.org/resource/King_Oliver__King_Oliver__1', 'http://dbpedia.org/resource/Kit_McClure', 'http://dbpedia.org/resource/Larry_Clinton', 'http://dbpedia.org/resource/Lee_Vincent', 'http://dbpedia.org/resource/Leon_McAuliffe', 'http://dbpedia.org/resource/Lester_Lanin', 'http://dbpedia.org/resource/Lew_Stone', 'http://dbpedia.org/resource/Lloyd_Glenn', 'http://dbpedia.org/resource/Lloyd_Hunter', 'http://dbpedia.org/resource/Lloyd_Price', 'http://dbpedia.org/resource/Lonnie_Youngblood', 'http://dbpedia.org/resource/Lou_Donaldson', 'http://dbpedia.org/resource/Mark_Bassey', 'http://dbpedia.org/resource/Mark_Masters_(musician)', 'http://dbpedia.org/resource/Marlon_Jordan', 'http://dbpedia.org/resource/Martin_Denny', 'http://dbpedia.org/resource/Mat_Walerian', 'http://dbpedia.org/resource/Mathias_Rüegg', 'http://dbpedia.org/resource/Matthew_Bourne_(musician)', 'http://dbpedia.org/resource/Maurice_Winnick', 'http://dbpedia.org/resource/Maynard_Ferguson', 'http://dbpedia.org/resource/Mel_Henke', 'http://dbpedia.org/resource/Memo_Acevedo', 'http://dbpedia.org/resource/Meredith_Willson', 'http://dbpedia.org/resource/Merl_Lindsay', 'http://dbpedia.org/resource/Metropolitan_Jazz_Octet__Jim_Gailloreto__1', 'http://dbpedia.org/resource/Metropolitan_Jazz_Octet', 'http://dbpedia.org/resource/Mick_Mulligan', 'http://dbpedia.org/resource/Mike_Daniels_(musician)', 'http://dbpedia.org/resource/Mop_Mop', 'http://dbpedia.org/resource/Moses_Boyd', 'http://dbpedia.org/resource/Mynie_Sutton', 'http://dbpedia.org/resource/Nat_Towles', 'http://dbpedia.org/resource/Nick_Lucas', 'http://dbpedia.org/resource/Nick_St._Nicholas', 'http://dbpedia.org/resource/Nicola_Conte', 'http://dbpedia.org/resource/Nicolas_Vatomanga', 'http://dbpedia.org/resource/Oliver_Sain', 'http://dbpedia.org/resource/Ollie_Mitchell', 'http://dbpedia.org/resource/Orestes_López', 'http://dbpedia.org/resource/Oscar_Rabin', 'http://dbpedia.org/resource/Otto_Lington', 'http://dbpedia.org/resource/Ovie_Alston', 'http://dbpedia.org/resource/Pacho_Galan', 'http://dbpedia.org/resource/Paco_Sery', 'http://dbpedia.org/resource/Paddy_Killoran', 'http://dbpedia.org/resource/Paul_Dunmall', 'http://dbpedia.org/resource/Paul_Specht', 'http://dbpedia.org/resource/Paul_Whiteman', 'http://dbpedia.org/resource/Peggy_Gilbert', 'http://dbpedia.org/resource/Percy_Faith', 'http://dbpedia.org/resource/Porky_Freeman', 'http://dbpedia.org/resource/Rabih_Abou-Khalil', 'http://dbpedia.org/resource/Ray_Anthony', 'http://dbpedia.org/resource/Ray_Lawrence_(record_producer)', 'http://dbpedia.org/resource/Ray_McKinley', 'http://dbpedia.org/resource/Raymond_Scott', 'http://dbpedia.org/resource/Red_Murrell', 'http://dbpedia.org/resource/Red_Perkins', 'http://dbpedia.org/resource/Reed_Mathis', 'http://dbpedia.org/resource/Richard_Maltby_Sr.', 'http://dbpedia.org/resource/Richie_Pratt', 'http://dbpedia.org/resource/Robby_Ameen', 'http://dbpedia.org/resource/Rockie_Charles', 'http://dbpedia.org/resource/Roger_Wolfe_Kahn', 'http://dbpedia.org/resource/Roy_Fox', 'http://dbpedia.org/resource/Roy_Nathanson', 'http://dbpedia.org/resource/Sam_Taylor_(blues_musician)', 'http://dbpedia.org/resource/Sam_Wooding', 'http://dbpedia.org/resource/Sean_Bergin', 'http://dbpedia.org/resource/Secondo_Casadei', 'http://dbpedia.org/resource/Shelly_Manne', 'http://dbpedia.org/resource/Simon_Brehm', 'http://dbpedia.org/resource/Solomon_Ilori', 'http://dbpedia.org/resource/Stan_Keller', 'http://dbpedia.org/resource/Steamboat_Willie_(musician)', 'http://dbpedia.org/resource/Sugar_Pie_DeSanto', 'http://dbpedia.org/resource/Tal_Henry', 'http://dbpedia.org/resource/Tal_Wilkenfeld', 'http://dbpedia.org/resource/Ted_Weems', 'http://dbpedia.org/resource/Teddy_Stauffer', 'http://dbpedia.org/resource/Terry_Woods', 'http://dbpedia.org/resource/Thelma_Terry', 'http://dbpedia.org/resource/Tiny_Bradshaw', 'http://dbpedia.org/resource/Tommy_Tucker_(bandleader)', 'http://dbpedia.org/resource/Tommy_Vig', 'http://dbpedia.org/resource/Torsten_Cassel', 'http://dbpedia.org/resource/Vigon_(artist)', 'http://dbpedia.org/resource/Vincent_Montana_Jr.', 'http://dbpedia.org/resource/Wallace_Hartley', 'http://dbpedia.org/resource/Will_Osborne_(singer)', 'http://dbpedia.org/resource/Willie_Rosario', 'http://dbpedia.org/resource/Woody_Herman', 'http://dbpedia.org/resource/Yvonnick_Prené', 'http://dbpedia.org/resource/Aaron_Bertram', 'http://dbpedia.org/resource/Abatte_Barihun', 'http://dbpedia.org/resource/Adam_Deibert', 'http://dbpedia.org/resource/Adam_Gardner', 'http://dbpedia.org/resource/Adam_Taubitz', 'http://dbpedia.org/resource/Ade_Monsbourgh', 'http://dbpedia.org/resource/Adolf_Scherbaum', 'http://dbpedia.org/resource/Adolph_Herseth', 'http://dbpedia.org/resource/Afro-Cuban_jazz', 'http://dbpedia.org/resource/Afrodizz', 'http://dbpedia.org/resource/Al_Caldwell', 'http://dbpedia.org/resource/Al_Hurricane_Jr.', 'http://dbpedia.org/resource/Alan_Rubin', 'http://dbpedia.org/resource/Alan_Shorter', 'http://dbpedia.org/resource/Alan_Silva', 'http://dbpedia.org/resource/Alcione_Nazareth', 'http://dbpedia.org/resource/Alex_St._Clair', 'http://dbpedia.org/resource/Alfredo_%22Chocolate%22_Armenteros', 'http://dbpedia.org/resource/Alison_Balsom__Alison_Balsom__1', 'http://dbpedia.org/resource/Ambrose_Akinmusire', 'http://dbpedia.org/resource/Andre_Canniere', 'http://dbpedia.org/resource/Andrzej_Przybielski', 'http://dbpedia.org/resource/Andy_Blakeney', 'http://dbpedia.org/resource/Anssi_Neuvonen', 'http://dbpedia.org/resource/Anthony_Harley', 'http://dbpedia.org/resource/Anthony_Rossomando', 'http://dbpedia.org/resource/Antonio_Breschi', 'http://dbpedia.org/resource/Arthur_Whetsel', 'http://dbpedia.org/resource/Artie_Fields', 'http://dbpedia.org/resource/Arturo_Sandoval', 'http://dbpedia.org/resource/Arve_Henriksen', 'http://dbpedia.org/resource/Atle_Hammer', 'http://dbpedia.org/resource/Augustine_Leudar', 'http://dbpedia.org/resource/Baba_Brooks', 'http://dbpedia.org/resource/Balkan_ballad', 'http://dbpedia.org/resource/Balkan_Bump', 'http://dbpedia.org/resource/Banda_music', 'http://dbpedia.org/resource/Bart_Maris', 'http://dbpedia.org/resource/Ben_Cauley', 'http://dbpedia.org/resource/Ben_Zion_Solomon', 'http://dbpedia.org/resource/Bernard_Anderson_(trumpeter)', 'http://dbpedia.org/resource/Billy_Butterfield', 'http://dbpedia.org/resource/Boban_Marković', 'http://dbpedia.org/resource/Bobby_Bryant_(musician)', 'http://dbpedia.org/resource/Bobby_Shew', 'http://dbpedia.org/resource/Bobby_Stark', 'http://dbpedia.org/resource/Brad_Turner_(musician)', 'http://dbpedia.org/resource/Brian_Carpenter_(musician)', 'http://dbpedia.org/resource/Bud_Brisbois', 'http://dbpedia.org/resource/Cag_Cagnolatti', 'http://dbpedia.org/resource/Cal_Harris_Jr.', 'http://dbpedia.org/resource/Canadian_blues', 'http://dbpedia.org/resource/Carl_Saunders', 'http://dbpedia.org/resource/Cecil_Bridgewater', 'http://dbpedia.org/resource/Charles_Sullivan_(musician)', 'http://dbpedia.org/resource/Charles_Tolliver', 'http://dbpedia.org/resource/Charlie_Green_(singer)', 'http://dbpedia.org/resource/Charlie_Spivak', 'http://dbpedia.org/resource/Chase_Sanborn', 'http://dbpedia.org/resource/Chris_Botti', 'http://dbpedia.org/resource/Chris_Kelly_(jazz)', 'http://dbpedia.org/resource/Chris_Walden', 'http://dbpedia.org/resource/Chuck_Mangione', 'http://dbpedia.org/resource/Cindy_Bradley', 'http://dbpedia.org/resource/CJ_Camerieri', 'http://dbpedia.org/resource/Clarence_Shaw', 'http://dbpedia.org/resource/Claude_Deppa', 'http://dbpedia.org/resource/Claude_Gordon', 'http://dbpedia.org/resource/Clyde_Hurley', 'http://dbpedia.org/resource/Colin_Smith_(musician)', 'http://dbpedia.org/resource/Conrad_Gozzo', 'http://dbpedia.org/resource/Cootie_Williams', 'http://dbpedia.org/resource/Cynthia_Robinson', 'http://dbpedia.org/resource/Dale_Turner_(trumpeter)', 'http://dbpedia.org/resource/Dan_Jacobs_(trumpeter)', 'http://dbpedia.org/resource/Danijela_Veselinović', 'http://dbpedia.org/resource/Danny_Davis_(country_musician)', 'http://dbpedia.org/resource/Danny_Heifetz', 'http://dbpedia.org/resource/Dave_Clark_(Canadian_musician)', 'http://dbpedia.org/resource/David_Blink', 'http://dbpedia.org/resource/David_Rosebrook', "http://dbpedia.org/resource/Days_N'_Daze", 'http://dbpedia.org/resource/Del_Staigers', 'http://dbpedia.org/resource/Dennis_González', 'http://dbpedia.org/resource/Dick_Cuthell', 'http://dbpedia.org/resource/Dick_Sudhalter', 'http://dbpedia.org/resource/Dixieland_jazz', 'http://dbpedia.org/resource/Dizzy_Gillespie', 'http://dbpedia.org/resource/Doc_Cheatham', 'http://dbpedia.org/resource/Doc_Severinsen', 'http://dbpedia.org/resource/Dominique_Leone', 'http://dbpedia.org/resource/Don_Fagerquist', 'http://dbpedia.org/resource/Don_Sleet', 'http://dbpedia.org/resource/Dwayne_Goettel', 'http://dbpedia.org/resource/Eddie_Calvert', 'http://dbpedia.org/resource/Eddie_Thornton', 'http://dbpedia.org/resource/Eddie_Vartan', 'http://dbpedia.org/resource/Eddy_Okonta', 'http://dbpedia.org/resource/Edna_White', 'http://dbpedia.org/resource/Eduardo_Cabra', 'http://dbpedia.org/resource/Edward_Carroll_(musician)', 'http://dbpedia.org/resource/Eivind_Lønning', 'http://dbpedia.org/resource/Elmer_Chambers', 'http://dbpedia.org/resource/Elwood_Buchanan', 'http://dbpedia.org/resource/Ephraim_Owens', 'http://dbpedia.org/resource/Erik_Jekabson', 'http://dbpedia.org/resource/Ernest_%22Doc%22_Paulin', 'http://dbpedia.org/resource/Ernie_Hammes', 'http://dbpedia.org/resource/Ernie_Royal', 'http://dbpedia.org/resource/Euel_Box', 'http://dbpedia.org/resource/Félix_Chappottín', 'http://dbpedia.org/resource/Flea_(musician)', 'http://dbpedia.org/resource/Floyd_LeFlore', 'http://dbpedia.org/resource/Folk_jazz', 'http://dbpedia.org/resource/François_Dauverné', 'http://dbpedia.org/resource/Frank_Lacy', 'http://dbpedia.org/resource/Franz_Koglmann', 'http://dbpedia.org/resource/Fred_Mills_(musician)', 'http://dbpedia.org/resource/Fred_Stone_(musician)', 'http://dbpedia.org/resource/Fred_Tackett', 'http://dbpedia.org/resource/Freddie_Hubbard', 'http://dbpedia.org/resource/Freddy_Randall', 'http://dbpedia.org/resource/Frode_Thingnæs', 'http://dbpedia.org/resource/Gary_Grant_(musician)', 'http://dbpedia.org/resource/Gediminas_Gelgotas', 'http://dbpedia.org/resource/George_Dixon_(trumpeter)__George_Dixon__1', 'http://dbpedia.org/resource/George_Stone_(composer)', 'http://dbpedia.org/resource/Giovanni_Srofenaur', 'http://dbpedia.org/resource/Gracie_Cole', 'http://dbpedia.org/resource/Greg_Adams_(musician)', 'http://dbpedia.org/resource/Gunhild_Carling', 'http://dbpedia.org/resource/Harry_Beckett', 'http://dbpedia.org/resource/Hazy_Osterwald', 'http://dbpedia.org/resource/Henry_Busse', 'http://dbpedia.org/resource/Herb_Alpert', 'http://dbpedia.org/resource/Herb_Pomeroy', 'http://dbpedia.org/resource/Herbert_Hardesty', 'http://dbpedia.org/resource/Herbert_Joos', 'http://dbpedia.org/resource/Herbert_L._Clarke', 'http://dbpedia.org/resource/Hollie_Farris', 'http://dbpedia.org/resource/Hoodlum_Priest_(musician)', 'http://dbpedia.org/resource/Hot_Lips_Page', 'http://dbpedia.org/resource/Humphrey_Lyttelton', 'http://dbpedia.org/resource/Ian_Hamer_(musician)', 'http://dbpedia.org/resource/Ian_Svenonius', 'http://dbpedia.org/resource/Ibrahim_Maalouf', 'http://dbpedia.org/resource/Idrees_Sulieman', 'http://dbpedia.org/resource/Ivana_Santilli', 'http://dbpedia.org/resource/Izudin_Čavrković', 'http://dbpedia.org/resource/J._Greg_Miller', 'http://dbpedia.org/resource/Jack_Daugherty_(musician)', 'http://dbpedia.org/resource/Jack_Jackson_(radio_personality)', 'http://dbpedia.org/resource/Jacobo_Rubalcaba', 'http://dbpedia.org/resource/James_%22Bubber%22_Miley', 'http://dbpedia.org/resource/James_F._Burke_(musician)', 'http://dbpedia.org/resource/James_Morrison_(jazz_musician)', 'http://dbpedia.org/resource/Jay_Saunders', 'http://dbpedia.org/resource/Jazz', 'http://dbpedia.org/resource/Jean-Claude_Borelly', 'http://dbpedia.org/resource/Jeff_Bova', 'http://dbpedia.org/resource/Jeff_Irwin', 'http://dbpedia.org/resource/Jeff_Kaiser_(musician)', 'http://dbpedia.org/resource/Jeff_Rosenstock', 'http://dbpedia.org/resource/Jeff_Tyzik', 'http://dbpedia.org/resource/Jeffrey_Morgan_(musician)', 'http://dbpedia.org/resource/Jens_Lindemann', 'http://dbpedia.org/resource/Jens_Petter_Antonsen', 'http://dbpedia.org/resource/Jeremy_Adelman_(composer)', 'http://dbpedia.org/resource/Jerry_González', 'http://dbpedia.org/resource/Jerry_Hey', 'http://dbpedia.org/resource/Jim_Knapp', 'http://dbpedia.org/resource/Jim_Price_(musician)', 'http://dbpedia.org/resource/Jimmy_Brown_(musician)', 'http://dbpedia.org/resource/Jimmy_Dorsey', 'http://dbpedia.org/resource/Jimmy_Sturr', 'http://dbpedia.org/resource/Joan_Hinde', 'http://dbpedia.org/resource/Joe_Lancaster_(musician)', 'http://dbpedia.org/resource/John_Anderson_(jazz_trumpeter)', 'http://dbpedia.org/resource/John_Carisi', 'http://dbpedia.org/resource/John_Chilton', "http://dbpedia.org/resource/John_D'earth__John_D'earth__1", 'http://dbpedia.org/resource/John_Du_Prez', 'http://dbpedia.org/resource/John_Flansburgh', 'http://dbpedia.org/resource/John_Korsrud', 'http://dbpedia.org/resource/John_Madrid', 'http://dbpedia.org/resource/John_McLevy', 'http://dbpedia.org/resource/John_McNeil_(musician)', 'http://dbpedia.org/resource/John_Sangster', 'http://dbpedia.org/resource/Johnny_Carroll_(trumpeter)', 'http://dbpedia.org/resource/Johnny_Moore_(trumpeter)', 'http://dbpedia.org/resource/Johnny_Windhurst', 'http://dbpedia.org/resource/Johnny_Zell', 'http://dbpedia.org/resource/Jon_Hassell', 'http://dbpedia.org/resource/José_Areas', 'http://dbpedia.org/resource/Josh_Deutsch', 'http://dbpedia.org/resource/Jovem_Guarda', 'http://dbpedia.org/resource/Juanchín_Ramírez', 'http://dbpedia.org/resource/Jun_Miyake__Jun_Miyake__1', 'http://dbpedia.org/resource/Kaj_Backlund', 'http://dbpedia.org/resource/Kansas_City_jazz', 'http://dbpedia.org/resource/Kaseko', 'http://dbpedia.org/resource/Ken_Albers', 'http://dbpedia.org/resource/Ken_Greengrass', 'http://dbpedia.org/resource/Ken_Rattenbury', 'http://dbpedia.org/resource/Ken_Watters', 'http://dbpedia.org/resource/Kenny_Passarelli', 'http://dbpedia.org/resource/Kidandali', 'http://dbpedia.org/resource/Kirk_Reeves', 'http://dbpedia.org/resource/Kye_Palmer', 'http://dbpedia.org/resource/Lab_Ox', 'http://dbpedia.org/resource/Laco_Déczi', 'http://dbpedia.org/resource/Larry_Lake_(musician)', 'http://dbpedia.org/resource/Lars_Samuelson', 'http://dbpedia.org/resource/Laura_Jurd', 'http://dbpedia.org/resource/Lee_Loughnane', 'http://dbpedia.org/resource/Leonard_B._Smith_(musician)', 'http://dbpedia.org/resource/Leron_Thomas', 'http://dbpedia.org/resource/Leroy_Jones_(trumpeter)', 'http://dbpedia.org/resource/Lester_Sterling', 'http://dbpedia.org/resource/Lew_Soloff', 'http://dbpedia.org/resource/Lina_Allemano', 'http://dbpedia.org/resource/Lionel_Ferbos', 'http://dbpedia.org/resource/Lloyd_Hunter', 'http://dbpedia.org/resource/Lonnie_McFadden', 'http://dbpedia.org/resource/Louis_de_Vries', 'http://dbpedia.org/resource/Louis_Prima_Jr.', 'http://dbpedia.org/resource/Luis_%22Perico%22_Ortiz', 'http://dbpedia.org/resource/Luis_Beza', 'http://dbpedia.org/resource/Magic_Dick', 'http://dbpedia.org/resource/Malcolm_McNab', 'http://dbpedia.org/resource/Manuel_%22Guajiro%22_Mirabal', 'http://dbpedia.org/resource/Marcus_Belgrave', 'http://dbpedia.org/resource/Mark_DeBarge', 'http://dbpedia.org/resource/Mark_Escueta', 'http://dbpedia.org/resource/Mark_Isham', 'http://dbpedia.org/resource/Mark_Pender', 'http://dbpedia.org/resource/Marlon_Jordan', 'http://dbpedia.org/resource/Marquis_Hill', 'http://dbpedia.org/resource/Marty_Marsala', 'http://dbpedia.org/resource/Mathias_Eick', 'http://dbpedia.org/resource/Maurice_Murphy_(musician)', 'http://dbpedia.org/resource/Maury_Deutsch', 'http://dbpedia.org/resource/Max_Kaminsky_(musician)', 'http://dbpedia.org/resource/Max_Schlossberg', 'http://dbpedia.org/resource/Melissa_Venema', 'http://dbpedia.org/resource/Merenhouse', 'http://dbpedia.org/resource/Méringue', 'http://dbpedia.org/resource/Messaoud_Bellemou', 'http://dbpedia.org/resource/Mic_Gillette', 'http://dbpedia.org/resource/Michael_Wyckoff', 'http://dbpedia.org/resource/Mick_Cooke', 'http://dbpedia.org/resource/Mick_Mulligan', 'http://dbpedia.org/resource/Miguel_Martínez_Domínguez', 'http://dbpedia.org/resource/Mihai_Timofti', 'http://dbpedia.org/resource/Mike_Cotton_(musician)', 'http://dbpedia.org/resource/Mike_Mosiello', 'http://dbpedia.org/resource/Mike_Price_(jazz_trumpeter)', 'http://dbpedia.org/resource/Miles_Davis', 'http://dbpedia.org/resource/Modal_jazz', 'http://dbpedia.org/resource/Mongezi_Feza', 'http://dbpedia.org/resource/Morenada', 'http://dbpedia.org/resource/Muggsy_Spanier', 'http://dbpedia.org/resource/Mutt_Carey', 'http://dbpedia.org/resource/Nat_Adderley', 'http://dbpedia.org/resource/Neo-bop', 'http://dbpedia.org/resource/Nick_LaRocca', 'http://dbpedia.org/resource/Nick_Travis', 'http://dbpedia.org/resource/Nigel_Boddice', 'http://dbpedia.org/resource/Norman_Bailey_(musician)', 'http://dbpedia.org/resource/Oleh_Skrypka', 'http://dbpedia.org/resource/Ollie_Mitchell', 'http://dbpedia.org/resource/Orbert_Davis', 'http://dbpedia.org/resource/Orenda_Fink', 'http://dbpedia.org/resource/Outline_of_jazz', 'http://dbpedia.org/resource/Ovie_Alston', 'http://dbpedia.org/resource/Pacho_Galan', 'http://dbpedia.org/resource/Pamela_Fleming', 'http://dbpedia.org/resource/Paolo_Fresu', 'http://dbpedia.org/resource/Paraguayan_polka', 'http://dbpedia.org/resource/Pat_the_Bunny_(musician)', 'http://dbpedia.org/resource/Patrick_Henry_Hughes', 'http://dbpedia.org/resource/Patsy_Torres', 'http://dbpedia.org/resource/Pee_Wee_Erwin', 'http://dbpedia.org/resource/Per_Nielsen_(musician)', 'http://dbpedia.org/resource/Pete_Rodriguez_(jazz_musician)', 'http://dbpedia.org/resource/Phil_Cohran', 'http://dbpedia.org/resource/Phil_Napoleon', 'http://dbpedia.org/resource/Phil_Slater', 'http://dbpedia.org/resource/Philip_Harper_(trumpeter)', 'http://dbpedia.org/resource/Pietro_Capodiferro', 'http://dbpedia.org/resource/Poncie_Ponce', 'http://dbpedia.org/resource/Pops_Foster', 'http://dbpedia.org/resource/Post-bop', 'http://dbpedia.org/resource/Ralph_Towner', 'http://dbpedia.org/resource/Randy_Brecker', 'http://dbpedia.org/resource/Rashawn_Ross', 'http://dbpedia.org/resource/Ray_Nance', 'http://dbpedia.org/resource/Raymond_Crisara', 'http://dbpedia.org/resource/Raymond_Harry_Brown', 'http://dbpedia.org/resource/Red_Perkins', 'http://dbpedia.org/resource/Rhys_Chatham', 'http://dbpedia.org/resource/Rich_Harrison', 'http://dbpedia.org/resource/Richard_Maltby_Sr.', 'http://dbpedia.org/resource/Richard_Williams_(musician)', 'http://dbpedia.org/resource/Rizzle_Kicks', 'http://dbpedia.org/resource/Robert_Duncan_(composer)', 'http://dbpedia.org/resource/Robert_Russell_Bennett', 'http://dbpedia.org/resource/Robert_Wyatt', 'http://dbpedia.org/resource/Robin_Bengtsson', 'http://dbpedia.org/resource/Roger_Powell_(musician)', 'http://dbpedia.org/resource/Romy_Gosz', 'http://dbpedia.org/resource/Roy_Caton', 'http://dbpedia.org/resource/Roy_Hargrove', 'http://dbpedia.org/resource/Ruby_Braff', 'http://dbpedia.org/resource/Ryan_Anthony', 'http://dbpedia.org/resource/Ryan_Lofty', 'http://dbpedia.org/resource/Samba-choro', 'http://dbpedia.org/resource/Samuel_Miller_(musician)', 'http://dbpedia.org/resource/Saskia_Laroo', 'http://dbpedia.org/resource/Satoru_Kōsaki', 'http://dbpedia.org/resource/Scott_Klopfenstein', 'http://dbpedia.org/resource/Sean_Jones_(trumpeter)', 'http://dbpedia.org/resource/Sergei_Nakariakov', 'http://dbpedia.org/resource/Shahin_Najafi', 'http://dbpedia.org/resource/Shalom_Ronli-Riklis', 'http://dbpedia.org/resource/Snooky_Young', 'http://dbpedia.org/resource/Son_montuno', 'http://dbpedia.org/resource/Sonny_Cohn', 'http://dbpedia.org/resource/Sonny_Lester', 'http://dbpedia.org/resource/Sotelúm', 'http://dbpedia.org/resource/Soundism', 'http://dbpedia.org/resource/Stan_Reynolds_(musician)', 'http://dbpedia.org/resource/Steamboat_Willie_(musician)', 'http://dbpedia.org/resource/Stéphane_Belmondo', 'http://dbpedia.org/resource/Steve_Lieberman', 'http://dbpedia.org/resource/Steven_Bernstein_(musician)', 'http://dbpedia.org/resource/Steven_Reineke', 'http://dbpedia.org/resource/Stewart_%22Dirk%22_Fischer', 'http://dbpedia.org/resource/Stuart_Laughton', 'http://dbpedia.org/resource/Tamborera', 'http://dbpedia.org/resource/Taylor_Ho_Bynum', 'http://dbpedia.org/resource/Teddy_Buckner__Teddy_Buckner__1', 'http://dbpedia.org/resource/Terence_Blanchard', 'http://dbpedia.org/resource/Terrance_Simien', 'http://dbpedia.org/resource/Thad_Jones', 'http://dbpedia.org/resource/The_Potash_Twins', 'http://dbpedia.org/resource/Théo_Charlier', 'http://dbpedia.org/resource/Thomas_Bergersen', 'http://dbpedia.org/resource/Tierra_Caliente_music', 'http://dbpedia.org/resource/Timba_Harris', 'http://dbpedia.org/resource/Timmy_Trumpet', 'http://dbpedia.org/resource/Tine_Thing_Helseth', 'http://dbpedia.org/resource/Tom_Peloso', 'http://dbpedia.org/resource/Tommy_McQuater', 'http://dbpedia.org/resource/Tommy_Stevenson', 'http://dbpedia.org/resource/Tony_Fruscella', 'http://dbpedia.org/resource/Tony_Glausi', 'http://dbpedia.org/resource/Tony_Terran', 'http://dbpedia.org/resource/Torquil_Campbell', 'http://dbpedia.org/resource/Toshinori_Kondo', 'http://dbpedia.org/resource/Trad_jazz', 'http://dbpedia.org/resource/Tyler_James_(American_musician)', 'http://dbpedia.org/resource/Uan_Rasey', 'http://dbpedia.org/resource/Uli_Beckerhoff', 'http://dbpedia.org/resource/Valaida_Snow', 'http://dbpedia.org/resource/Valentine_Snow', 'http://dbpedia.org/resource/Vassily_Brandt__Vassily_Brandt__1', 'http://dbpedia.org/resource/Verneri_Pohjola', 'http://dbpedia.org/resource/Victor_Coulsen', 'http://dbpedia.org/resource/Victoria_Vox', 'http://dbpedia.org/resource/Vince_DiFiore', 'http://dbpedia.org/resource/Vincent_Buono', 'http://dbpedia.org/resource/Vincent_Walker', 'http://dbpedia.org/resource/Walter_%22Junie%22_Morrison', 'http://dbpedia.org/resource/Ward_Pinkett', 'http://dbpedia.org/resource/Webster_Young', 'http://dbpedia.org/resource/Wilbur_Harden', 'http://dbpedia.org/resource/William_Adam_(trumpeter)', 'http://dbpedia.org/resource/William_Dehning', 'http://dbpedia.org/resource/Willie_Colón', 'http://dbpedia.org/resource/Wouter_Hardy']</t>
+          <t>['34084130000']</t>
         </is>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>What is the capital of Cameroon?</t>
+          <t>How many employees does IBM have?</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Yaoundé']</t>
+          <t>['282100']</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>['http://dbpedia.org/resource/Yaoundé']</t>
+          <t>['282100']</t>
         </is>
       </c>
       <c r="D30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Give me all cosmonauts.</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>['http://dbpedia.org/resource/Aleksandr_Aleksandrovich_Volkov', 'http://dbpedia.org/resource/Aleksandr_Ivanchenkov', 'http://dbpedia.org/resource/Aleksandr_Laveykin', 'http://dbpedia.org/resource/Aleksandr_Nikolayevich_Balandin', 'http://dbpedia.org/resource/Aleksandr_Pavlovich_Aleksandrov__Aleksandr_Pavlovich_Aleksandrov__1', 'http://dbpedia.org/resource/Aleksandr_Serebrov', 'http://dbpedia.org/resource/Aleksandr_Viktorenko', 'http://dbpedia.org/resource/Aleksei_Gubarev', 'http://dbpedia.org/resource/Aleksei_Yeliseyev', 'http://dbpedia.org/resource/Anatoly_Berezovoy', 'http://dbpedia.org/resource/Anatoly_Filipchenko', 'http://dbpedia.org/resource/Anatoly_Levchenko__Anatoly_Semyonovich_Levchenko__1', 'http://dbpedia.org/resource/Andriyan_Nikolayev', 'http://dbpedia.org/resource/Boris_Andreyev_(cosmonaut)', 'http://dbpedia.org/resource/Boris_Volynov', 'http://dbpedia.org/resource/Boris_Yegorov', 'http://dbpedia.org/resource/Gennady_Manakov', 'http://dbpedia.org/resource/Gennady_Sarafanov', 'http://dbpedia.org/resource/Gennady_Strekalov', 'http://dbpedia.org/resource/Georgy_Dobrovolsky', 'http://dbpedia.org/resource/Georgy_Grechko', 'http://dbpedia.org/resource/Ivan_Anikeyev', 'http://dbpedia.org/resource/Konstantin_Feoktistov', 'http://dbpedia.org/resource/Leonid_Ivanov_(test_pilot)', 'http://dbpedia.org/resource/Leonid_Kizim', 'http://dbpedia.org/resource/Leonid_Popov', 'http://dbpedia.org/resource/Lev_Dyomin', 'http://dbpedia.org/resource/Mars_Rafikov', 'http://dbpedia.org/resource/Nikolai_Rukavishnikov', 'http://dbpedia.org/resource/Oleg_Atkov', 'http://dbpedia.org/resource/Oleg_Grigoriyevich_Kononenko', 'http://dbpedia.org/resource/Oleg_Makarov_(cosmonaut)', 'http://dbpedia.org/resource/Pavel_Belyayev', 'http://dbpedia.org/resource/Sergey_Volkov_(cosmonaut)', 'http://dbpedia.org/resource/Sergey_Vozovikov', 'http://dbpedia.org/resource/Valentin_Bondarenko', 'http://dbpedia.org/resource/Valentin_Lebedev', 'http://dbpedia.org/resource/Valery_Bykovsky', 'http://dbpedia.org/resource/Valery_Kubasov', 'http://dbpedia.org/resource/Valery_Rozhdestvensky', 'http://dbpedia.org/resource/Valery_Ryumin', 'http://dbpedia.org/resource/Vasily_Lazarev', 'http://dbpedia.org/resource/Viktor_Gorbatko', 'http://dbpedia.org/resource/Viktor_Patsayev', 'http://dbpedia.org/resource/Viktor_Savinykh', 'http://dbpedia.org/resource/Vitaly_Sevastyanov', 'http://dbpedia.org/resource/Vladimir_Aksyonov', 'http://dbpedia.org/resource/Vladimir_Dzhanibekov', 'http://dbpedia.org/resource/Vladimir_Shatalov', 'http://dbpedia.org/resource/Vladimir_Solovyov_(cosmonaut)', 'http://dbpedia.org/resource/Vladimir_Vasyutin', 'http://dbpedia.org/resource/Vladislav_Volkov', 'http://dbpedia.org/resource/Vyacheslav_Zudov', 'http://dbpedia.org/resource/Yevgeny_Khrunov', 'http://dbpedia.org/resource/Yuri_Artyukhin', 'http://dbpedia.org/resource/Yuri_Glazkov', 'http://dbpedia.org/resource/Yuri_Malyshev_(cosmonaut)', 'http://dbpedia.org/resource/Yuri_Romanenko']</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>['http://dbpedia.org/resource/Aleksandr_Aleksandrovich_Volkov', 'http://dbpedia.org/resource/Aleksandr_Ivanchenkov', 'http://dbpedia.org/resource/Aleksandr_Laveykin', 'http://dbpedia.org/resource/Aleksandr_Nikolayevich_Balandin', 'http://dbpedia.org/resource/Aleksandr_Pavlovich_Aleksandrov__Aleksandr_Pavlovich_Aleksandrov__1', 'http://dbpedia.org/resource/Aleksandr_Serebrov', 'http://dbpedia.org/resource/Aleksandr_Viktorenko', 'http://dbpedia.org/resource/Aleksei_Gubarev', 'http://dbpedia.org/resource/Aleksei_Yeliseyev', 'http://dbpedia.org/resource/Anatoly_Berezovoy', 'http://dbpedia.org/resource/Anatoly_Filipchenko', 'http://dbpedia.org/resource/Anatoly_Levchenko__Anatoly_Semyonovich_Levchenko__1', 'http://dbpedia.org/resource/Andriyan_Nikolayev', 'http://dbpedia.org/resource/Boris_Andreyev_(cosmonaut)', 'http://dbpedia.org/resource/Boris_Volynov', 'http://dbpedia.org/resource/Boris_Yegorov', 'http://dbpedia.org/resource/Gennady_Manakov', 'http://dbpedia.org/resource/Gennady_Sarafanov', 'http://dbpedia.org/resource/Gennady_Strekalov', 'http://dbpedia.org/resource/Georgy_Dobrovolsky', 'http://dbpedia.org/resource/Georgy_Grechko', 'http://dbpedia.org/resource/Ivan_Anikeyev', 'http://dbpedia.org/resource/Konstantin_Feoktistov', 'http://dbpedia.org/resource/Leonid_Ivanov_(test_pilot)', 'http://dbpedia.org/resource/Leonid_Kizim', 'http://dbpedia.org/resource/Leonid_Popov', 'http://dbpedia.org/resource/Lev_Dyomin', 'http://dbpedia.org/resource/Mars_Rafikov', 'http://dbpedia.org/resource/Nikolai_Rukavishnikov', 'http://dbpedia.org/resource/Oleg_Atkov', 'http://dbpedia.org/resource/Oleg_Grigoriyevich_Kononenko', 'http://dbpedia.org/resource/Oleg_Makarov_(cosmonaut)', 'http://dbpedia.org/resource/Pavel_Belyayev', 'http://dbpedia.org/resource/Sergey_Volkov_(cosmonaut)', 'http://dbpedia.org/resource/Sergey_Vozovikov', 'http://dbpedia.org/resource/Valentin_Bondarenko', 'http://dbpedia.org/resource/Valentin_Lebedev', 'http://dbpedia.org/resource/Valery_Bykovsky', 'http://dbpedia.org/resource/Valery_Kubasov', 'http://dbpedia.org/resource/Valery_Rozhdestvensky', 'http://dbpedia.org/resource/Valery_Ryumin', 'http://dbpedia.org/resource/Vasily_Lazarev', 'http://dbpedia.org/resource/Viktor_Gorbatko', 'http://dbpedia.org/resource/Viktor_Patsayev', 'http://dbpedia.org/resource/Viktor_Savinykh', 'http://dbpedia.org/resource/Vitaly_Sevastyanov', 'http://dbpedia.org/resource/Vladimir_Aksyonov', 'http://dbpedia.org/resource/Vladimir_Dzhanibekov', 'http://dbpedia.org/resource/Vladimir_Shatalov', 'http://dbpedia.org/resource/Vladimir_Solovyov_(cosmonaut)', 'http://dbpedia.org/resource/Vladimir_Vasyutin', 'http://dbpedia.org/resource/Vladislav_Volkov', 'http://dbpedia.org/resource/Vyacheslav_Zudov', 'http://dbpedia.org/resource/Yevgeny_Khrunov', 'http://dbpedia.org/resource/Yuri_Artyukhin', 'http://dbpedia.org/resource/Yuri_Glazkov', 'http://dbpedia.org/resource/Yuri_Malyshev_(cosmonaut)', 'http://dbpedia.org/resource/Yuri_Romanenko']</t>
-        </is>
-      </c>
-      <c r="D31" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Who created Family Guy?</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>['http://dbpedia.org/resource/Seth_MacFarlane']</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>['http://dbpedia.org/resource/Seth_MacFarlane']</t>
-        </is>
-      </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>How many people live in the capital of Australia?</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>['453558']</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>['453558']</t>
-        </is>
-      </c>
-      <c r="D33" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Who created Goofy?</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>['http://dbpedia.org/resource/Bob_Ogle', 'http://dbpedia.org/resource/Paul_Murry']</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>['http://dbpedia.org/resource/Bob_Ogle', 'http://dbpedia.org/resource/Paul_Murry']</t>
-        </is>
-      </c>
-      <c r="D34" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>